<commit_message>
Ending obvious exclusion identification of 2017-2018.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D091B518-45B0-4C61-ACBA-6BF3B66FE335}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2BB92C-FEE3-4A16-916C-0E0694F4621E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3680" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="680" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="320">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -964,6 +964,27 @@
   </si>
   <si>
     <t>3410-3470</t>
+  </si>
+  <si>
+    <t>975-</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes, 050-051</t>
+  </si>
+  <si>
+    <t>2555-2595 14805-14830 15800-15855</t>
+  </si>
+  <si>
+    <t>1000-1270 2720-2800 5170-5210 6750-6800</t>
+  </si>
+  <si>
+    <t>920-940 2510-2560 6715-6760</t>
+  </si>
+  <si>
+    <t>1420-1620</t>
   </si>
 </sst>
 </file>
@@ -1318,8 +1339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
   <dimension ref="A1:E194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A171" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E194" sqref="E194"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1405,6 +1426,9 @@
       <c r="B6" t="s">
         <v>196</v>
       </c>
+      <c r="C6" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -1413,6 +1437,9 @@
       <c r="B7" t="s">
         <v>196</v>
       </c>
+      <c r="C7" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -1421,6 +1448,12 @@
       <c r="B8" t="s">
         <v>196</v>
       </c>
+      <c r="C8" t="s">
+        <v>203</v>
+      </c>
+      <c r="E8" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
@@ -1429,6 +1462,9 @@
       <c r="B9" t="s">
         <v>196</v>
       </c>
+      <c r="C9" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1437,6 +1473,9 @@
       <c r="B10" t="s">
         <v>196</v>
       </c>
+      <c r="C10" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
@@ -1445,6 +1484,9 @@
       <c r="B11" t="s">
         <v>196</v>
       </c>
+      <c r="C11" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -1453,6 +1495,9 @@
       <c r="B12" t="s">
         <v>196</v>
       </c>
+      <c r="C12" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1461,6 +1506,9 @@
       <c r="B13" t="s">
         <v>196</v>
       </c>
+      <c r="C13" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -1469,6 +1517,15 @@
       <c r="B14" t="s">
         <v>196</v>
       </c>
+      <c r="C14" t="s">
+        <v>203</v>
+      </c>
+      <c r="D14" t="s">
+        <v>315</v>
+      </c>
+      <c r="E14" t="s">
+        <v>316</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -1477,6 +1534,12 @@
       <c r="B15" t="s">
         <v>196</v>
       </c>
+      <c r="C15" t="s">
+        <v>203</v>
+      </c>
+      <c r="E15" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -1485,6 +1548,9 @@
       <c r="B16" t="s">
         <v>196</v>
       </c>
+      <c r="C16" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
@@ -1493,6 +1559,12 @@
       <c r="B17" t="s">
         <v>196</v>
       </c>
+      <c r="C17" t="s">
+        <v>203</v>
+      </c>
+      <c r="E17" t="s">
+        <v>318</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
@@ -1501,6 +1573,12 @@
       <c r="B18" t="s">
         <v>196</v>
       </c>
+      <c r="C18" t="s">
+        <v>203</v>
+      </c>
+      <c r="E18" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
@@ -1509,6 +1587,9 @@
       <c r="B19" t="s">
         <v>196</v>
       </c>
+      <c r="C19" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
@@ -1516,6 +1597,12 @@
       </c>
       <c r="B20" t="s">
         <v>196</v>
+      </c>
+      <c r="C20" t="s">
+        <v>203</v>
+      </c>
+      <c r="E20">
+        <v>-640</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Adding the obvious exclusions to corresponding datetracks.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C2BB92C-FEE3-4A16-916C-0E0694F4621E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF6F2AB-FFE6-41D0-9289-BA70F5BC3CFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3680" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -717,6 +717,9 @@
     <t>Yes, 072</t>
   </si>
   <si>
+    <t>Yes, 077</t>
+  </si>
+  <si>
     <t>Yes, 179</t>
   </si>
   <si>
@@ -724,9 +727,6 @@
   </si>
   <si>
     <t>Yes, 145</t>
-  </si>
-  <si>
-    <t>Yes, 076</t>
   </si>
   <si>
     <t>Obvious exclusions</t>
@@ -1339,8 +1339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
   <dimension ref="A1:E194"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F190" sqref="F190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3636,7 +3636,7 @@
         <v>203</v>
       </c>
       <c r="D176" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.35">
@@ -3661,7 +3661,7 @@
         <v>203</v>
       </c>
       <c r="D178" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E178" t="s">
         <v>302</v>
@@ -3781,7 +3781,7 @@
         <v>203</v>
       </c>
       <c r="D187" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.35">
@@ -3837,7 +3837,7 @@
         <v>203</v>
       </c>
       <c r="D191" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="E191" t="s">
         <v>309</v>

</xml_diff>

<commit_message>
Adding new_data_selection_20172018.txt to be trackes. This is actually the file Exclusions_new_data_selections.txt which has been renamed.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BF6F2AB-FFE6-41D0-9289-BA70F5BC3CFE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D180B52B-ECD2-44CE-BBCF-7296B62DF40A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3680" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -1340,7 +1340,7 @@
   <dimension ref="A1:E194"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A175" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F190" sqref="F190"/>
+      <selection activeCell="J189" sqref="J189"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Modyfying so that it work. It was overlapping before: 20170412_01_035_057 20170412_01_056_062
Now:

20170412_01_035_055
20170412_01_057_062
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D180B52B-ECD2-44CE-BBCF-7296B62DF40A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10B449A-3AD1-4558-9D3B-8C923A1C4914}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3680" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="701" uniqueCount="320">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="322">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -985,6 +985,12 @@
   </si>
   <si>
     <t>1420-1620</t>
+  </si>
+  <si>
+    <t>Yes, 056-057</t>
+  </si>
+  <si>
+    <t>Start now at 057</t>
   </si>
 </sst>
 </file>
@@ -1339,8 +1345,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
   <dimension ref="A1:E194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J189" sqref="J189"/>
+    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E66" sqref="E66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2201,6 +2207,9 @@
       <c r="C65" t="s">
         <v>203</v>
       </c>
+      <c r="D65" t="s">
+        <v>320</v>
+      </c>
       <c r="E65" t="s">
         <v>259</v>
       </c>
@@ -2214,6 +2223,9 @@
       </c>
       <c r="C66" t="s">
         <v>203</v>
+      </c>
+      <c r="D66" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Define sections for the different phases of exclusion indentification.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F10B449A-3AD1-4558-9D3B-8C923A1C4914}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC07A5C-41E4-4423-B98B-2B727A0AB54A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3680" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="703" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="321">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -42,12 +42,6 @@
     <t>20170322_04_001_001</t>
   </si>
   <si>
-    <t>20170322_04_003_005</t>
-  </si>
-  <si>
-    <t>20170322_04_006_008</t>
-  </si>
-  <si>
     <t>20170322_04_010_013</t>
   </si>
   <si>
@@ -966,9 +960,6 @@
     <t>3410-3470</t>
   </si>
   <si>
-    <t>975-</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
@@ -990,7 +981,13 @@
     <t>Yes, 056-057</t>
   </si>
   <si>
-    <t>Start now at 057</t>
+    <t>20170322_04_003_008</t>
+  </si>
+  <si>
+    <t>4972-</t>
+  </si>
+  <si>
+    <t>Yes, 056</t>
   </si>
 </sst>
 </file>
@@ -1343,10 +1340,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
-  <dimension ref="A1:E194"/>
+  <dimension ref="A1:E193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E66" sqref="E66"/>
+    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1360,19 +1357,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D1" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E1" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
@@ -1380,10 +1377,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C2" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -1391,10 +1388,10 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C3" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -1402,16 +1399,16 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>205</v>
-      </c>
       <c r="E4" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -1419,10 +1416,10 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -1430,1314 +1427,1314 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C6" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>318</v>
       </c>
       <c r="B7" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C7" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E7" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C8" t="s">
-        <v>203</v>
-      </c>
-      <c r="E8" t="s">
-        <v>313</v>
+        <v>201</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C9" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C10" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B11" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C11" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C12" t="s">
-        <v>203</v>
+        <v>311</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C13" t="s">
-        <v>314</v>
+        <v>201</v>
+      </c>
+      <c r="D13" t="s">
+        <v>312</v>
+      </c>
+      <c r="E13" t="s">
+        <v>313</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C14" t="s">
-        <v>203</v>
-      </c>
-      <c r="D14" t="s">
-        <v>315</v>
+        <v>201</v>
       </c>
       <c r="E14" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C15" t="s">
-        <v>203</v>
-      </c>
-      <c r="E15" t="s">
-        <v>317</v>
+        <v>201</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C16" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E16" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C17" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E17" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C18" t="s">
-        <v>203</v>
-      </c>
-      <c r="E18" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C19" t="s">
-        <v>314</v>
+        <v>201</v>
+      </c>
+      <c r="E19">
+        <v>-640</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C20" t="s">
-        <v>203</v>
-      </c>
-      <c r="E20">
-        <v>-640</v>
+        <v>201</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C21" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C22" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C23" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C24" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="D24" t="s">
+        <v>204</v>
+      </c>
+      <c r="E24" t="s">
+        <v>234</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C25" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D25" t="s">
-        <v>206</v>
-      </c>
-      <c r="E25" t="s">
-        <v>236</v>
+        <v>205</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C26" t="s">
-        <v>203</v>
-      </c>
-      <c r="D26" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C27" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C28" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="D28" t="s">
+        <v>206</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C29" t="s">
-        <v>203</v>
-      </c>
-      <c r="D29" t="s">
-        <v>208</v>
+        <v>201</v>
+      </c>
+      <c r="E29" t="s">
+        <v>235</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C30" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E30" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C31" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E31" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C32" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E32" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C33" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E33" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C34" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E34" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C35" t="s">
-        <v>203</v>
-      </c>
-      <c r="E35" t="s">
-        <v>242</v>
+        <v>201</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C36" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C37" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C38" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="D38" t="s">
+        <v>207</v>
+      </c>
+      <c r="E38">
+        <v>-1815</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C39" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D39" t="s">
         <v>209</v>
       </c>
       <c r="E39">
-        <v>-1815</v>
+        <v>-375</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C40" t="s">
-        <v>203</v>
-      </c>
-      <c r="D40" t="s">
-        <v>211</v>
-      </c>
-      <c r="E40">
-        <v>-375</v>
+        <v>198</v>
+      </c>
+      <c r="E40" t="s">
+        <v>241</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C41" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E41" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C42" t="s">
-        <v>203</v>
-      </c>
-      <c r="E42" t="s">
-        <v>244</v>
+        <v>201</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>243</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C43" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C44" t="s">
-        <v>203</v>
-      </c>
-      <c r="E44" s="1" t="s">
-        <v>246</v>
+        <v>201</v>
+      </c>
+      <c r="E44" t="s">
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B45" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C45" t="s">
-        <v>203</v>
-      </c>
-      <c r="E45" t="s">
-        <v>247</v>
+        <v>201</v>
+      </c>
+      <c r="E45" s="1">
+        <v>-1840</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C46" t="s">
-        <v>203</v>
-      </c>
-      <c r="E46" s="1">
-        <v>-1840</v>
+        <v>201</v>
+      </c>
+      <c r="E46">
+        <v>-625</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B47" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C47" t="s">
-        <v>203</v>
-      </c>
-      <c r="E47">
-        <v>-625</v>
+        <v>201</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>246</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B48" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C48" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B49" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C49" t="s">
-        <v>203</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>249</v>
+        <v>201</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B50" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C50" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B51" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C51" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E51" t="s">
+        <v>248</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C52" t="s">
-        <v>203</v>
-      </c>
-      <c r="E52" t="s">
-        <v>250</v>
+        <v>201</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>249</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B53" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C53" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B54" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C54" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B55" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C55" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B56" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C56" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B57" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C57" t="s">
-        <v>203</v>
-      </c>
-      <c r="E57" s="1" t="s">
-        <v>255</v>
+        <v>201</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B58" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C58" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B59" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C59" t="s">
-        <v>203</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>256</v>
+        <v>201</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B60" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C60" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B61" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C61" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="D61" t="s">
+        <v>211</v>
+      </c>
+      <c r="E61" t="s">
+        <v>255</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B62" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C62" t="s">
-        <v>203</v>
-      </c>
-      <c r="D62" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="E62" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B63" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C63" t="s">
-        <v>203</v>
-      </c>
-      <c r="E63" t="s">
-        <v>258</v>
+        <v>201</v>
+      </c>
+      <c r="E63">
+        <v>-840</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B64" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C64" t="s">
-        <v>203</v>
-      </c>
-      <c r="E64">
-        <v>-840</v>
+        <v>201</v>
+      </c>
+      <c r="D64" t="s">
+        <v>317</v>
+      </c>
+      <c r="E64" t="s">
+        <v>257</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B65" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C65" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D65" t="s">
         <v>320</v>
       </c>
-      <c r="E65" t="s">
-        <v>259</v>
-      </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B66" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C66" t="s">
-        <v>203</v>
-      </c>
-      <c r="D66" t="s">
-        <v>321</v>
+        <v>201</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B67" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C67" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E67" t="s">
+        <v>258</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B68" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C68" t="s">
-        <v>203</v>
-      </c>
-      <c r="E68" t="s">
-        <v>260</v>
+        <v>201</v>
+      </c>
+      <c r="E68">
+        <v>-840</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B69" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C69" t="s">
-        <v>203</v>
-      </c>
-      <c r="E69">
-        <v>-840</v>
+        <v>201</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B70" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C70" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E70" t="s">
+        <v>259</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B71" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C71" t="s">
-        <v>203</v>
-      </c>
-      <c r="E71" t="s">
-        <v>261</v>
+        <v>201</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B72" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C72" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E72">
+        <v>-610</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B73" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C73" t="s">
-        <v>203</v>
-      </c>
-      <c r="E73">
-        <v>-610</v>
+        <v>201</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B74" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C74" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B75" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C75" t="s">
-        <v>203</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>262</v>
+        <v>201</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B76" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C76" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B77" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C77" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="D77" t="s">
+        <v>212</v>
+      </c>
+      <c r="E77" t="s">
+        <v>261</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B78" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C78" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D78" t="s">
         <v>214</v>
       </c>
-      <c r="E78" t="s">
-        <v>263</v>
-      </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B79" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C79" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D79" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B80" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C80" t="s">
-        <v>203</v>
-      </c>
-      <c r="D80" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B81" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C81" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="D81" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B82" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C82" t="s">
-        <v>203</v>
-      </c>
-      <c r="D82" t="s">
-        <v>217</v>
+        <v>201</v>
+      </c>
+      <c r="E82" t="s">
+        <v>262</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B83" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C83" t="s">
-        <v>203</v>
-      </c>
-      <c r="E83" t="s">
-        <v>264</v>
+        <v>201</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B84" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C84" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B85" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C85" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="D85" t="s">
+        <v>210</v>
+      </c>
+      <c r="E85" t="s">
+        <v>263</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B86" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C86" t="s">
-        <v>203</v>
-      </c>
-      <c r="D86" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="E86" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B87" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C87" t="s">
-        <v>203</v>
-      </c>
-      <c r="E87" t="s">
-        <v>266</v>
+        <v>201</v>
+      </c>
+      <c r="E87" s="1" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B88" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C88" t="s">
-        <v>203</v>
-      </c>
-      <c r="E88" s="1" t="s">
-        <v>267</v>
+        <v>201</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B89" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C89" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E89">
+        <v>-750</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B90" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C90" t="s">
-        <v>203</v>
-      </c>
-      <c r="E90">
-        <v>-750</v>
+        <v>201</v>
+      </c>
+      <c r="E90" s="1" t="s">
+        <v>266</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B91" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C91" t="s">
-        <v>203</v>
-      </c>
-      <c r="E91" s="1" t="s">
-        <v>268</v>
+        <v>201</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B92" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C92" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B93" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C93" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E93" t="s">
+        <v>267</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B94" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C94" t="s">
-        <v>203</v>
-      </c>
-      <c r="E94" t="s">
-        <v>269</v>
+        <v>201</v>
+      </c>
+      <c r="D94" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B95" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C95" t="s">
-        <v>203</v>
-      </c>
-      <c r="D95" t="s">
-        <v>218</v>
+        <v>201</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B96" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C96" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B97" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C97" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B98" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C98" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E98" t="s">
+        <v>268</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B99" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C99" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="D99" t="s">
+        <v>217</v>
       </c>
       <c r="E99" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B100" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C100" t="s">
-        <v>203</v>
-      </c>
-      <c r="D100" t="s">
-        <v>219</v>
-      </c>
-      <c r="E100" t="s">
-        <v>271</v>
+        <v>201</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B101" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C101" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B102" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C102" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="D102" t="s">
+        <v>220</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B103" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C103" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D103" t="s">
-        <v>222</v>
+        <v>221</v>
+      </c>
+      <c r="E103" t="s">
+        <v>270</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B104" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C104" t="s">
-        <v>203</v>
-      </c>
-      <c r="D104" t="s">
-        <v>223</v>
-      </c>
-      <c r="E104" t="s">
-        <v>272</v>
+        <v>201</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B105" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C105" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B106" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C106" t="s">
         <v>201</v>
@@ -2745,988 +2742,991 @@
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B107" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C107" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E107" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B108" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C108" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E108" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B109" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C109" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E109" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B110" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C110" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E110" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B111" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C111" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E111" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B112" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C112" t="s">
-        <v>203</v>
-      </c>
-      <c r="E112" t="s">
-        <v>277</v>
+        <v>201</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B113" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C113" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E113" t="s">
+        <v>276</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B114" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C114" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E114" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B115" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C115" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E115" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B116" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C116" t="s">
-        <v>203</v>
-      </c>
-      <c r="E116" t="s">
-        <v>280</v>
+        <v>201</v>
+      </c>
+      <c r="D116" t="s">
+        <v>222</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B117" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C117" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D117" t="s">
-        <v>224</v>
+        <v>209</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B118" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C118" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D118" t="s">
-        <v>211</v>
+        <v>223</v>
+      </c>
+      <c r="E118" t="s">
+        <v>279</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B119" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C119" t="s">
-        <v>203</v>
-      </c>
-      <c r="D119" t="s">
-        <v>225</v>
+        <v>201</v>
       </c>
       <c r="E119" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B120" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C120" t="s">
-        <v>203</v>
-      </c>
-      <c r="E120" t="s">
-        <v>282</v>
+        <v>201</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B121" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C121" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E121" t="s">
+        <v>281</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B122" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C122" t="s">
-        <v>203</v>
-      </c>
-      <c r="E122" t="s">
-        <v>283</v>
+        <v>201</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B123" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C123" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B124" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C124" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B125" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C125" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B126" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C126" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E126" t="s">
+        <v>282</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B127" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C127" t="s">
-        <v>203</v>
-      </c>
-      <c r="E127" t="s">
-        <v>284</v>
+        <v>201</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B128" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C128" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B129" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C129" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B130" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C130" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B131" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C131" t="s">
-        <v>202</v>
+        <v>201</v>
+      </c>
+      <c r="E131" t="s">
+        <v>283</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B132" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C132" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E132" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B133" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C133" t="s">
-        <v>203</v>
-      </c>
-      <c r="E133" t="s">
-        <v>286</v>
+        <v>201</v>
+      </c>
+      <c r="E133">
+        <v>-590</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B134" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C134" t="s">
-        <v>203</v>
-      </c>
-      <c r="E134">
-        <v>-590</v>
+        <v>201</v>
+      </c>
+      <c r="E134" t="s">
+        <v>285</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B135" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C135" t="s">
-        <v>203</v>
-      </c>
-      <c r="E135" t="s">
-        <v>287</v>
+        <v>201</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B136" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C136" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E136" t="s">
+        <v>286</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B137" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C137" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E137" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B138" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C138" t="s">
-        <v>203</v>
-      </c>
-      <c r="E138" t="s">
-        <v>289</v>
+        <v>201</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B139" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C139" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E139" t="s">
+        <v>288</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B140" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C140" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E140" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B141" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C141" t="s">
-        <v>203</v>
-      </c>
-      <c r="E141" t="s">
-        <v>291</v>
+        <v>201</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B142" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C142" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B143" t="s">
         <v>195</v>
       </c>
       <c r="C143" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="D143" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B144" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C144" t="s">
-        <v>203</v>
-      </c>
-      <c r="D144" t="s">
-        <v>220</v>
+        <v>201</v>
+      </c>
+      <c r="E144">
+        <v>-1600</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B145" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C145" t="s">
-        <v>203</v>
-      </c>
-      <c r="E145">
-        <v>-1600</v>
+        <v>201</v>
+      </c>
+      <c r="D145" t="s">
+        <v>219</v>
+      </c>
+      <c r="E145" t="s">
+        <v>290</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B146" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C146" t="s">
-        <v>203</v>
-      </c>
-      <c r="D146" t="s">
-        <v>221</v>
-      </c>
-      <c r="E146" t="s">
-        <v>292</v>
+        <v>201</v>
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B147" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C147" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B148" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C148" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E148" t="s">
+        <v>291</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B149" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C149" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E149" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B150" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C150" t="s">
-        <v>203</v>
-      </c>
-      <c r="E150" t="s">
-        <v>294</v>
+        <v>201</v>
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B151" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C151" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B152" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C152" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="D152" t="s">
+        <v>210</v>
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B153" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C153" t="s">
-        <v>203</v>
-      </c>
-      <c r="D153" t="s">
-        <v>212</v>
+        <v>201</v>
+      </c>
+      <c r="E153" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B154" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C154" t="s">
-        <v>203</v>
-      </c>
-      <c r="E154" t="s">
-        <v>295</v>
+        <v>201</v>
+      </c>
+      <c r="E154">
+        <v>-70</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B155" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C155" t="s">
-        <v>203</v>
-      </c>
-      <c r="E155">
-        <v>-70</v>
+        <v>201</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B156" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C156" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B157" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C157" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B158" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C158" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E158" t="s">
+        <v>294</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B159" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C159" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E159" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B160" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C160" t="s">
-        <v>203</v>
-      </c>
-      <c r="E160" t="s">
-        <v>297</v>
+        <v>201</v>
+      </c>
+      <c r="E160">
+        <v>-440</v>
       </c>
     </row>
     <row r="161" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B161" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C161" t="s">
-        <v>203</v>
-      </c>
-      <c r="E161">
-        <v>-440</v>
+        <v>201</v>
+      </c>
+      <c r="D161" t="s">
+        <v>224</v>
+      </c>
+      <c r="E161" t="s">
+        <v>296</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B162" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C162" t="s">
-        <v>203</v>
-      </c>
-      <c r="D162" t="s">
-        <v>226</v>
-      </c>
-      <c r="E162" t="s">
-        <v>298</v>
+        <v>201</v>
       </c>
     </row>
     <row r="163" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B163" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C163" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="164" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B164" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C164" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="D164" t="s">
+        <v>225</v>
       </c>
     </row>
     <row r="165" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B165" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C165" t="s">
-        <v>203</v>
-      </c>
-      <c r="D165" t="s">
-        <v>227</v>
+        <v>201</v>
       </c>
     </row>
     <row r="166" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B166" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C166" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="D166" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="167" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B167" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C167" t="s">
-        <v>203</v>
-      </c>
-      <c r="D167" t="s">
-        <v>221</v>
+        <v>201</v>
+      </c>
+      <c r="E167" t="s">
+        <v>297</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B168" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C168" t="s">
-        <v>203</v>
-      </c>
-      <c r="E168" t="s">
-        <v>299</v>
+        <v>201</v>
+      </c>
+      <c r="D168" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="169" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B169" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C169" t="s">
-        <v>203</v>
-      </c>
-      <c r="D169" t="s">
-        <v>228</v>
+        <v>201</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B170" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C170" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="D170" t="s">
+        <v>227</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B171" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C171" t="s">
-        <v>203</v>
-      </c>
-      <c r="D171" t="s">
-        <v>229</v>
+        <v>201</v>
+      </c>
+      <c r="E171" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B172" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C172" t="s">
-        <v>203</v>
-      </c>
-      <c r="E172" t="s">
-        <v>300</v>
+        <v>201</v>
+      </c>
+      <c r="E172">
+        <v>-1100</v>
       </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B173" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C173" t="s">
-        <v>203</v>
-      </c>
-      <c r="E173">
-        <v>-1100</v>
+        <v>201</v>
       </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B174" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C174" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E174" t="s">
+        <v>299</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B175" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C175" t="s">
-        <v>203</v>
-      </c>
-      <c r="E175" t="s">
-        <v>301</v>
+        <v>201</v>
+      </c>
+      <c r="D175" t="s">
+        <v>229</v>
       </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B176" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C176" t="s">
-        <v>203</v>
-      </c>
-      <c r="D176" t="s">
-        <v>231</v>
+        <v>201</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B177" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C177" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="D177" t="s">
+        <v>230</v>
+      </c>
+      <c r="E177" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B178" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C178" t="s">
-        <v>203</v>
-      </c>
-      <c r="D178" t="s">
-        <v>232</v>
-      </c>
-      <c r="E178" t="s">
-        <v>302</v>
+        <v>201</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B179" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C179" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E179" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B180" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C180" t="s">
-        <v>203</v>
-      </c>
-      <c r="E180" t="s">
-        <v>303</v>
+        <v>201</v>
+      </c>
+      <c r="D180" t="s">
+        <v>218</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B181" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C181" t="s">
-        <v>203</v>
-      </c>
-      <c r="D181" t="s">
-        <v>220</v>
+        <v>201</v>
+      </c>
+      <c r="E181" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B182" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C182" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E182" t="s">
         <v>304</v>
@@ -3734,167 +3734,153 @@
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B183" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C183" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E183" t="s">
-        <v>306</v>
+        <v>303</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B184" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C184" t="s">
-        <v>203</v>
-      </c>
-      <c r="E184" t="s">
-        <v>305</v>
+        <v>201</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B185" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C185" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B186" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C186" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="D186" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B187" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C187" t="s">
-        <v>203</v>
-      </c>
-      <c r="D187" t="s">
-        <v>230</v>
+        <v>201</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B188" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C188" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="E188" t="s">
+        <v>305</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B189" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C189" t="s">
-        <v>203</v>
+        <v>201</v>
+      </c>
+      <c r="D189" t="s">
+        <v>208</v>
       </c>
       <c r="E189" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B190" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C190" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D190" t="s">
-        <v>210</v>
+        <v>231</v>
       </c>
       <c r="E190" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B191" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C191" t="s">
-        <v>203</v>
-      </c>
-      <c r="D191" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="E191" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B192" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C192" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E192" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B193" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C193" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E193" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A194" t="s">
-        <v>192</v>
-      </c>
-      <c r="B194" t="s">
-        <v>197</v>
-      </c>
-      <c r="C194" t="s">
-        <v>203</v>
-      </c>
-      <c r="E194" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deleting 20180430_01_139_144 because fail in the processing.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC07A5C-41E4-4423-B98B-2B727A0AB54A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814F800B-F192-4D4B-93CE-99DE865F69E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3680" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="344">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -988,6 +988,75 @@
   </si>
   <si>
     <t>Yes, 056</t>
+  </si>
+  <si>
+    <t>Exclusions after 1st run</t>
+  </si>
+  <si>
+    <t>-230 470-675 1350-1515 1680-1975 3600-'</t>
+  </si>
+  <si>
+    <t>-910 -2115'</t>
+  </si>
+  <si>
+    <t>To delete because very bad</t>
+  </si>
+  <si>
+    <t>9180-10400</t>
+  </si>
+  <si>
+    <t>-800 910-990 1130-1255 1395-'</t>
+  </si>
+  <si>
+    <t>-2850 4090-'</t>
+  </si>
+  <si>
+    <t>-21200 31320-'</t>
+  </si>
+  <si>
+    <t>-2480 2630-2690 3345-'</t>
+  </si>
+  <si>
+    <t>-5810 5825-5925 6060-</t>
+  </si>
+  <si>
+    <t>-1620 1790</t>
+  </si>
+  <si>
+    <t>-360 500-650 910-1060 1260-</t>
+  </si>
+  <si>
+    <t>-1000 2450-</t>
+  </si>
+  <si>
+    <t>-225 1200-</t>
+  </si>
+  <si>
+    <t>-500</t>
+  </si>
+  <si>
+    <t>-2740 2900-3055 6780-7220 9680-9860 10470-10560 19910-19990 27330-</t>
+  </si>
+  <si>
+    <t>2240-3560 10260-</t>
+  </si>
+  <si>
+    <t>2300-</t>
+  </si>
+  <si>
+    <t>-1010</t>
+  </si>
+  <si>
+    <t>to delete because bad</t>
+  </si>
+  <si>
+    <t>-3920 5100-7120</t>
+  </si>
+  <si>
+    <t>-1450 1720-1880 2730-</t>
+  </si>
+  <si>
+    <t>Deleted, cound not be processed (error in log10 computation)</t>
   </si>
 </sst>
 </file>
@@ -1003,12 +1072,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1023,9 +1104,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1340,10 +1429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
-  <dimension ref="A1:E193"/>
+  <dimension ref="A1:F193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D66" sqref="D66"/>
+    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D193" sqref="D193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1353,9 +1442,10 @@
     <col min="3" max="3" width="25.1796875" customWidth="1"/>
     <col min="4" max="4" width="18.54296875" customWidth="1"/>
     <col min="5" max="5" width="16.36328125" customWidth="1"/>
+    <col min="6" max="6" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>191</v>
       </c>
@@ -1371,8 +1461,11 @@
       <c r="E1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F1" s="4" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1382,19 +1475,23 @@
       <c r="C2" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="F2" s="5" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>197</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1410,8 +1507,11 @@
       <c r="E4" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F4" s="5" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1421,44 +1521,56 @@
       <c r="C5" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="F5" s="4">
+        <v>-620</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C6" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="C6" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
         <v>318</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C7" t="s">
-        <v>201</v>
-      </c>
-      <c r="E7" t="s">
+      <c r="C7" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>319</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="F7" s="7" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C8" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C8" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1468,8 +1580,11 @@
       <c r="C9" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F9" s="8" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1479,8 +1594,11 @@
       <c r="C10" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F10" s="9" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1490,8 +1608,11 @@
       <c r="C11" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F11" s="9" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1502,7 +1623,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1518,8 +1639,11 @@
       <c r="E13" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F13" s="5" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1532,19 +1656,25 @@
       <c r="E14" t="s">
         <v>314</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="F14" s="5" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C15" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="C15" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1557,8 +1687,11 @@
       <c r="E16" t="s">
         <v>315</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1571,8 +1704,11 @@
       <c r="E17" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F17" s="4" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1583,21 +1719,24 @@
         <v>311</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B19" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="C19" t="s">
-        <v>201</v>
-      </c>
-      <c r="E19">
+      <c r="C19" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="E19" s="3">
         <v>-640</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F19" s="7" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1607,8 +1746,11 @@
       <c r="C20" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F20" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1618,8 +1760,11 @@
       <c r="C21" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F21" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1629,8 +1774,11 @@
       <c r="C22" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F22" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1640,8 +1788,11 @@
       <c r="C23" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1657,8 +1808,11 @@
       <c r="E24" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" s="4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1671,8 +1825,11 @@
       <c r="D25" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1682,8 +1839,11 @@
       <c r="C26" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26" s="4" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1693,22 +1853,28 @@
       <c r="C27" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="F27" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B28" t="s">
-        <v>193</v>
-      </c>
-      <c r="C28" t="s">
-        <v>201</v>
-      </c>
-      <c r="D28" t="s">
+      <c r="B28" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="D28" s="3" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28" s="7" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1721,8 +1887,11 @@
       <c r="E29" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29" s="4" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1735,8 +1904,11 @@
       <c r="E30" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -1750,7 +1922,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -3648,7 +3820,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>174</v>
       </c>
@@ -3665,7 +3837,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>175</v>
       </c>
@@ -3676,7 +3848,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>176</v>
       </c>
@@ -3690,7 +3862,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>177</v>
       </c>
@@ -3704,7 +3876,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>178</v>
       </c>
@@ -3718,7 +3890,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>179</v>
       </c>
@@ -3732,7 +3904,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>180</v>
       </c>
@@ -3746,7 +3918,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>181</v>
       </c>
@@ -3757,7 +3929,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>182</v>
       </c>
@@ -3768,7 +3940,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>183</v>
       </c>
@@ -3782,7 +3954,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>184</v>
       </c>
@@ -3793,7 +3965,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>185</v>
       </c>
@@ -3807,7 +3979,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>186</v>
       </c>
@@ -3824,24 +3996,27 @@
         <v>306</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A190" t="s">
+    <row r="190" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A190" s="2" t="s">
         <v>187</v>
       </c>
-      <c r="B190" t="s">
-        <v>195</v>
-      </c>
-      <c r="C190" t="s">
-        <v>201</v>
-      </c>
-      <c r="D190" t="s">
+      <c r="B190" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C190" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D190" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="E190" t="s">
+      <c r="E190" s="2" t="s">
         <v>307</v>
       </c>
-    </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F190" s="6" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>188</v>
       </c>
@@ -3855,7 +4030,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>189</v>
       </c>

</xml_diff>

<commit_message>
Deleting several dates where data processing fails or no slabs presence.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{814F800B-F192-4D4B-93CE-99DE865F69E2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE50A3B-3A82-4AFB-946E-861862DCF278}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3680" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="471">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -768,9 +768,6 @@
     <t>-530 4760-'</t>
   </si>
   <si>
-    <t>-1040 6290'</t>
-  </si>
-  <si>
     <t>9795-9855 12630-</t>
   </si>
   <si>
@@ -1026,9 +1023,6 @@
     <t>-360 500-650 910-1060 1260-</t>
   </si>
   <si>
-    <t>-1000 2450-</t>
-  </si>
-  <si>
     <t>-225 1200-</t>
   </si>
   <si>
@@ -1057,6 +1051,393 @@
   </si>
   <si>
     <t>Deleted, cound not be processed (error in log10 computation)</t>
+  </si>
+  <si>
+    <t>4510-4950 27360-29020 29740-29910 30890-31460 35100-35700 37170-37420 38660-38900 40440-</t>
+  </si>
+  <si>
+    <t>5720-6310 6540-6815</t>
+  </si>
+  <si>
+    <t>2560-</t>
+  </si>
+  <si>
+    <t>-940 5050-5630 5810-6000 6050-6480 8150-8310 8450-11130</t>
+  </si>
+  <si>
+    <t>-550 2060-2280 3200-3310 4260-4400 4780-4900 5280-5460</t>
+  </si>
+  <si>
+    <t>-170 1050-</t>
+  </si>
+  <si>
+    <t>-1890 2370-</t>
+  </si>
+  <si>
+    <t>6360-</t>
+  </si>
+  <si>
+    <t>1540-2230</t>
+  </si>
+  <si>
+    <t>680-1250</t>
+  </si>
+  <si>
+    <t>-1040 6290-</t>
+  </si>
+  <si>
+    <t>840-890</t>
+  </si>
+  <si>
+    <t>-780</t>
+  </si>
+  <si>
+    <t>1160-1480 3230-3320 3700-3870 4220-4540</t>
+  </si>
+  <si>
+    <t>-1240</t>
+  </si>
+  <si>
+    <t>1550-1620 1860-</t>
+  </si>
+  <si>
+    <t>-1720 2340-2430</t>
+  </si>
+  <si>
+    <t>-1370</t>
+  </si>
+  <si>
+    <t>3830-</t>
+  </si>
+  <si>
+    <t>-270 2500-</t>
+  </si>
+  <si>
+    <t>-1130</t>
+  </si>
+  <si>
+    <t>-1130 2080-2300 2400-2500 26630-26730</t>
+  </si>
+  <si>
+    <t>80-240 300-450 700-980 1140-1630 1970-2120 5830-5920</t>
+  </si>
+  <si>
+    <t>2310-</t>
+  </si>
+  <si>
+    <t>-500 1100-</t>
+  </si>
+  <si>
+    <t>-1420 2330-2540</t>
+  </si>
+  <si>
+    <t>-830</t>
+  </si>
+  <si>
+    <t>1010-1120 1690-1770 2160-2420</t>
+  </si>
+  <si>
+    <t>1350-1530</t>
+  </si>
+  <si>
+    <t>-105 225-380 710-790 1310-1760</t>
+  </si>
+  <si>
+    <t>Deletion of ablation zone</t>
+  </si>
+  <si>
+    <t>4160-</t>
+  </si>
+  <si>
+    <t>10890-</t>
+  </si>
+  <si>
+    <t>4250-</t>
+  </si>
+  <si>
+    <t>7470-12440</t>
+  </si>
+  <si>
+    <t>-200 810-1600</t>
+  </si>
+  <si>
+    <t>-2860 6300-8920</t>
+  </si>
+  <si>
+    <t>450-1100</t>
+  </si>
+  <si>
+    <t>-210 1680-</t>
+  </si>
+  <si>
+    <t>-1000</t>
+  </si>
+  <si>
+    <t>2450-</t>
+  </si>
+  <si>
+    <t>19910-19990</t>
+  </si>
+  <si>
+    <t>-490</t>
+  </si>
+  <si>
+    <t>2455-3900</t>
+  </si>
+  <si>
+    <t>-965</t>
+  </si>
+  <si>
+    <t>35060-36700 37140-37590 38650-38910 40410-</t>
+  </si>
+  <si>
+    <t>-2800 3970-4665 6990-7350</t>
+  </si>
+  <si>
+    <t>-300 2565-3960 6280-</t>
+  </si>
+  <si>
+    <t>-825</t>
+  </si>
+  <si>
+    <t>-120</t>
+  </si>
+  <si>
+    <t>-1050</t>
+  </si>
+  <si>
+    <t>1050-</t>
+  </si>
+  <si>
+    <t>-900 1200-1740 2375-</t>
+  </si>
+  <si>
+    <t>6340-</t>
+  </si>
+  <si>
+    <t>-1380 5230-5710</t>
+  </si>
+  <si>
+    <t>1540-2230 5030-</t>
+  </si>
+  <si>
+    <t>-880 1490-2080 3460</t>
+  </si>
+  <si>
+    <t>2600-</t>
+  </si>
+  <si>
+    <t>4660-</t>
+  </si>
+  <si>
+    <t>6330-</t>
+  </si>
+  <si>
+    <t>-780 2880-3200 7030-7360 8700-9000 12460-</t>
+  </si>
+  <si>
+    <t>3700-4470 4760-5460 8200-</t>
+  </si>
+  <si>
+    <t>-1100</t>
+  </si>
+  <si>
+    <t>3000-</t>
+  </si>
+  <si>
+    <t>-1320 1450-1750 1870-2030</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2460-</t>
+  </si>
+  <si>
+    <t>-1260</t>
+  </si>
+  <si>
+    <t>-1270</t>
+  </si>
+  <si>
+    <t>-2600 4100-5800 6370-7250 11360-11820 17130-18480 19980-21440 25430-26250 28560-30485 34710-34810</t>
+  </si>
+  <si>
+    <t>26460-27760 30940-32180 35380-</t>
+  </si>
+  <si>
+    <t>1440-1690 1850-2220 2275-2330 2920-3650 3750-4120 4190-4330 4400-</t>
+  </si>
+  <si>
+    <t>-1170 2630-2900 3040-3355 4030-4120</t>
+  </si>
+  <si>
+    <t>-960</t>
+  </si>
+  <si>
+    <t>-90 1100-</t>
+  </si>
+  <si>
+    <t>-1300</t>
+  </si>
+  <si>
+    <t>1790-</t>
+  </si>
+  <si>
+    <t>-770</t>
+  </si>
+  <si>
+    <t>2230-2300 2360-2710</t>
+  </si>
+  <si>
+    <t>-970 5000-</t>
+  </si>
+  <si>
+    <t>1550-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-330 </t>
+  </si>
+  <si>
+    <t>8800-9770</t>
+  </si>
+  <si>
+    <t xml:space="preserve">-1130 </t>
+  </si>
+  <si>
+    <t>9350-</t>
+  </si>
+  <si>
+    <t>-560</t>
+  </si>
+  <si>
+    <t>2200-</t>
+  </si>
+  <si>
+    <t>-200</t>
+  </si>
+  <si>
+    <t>5400-</t>
+  </si>
+  <si>
+    <t>-270 4040-4320 6820-7200</t>
+  </si>
+  <si>
+    <t>3650-</t>
+  </si>
+  <si>
+    <t>3580-</t>
+  </si>
+  <si>
+    <t>-950 3160-</t>
+  </si>
+  <si>
+    <t>6370-7340</t>
+  </si>
+  <si>
+    <t>10880-</t>
+  </si>
+  <si>
+    <t>-3200</t>
+  </si>
+  <si>
+    <t>5780-</t>
+  </si>
+  <si>
+    <t>3750-</t>
+  </si>
+  <si>
+    <t>-275</t>
+  </si>
+  <si>
+    <t>-990</t>
+  </si>
+  <si>
+    <t>4860-</t>
+  </si>
+  <si>
+    <t>3820-</t>
+  </si>
+  <si>
+    <t>-1160</t>
+  </si>
+  <si>
+    <t>4850-</t>
+  </si>
+  <si>
+    <t>-1460</t>
+  </si>
+  <si>
+    <t>-1160 16560-</t>
+  </si>
+  <si>
+    <t>6720-</t>
+  </si>
+  <si>
+    <t>-1030 2810-3610 6570-6900 7920-8630</t>
+  </si>
+  <si>
+    <t>4390-</t>
+  </si>
+  <si>
+    <t>-1570 4093-4170</t>
+  </si>
+  <si>
+    <t>23180-</t>
+  </si>
+  <si>
+    <t>1770-</t>
+  </si>
+  <si>
+    <t>-850</t>
+  </si>
+  <si>
+    <t>3660-</t>
+  </si>
+  <si>
+    <t>3630-</t>
+  </si>
+  <si>
+    <t>-265</t>
+  </si>
+  <si>
+    <t>3470-</t>
+  </si>
+  <si>
+    <t>-40</t>
+  </si>
+  <si>
+    <t>2380-</t>
+  </si>
+  <si>
+    <t>-530</t>
+  </si>
+  <si>
+    <t>1385-1930 2170-2540</t>
+  </si>
+  <si>
+    <t>4040-</t>
+  </si>
+  <si>
+    <t>-100</t>
+  </si>
+  <si>
+    <t>-790 2010-</t>
+  </si>
+  <si>
+    <t>-910 3160-3510</t>
+  </si>
+  <si>
+    <t>-160 330-840 4000-4520 4730-4970 5000-</t>
+  </si>
+  <si>
+    <t>-800 2400-2970</t>
+  </si>
+  <si>
+    <t>3555-4260</t>
+  </si>
+  <si>
+    <t>8740-</t>
+  </si>
+  <si>
+    <t>-600</t>
   </si>
 </sst>
 </file>
@@ -1429,23 +1810,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
-  <dimension ref="A1:F193"/>
+  <dimension ref="A1:G193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A175" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D193" sqref="D193"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G142" sqref="G142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="20.453125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="25.1796875" customWidth="1"/>
+    <col min="3" max="3" width="4.36328125" customWidth="1"/>
     <col min="4" max="4" width="18.54296875" customWidth="1"/>
     <col min="5" max="5" width="16.36328125" customWidth="1"/>
-    <col min="6" max="6" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>191</v>
       </c>
@@ -1462,10 +1844,13 @@
         <v>232</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>321</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+        <v>372</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1475,11 +1860,14 @@
       <c r="C2" t="s">
         <v>201</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>322</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F2" s="4" t="s">
+        <v>373</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -1490,8 +1878,9 @@
         <v>197</v>
       </c>
       <c r="F3" s="6"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G3" s="6"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1507,11 +1896,14 @@
       <c r="E4" t="s">
         <v>233</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>323</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F4" s="4">
+        <v>-910</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1521,11 +1913,11 @@
       <c r="C5" t="s">
         <v>201</v>
       </c>
-      <c r="F5" s="4">
+      <c r="G5" s="4">
         <v>-620</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>4</v>
       </c>
@@ -1535,13 +1927,14 @@
       <c r="C6" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F6" s="7" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="F6" s="7"/>
+      <c r="G6" s="7" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>194</v>
@@ -1550,13 +1943,14 @@
         <v>201</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="F7" s="7" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>318</v>
+      </c>
+      <c r="F7" s="7"/>
+      <c r="G7" s="7" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>5</v>
       </c>
@@ -1566,11 +1960,12 @@
       <c r="C8" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F8" s="7" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F8" s="7"/>
+      <c r="G8" s="7" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>6</v>
       </c>
@@ -1580,11 +1975,14 @@
       <c r="C9" t="s">
         <v>201</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F9" s="4" t="s">
+        <v>374</v>
+      </c>
+      <c r="G9" s="8" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>7</v>
       </c>
@@ -1594,11 +1992,11 @@
       <c r="C10" t="s">
         <v>201</v>
       </c>
-      <c r="F10" s="9" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G10" s="9" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -1608,11 +2006,14 @@
       <c r="C11" t="s">
         <v>201</v>
       </c>
-      <c r="F11" s="9" t="s">
-        <v>327</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F11" s="4" t="s">
+        <v>375</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1620,10 +2021,10 @@
         <v>194</v>
       </c>
       <c r="C12" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -1634,16 +2035,19 @@
         <v>201</v>
       </c>
       <c r="D13" t="s">
+        <v>311</v>
+      </c>
+      <c r="E13" t="s">
         <v>312</v>
       </c>
-      <c r="E13" t="s">
-        <v>313</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>328</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F13" s="4" t="s">
+        <v>376</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -1654,13 +2058,16 @@
         <v>201</v>
       </c>
       <c r="E14" t="s">
-        <v>314</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>329</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>313</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>377</v>
+      </c>
+      <c r="G14" s="5" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
@@ -1670,11 +2077,12 @@
       <c r="C15" s="3" t="s">
         <v>201</v>
       </c>
-      <c r="F15" s="7" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F15" s="7"/>
+      <c r="G15" s="7" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1685,13 +2093,16 @@
         <v>201</v>
       </c>
       <c r="E16" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+        <v>378</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -1702,13 +2113,16 @@
         <v>201</v>
       </c>
       <c r="E17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="F17" s="4" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+        <v>379</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>15</v>
       </c>
@@ -1716,10 +2130,10 @@
         <v>194</v>
       </c>
       <c r="C18" t="s">
-        <v>311</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>16</v>
       </c>
@@ -1732,11 +2146,12 @@
       <c r="E19" s="3">
         <v>-640</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F19" s="7"/>
+      <c r="G19" s="7" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>17</v>
       </c>
@@ -1747,10 +2162,13 @@
         <v>201</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+        <v>380</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -1761,10 +2179,13 @@
         <v>201</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>333</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
+        <v>382</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -1774,11 +2195,11 @@
       <c r="C22" t="s">
         <v>201</v>
       </c>
-      <c r="F22" s="4" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G22" s="4" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>20</v>
       </c>
@@ -1789,10 +2210,13 @@
         <v>201</v>
       </c>
       <c r="F23" s="4" t="s">
-        <v>335</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+        <v>333</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>21</v>
       </c>
@@ -1809,10 +2233,13 @@
         <v>234</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>336</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
+        <v>383</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>22</v>
       </c>
@@ -1825,11 +2252,11 @@
       <c r="D25" t="s">
         <v>205</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="G25" s="4" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>23</v>
       </c>
@@ -1840,10 +2267,13 @@
         <v>201</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>338</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+        <v>336</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>24</v>
       </c>
@@ -1854,10 +2284,13 @@
         <v>201</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>339</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+        <v>384</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>25</v>
       </c>
@@ -1870,11 +2303,12 @@
       <c r="D28" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="F28" s="7" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F28" s="7"/>
+      <c r="G28" s="7" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>26</v>
       </c>
@@ -1888,10 +2322,13 @@
         <v>235</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+        <v>385</v>
+      </c>
+      <c r="G29" s="4" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>27</v>
       </c>
@@ -1905,10 +2342,13 @@
         <v>236</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
+        <v>386</v>
+      </c>
+      <c r="G30" s="4" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>28</v>
       </c>
@@ -1921,8 +2361,14 @@
       <c r="E31" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F31" s="4" t="s">
+        <v>387</v>
+      </c>
+      <c r="G31" s="4" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>29</v>
       </c>
@@ -1935,8 +2381,14 @@
       <c r="E32" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F32" s="4" t="s">
+        <v>388</v>
+      </c>
+      <c r="G32" s="4" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>30</v>
       </c>
@@ -1949,8 +2401,14 @@
       <c r="E33" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F33" s="4" t="s">
+        <v>389</v>
+      </c>
+      <c r="G33" s="4" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>31</v>
       </c>
@@ -1963,8 +2421,14 @@
       <c r="E34" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F34" s="4" t="s">
+        <v>390</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>32</v>
       </c>
@@ -1974,8 +2438,11 @@
       <c r="C35" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G35" s="4" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>33</v>
       </c>
@@ -1985,8 +2452,14 @@
       <c r="C36" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F36" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="G36" s="4" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>34</v>
       </c>
@@ -1996,8 +2469,14 @@
       <c r="C37" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F37" s="4" t="s">
+        <v>394</v>
+      </c>
+      <c r="G37" s="4" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>35</v>
       </c>
@@ -2014,7 +2493,7 @@
         <v>-1815</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>36</v>
       </c>
@@ -2030,8 +2509,14 @@
       <c r="E39">
         <v>-375</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F39" s="4" t="s">
+        <v>395</v>
+      </c>
+      <c r="G39" s="4" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>37</v>
       </c>
@@ -2044,8 +2529,11 @@
       <c r="E40" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F40" s="4" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>38</v>
       </c>
@@ -2058,8 +2546,11 @@
       <c r="E41" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F41" s="4" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>39</v>
       </c>
@@ -2072,8 +2563,14 @@
       <c r="E42" s="1" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F42" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="G42" s="4" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>40</v>
       </c>
@@ -2086,8 +2583,11 @@
       <c r="E43" s="1" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F43" s="5" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>41</v>
       </c>
@@ -2100,8 +2600,11 @@
       <c r="E44" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G44" s="4" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>42</v>
       </c>
@@ -2114,8 +2617,11 @@
       <c r="E45" s="1">
         <v>-1840</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F45" s="5" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
         <v>43</v>
       </c>
@@ -2129,7 +2635,7 @@
         <v>-625</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
         <v>44</v>
       </c>
@@ -2142,8 +2648,11 @@
       <c r="E47" s="1" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F47" s="5" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
         <v>45</v>
       </c>
@@ -2154,10 +2663,13 @@
         <v>201</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+        <v>352</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
         <v>46</v>
       </c>
@@ -2168,7 +2680,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
         <v>47</v>
       </c>
@@ -2178,8 +2690,11 @@
       <c r="C50" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G50" s="4" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
         <v>48</v>
       </c>
@@ -2190,10 +2705,16 @@
         <v>201</v>
       </c>
       <c r="E51" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+        <v>247</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="G51" s="4" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
         <v>49</v>
       </c>
@@ -2204,10 +2725,16 @@
         <v>201</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+        <v>248</v>
+      </c>
+      <c r="F52" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="G52" s="4" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
         <v>50</v>
       </c>
@@ -2218,10 +2745,16 @@
         <v>201</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+        <v>249</v>
+      </c>
+      <c r="F53" s="5" t="s">
+        <v>404</v>
+      </c>
+      <c r="G53" s="4" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
         <v>51</v>
       </c>
@@ -2232,10 +2765,14 @@
         <v>201</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+        <v>250</v>
+      </c>
+      <c r="F54" s="5"/>
+      <c r="G54" s="4" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
         <v>52</v>
       </c>
@@ -2246,10 +2783,13 @@
         <v>201</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+        <v>251</v>
+      </c>
+      <c r="F55" s="4" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
         <v>53</v>
       </c>
@@ -2260,10 +2800,16 @@
         <v>201</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
+        <v>252</v>
+      </c>
+      <c r="F56" s="5" t="s">
+        <v>405</v>
+      </c>
+      <c r="G56" s="4" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
         <v>54</v>
       </c>
@@ -2273,8 +2819,11 @@
       <c r="C57" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F57" s="4" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
         <v>55</v>
       </c>
@@ -2285,10 +2834,11 @@
         <v>201</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>254</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+        <v>253</v>
+      </c>
+      <c r="F58" s="5"/>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
         <v>56</v>
       </c>
@@ -2298,8 +2848,14 @@
       <c r="C59" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F59" s="4" t="s">
+        <v>407</v>
+      </c>
+      <c r="G59" s="4" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
         <v>57</v>
       </c>
@@ -2309,8 +2865,14 @@
       <c r="C60" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F60" s="4" t="s">
+        <v>408</v>
+      </c>
+      <c r="G60" s="4" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A61" t="s">
         <v>58</v>
       </c>
@@ -2324,10 +2886,13 @@
         <v>211</v>
       </c>
       <c r="E61" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+        <v>254</v>
+      </c>
+      <c r="G61" s="4" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A62" t="s">
         <v>59</v>
       </c>
@@ -2338,10 +2903,16 @@
         <v>201</v>
       </c>
       <c r="E62" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+        <v>255</v>
+      </c>
+      <c r="F62" s="4" t="s">
+        <v>411</v>
+      </c>
+      <c r="G62" s="4" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A63" t="s">
         <v>60</v>
       </c>
@@ -2354,8 +2925,14 @@
       <c r="E63">
         <v>-840</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F63" s="4" t="s">
+        <v>413</v>
+      </c>
+      <c r="G63" s="4" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A64" t="s">
         <v>61</v>
       </c>
@@ -2366,13 +2943,19 @@
         <v>201</v>
       </c>
       <c r="D64" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="E64" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+        <v>256</v>
+      </c>
+      <c r="F64" s="4" t="s">
+        <v>414</v>
+      </c>
+      <c r="G64" s="4" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A65" t="s">
         <v>62</v>
       </c>
@@ -2383,10 +2966,13 @@
         <v>201</v>
       </c>
       <c r="D65" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+        <v>319</v>
+      </c>
+      <c r="G65" s="4" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A66" t="s">
         <v>63</v>
       </c>
@@ -2396,8 +2982,11 @@
       <c r="C66" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F66" s="4" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
         <v>64</v>
       </c>
@@ -2408,10 +2997,16 @@
         <v>201</v>
       </c>
       <c r="E67" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+        <v>257</v>
+      </c>
+      <c r="F67" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="G67" s="4" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A68" t="s">
         <v>65</v>
       </c>
@@ -2424,8 +3019,14 @@
       <c r="E68">
         <v>-840</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F68" s="4" t="s">
+        <v>416</v>
+      </c>
+      <c r="G68" s="4" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A69" t="s">
         <v>66</v>
       </c>
@@ -2436,7 +3037,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A70" t="s">
         <v>67</v>
       </c>
@@ -2447,10 +3048,10 @@
         <v>201</v>
       </c>
       <c r="E70" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A71" t="s">
         <v>68</v>
       </c>
@@ -2460,8 +3061,14 @@
       <c r="C71" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F71" s="4" t="s">
+        <v>368</v>
+      </c>
+      <c r="G71" s="4" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A72" t="s">
         <v>69</v>
       </c>
@@ -2474,8 +3081,14 @@
       <c r="E72">
         <v>-610</v>
       </c>
-    </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F72" s="4" t="s">
+        <v>418</v>
+      </c>
+      <c r="G72" s="4" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A73" t="s">
         <v>70</v>
       </c>
@@ -2485,8 +3098,11 @@
       <c r="C73" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="G73" s="4" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A74" t="s">
         <v>71</v>
       </c>
@@ -2497,10 +3113,16 @@
         <v>201</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>260</v>
-      </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+        <v>259</v>
+      </c>
+      <c r="F74" s="5" t="s">
+        <v>420</v>
+      </c>
+      <c r="G74" s="4" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A75" t="s">
         <v>72</v>
       </c>
@@ -2510,8 +3132,14 @@
       <c r="C75" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F75" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="G75" s="4" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A76" t="s">
         <v>73</v>
       </c>
@@ -2522,7 +3150,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A77" t="s">
         <v>74</v>
       </c>
@@ -2536,10 +3164,16 @@
         <v>212</v>
       </c>
       <c r="E77" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+        <v>260</v>
+      </c>
+      <c r="F77" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="G77" s="4" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
         <v>75</v>
       </c>
@@ -2552,8 +3186,14 @@
       <c r="D78" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F78" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="G78" s="4" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A79" t="s">
         <v>76</v>
       </c>
@@ -2566,8 +3206,11 @@
       <c r="D79" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F79" s="4" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A80" t="s">
         <v>77</v>
       </c>
@@ -2577,8 +3220,11 @@
       <c r="C80" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F80" s="4" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>78</v>
       </c>
@@ -2591,8 +3237,11 @@
       <c r="D81" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F81" s="4" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>79</v>
       </c>
@@ -2603,10 +3252,10 @@
         <v>201</v>
       </c>
       <c r="E82" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>80</v>
       </c>
@@ -2617,7 +3266,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>81</v>
       </c>
@@ -2627,8 +3276,11 @@
       <c r="C84" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F84" s="4" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>82</v>
       </c>
@@ -2642,10 +3294,13 @@
         <v>210</v>
       </c>
       <c r="E85" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+        <v>262</v>
+      </c>
+      <c r="F85" s="4" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>83</v>
       </c>
@@ -2656,10 +3311,13 @@
         <v>201</v>
       </c>
       <c r="E86" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+        <v>263</v>
+      </c>
+      <c r="F86" s="4" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>84</v>
       </c>
@@ -2670,10 +3328,11 @@
         <v>201</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>265</v>
-      </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+        <v>264</v>
+      </c>
+      <c r="F87" s="5"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>85</v>
       </c>
@@ -2683,8 +3342,11 @@
       <c r="C88" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F88" s="4" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>86</v>
       </c>
@@ -2697,8 +3359,11 @@
       <c r="E89">
         <v>-750</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F89" s="4" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>87</v>
       </c>
@@ -2709,10 +3374,13 @@
         <v>201</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+        <v>265</v>
+      </c>
+      <c r="F90" s="5" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>88</v>
       </c>
@@ -2723,7 +3391,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>89</v>
       </c>
@@ -2733,8 +3401,11 @@
       <c r="C92" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F92" s="4" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>90</v>
       </c>
@@ -2745,10 +3416,13 @@
         <v>201</v>
       </c>
       <c r="E93" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+        <v>266</v>
+      </c>
+      <c r="F93" s="4" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>91</v>
       </c>
@@ -2761,8 +3435,11 @@
       <c r="D94" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F94" s="4" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>92</v>
       </c>
@@ -2772,8 +3449,11 @@
       <c r="C95" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F95" s="4" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>93</v>
       </c>
@@ -2784,7 +3464,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>94</v>
       </c>
@@ -2794,8 +3474,11 @@
       <c r="C97" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F97" s="4" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>95</v>
       </c>
@@ -2806,10 +3489,13 @@
         <v>201</v>
       </c>
       <c r="E98" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.35">
+        <v>267</v>
+      </c>
+      <c r="F98" s="4" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>96</v>
       </c>
@@ -2823,10 +3509,10 @@
         <v>217</v>
       </c>
       <c r="E99" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.35">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>97</v>
       </c>
@@ -2836,8 +3522,11 @@
       <c r="C100" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F100" s="4" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>98</v>
       </c>
@@ -2847,8 +3536,11 @@
       <c r="C101" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F101" s="4" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>99</v>
       </c>
@@ -2862,7 +3554,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>100</v>
       </c>
@@ -2876,10 +3568,13 @@
         <v>221</v>
       </c>
       <c r="E103" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.35">
+        <v>269</v>
+      </c>
+      <c r="F103" s="4" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>101</v>
       </c>
@@ -2889,8 +3584,11 @@
       <c r="C104" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F104" s="4" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A105" t="s">
         <v>102</v>
       </c>
@@ -2901,7 +3599,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>103</v>
       </c>
@@ -2911,8 +3609,11 @@
       <c r="C106" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F106" s="4" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>104</v>
       </c>
@@ -2923,10 +3624,13 @@
         <v>201</v>
       </c>
       <c r="E107" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.35">
+        <v>270</v>
+      </c>
+      <c r="F107" s="4" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>105</v>
       </c>
@@ -2937,10 +3641,13 @@
         <v>201</v>
       </c>
       <c r="E108" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.35">
+        <v>271</v>
+      </c>
+      <c r="F108" s="4" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>106</v>
       </c>
@@ -2951,10 +3658,13 @@
         <v>201</v>
       </c>
       <c r="E109" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.35">
+        <v>272</v>
+      </c>
+      <c r="F109" s="4" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>107</v>
       </c>
@@ -2965,10 +3675,13 @@
         <v>201</v>
       </c>
       <c r="E110" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.35">
+        <v>273</v>
+      </c>
+      <c r="F110" s="4" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>108</v>
       </c>
@@ -2979,10 +3692,10 @@
         <v>201</v>
       </c>
       <c r="E111" t="s">
-        <v>275</v>
-      </c>
-    </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.35">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>109</v>
       </c>
@@ -2992,8 +3705,11 @@
       <c r="C112" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F112" s="4" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>110</v>
       </c>
@@ -3004,10 +3720,13 @@
         <v>201</v>
       </c>
       <c r="E113" t="s">
-        <v>276</v>
-      </c>
-    </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.35">
+        <v>275</v>
+      </c>
+      <c r="F113" s="4" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>111</v>
       </c>
@@ -3018,10 +3737,13 @@
         <v>201</v>
       </c>
       <c r="E114" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.35">
+        <v>276</v>
+      </c>
+      <c r="F114" s="4" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>112</v>
       </c>
@@ -3032,10 +3754,13 @@
         <v>201</v>
       </c>
       <c r="E115" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.35">
+        <v>277</v>
+      </c>
+      <c r="F115" s="4" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>113</v>
       </c>
@@ -3048,8 +3773,11 @@
       <c r="D116" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F116" s="4" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>114</v>
       </c>
@@ -3062,8 +3790,11 @@
       <c r="D117" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F117" s="4" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>115</v>
       </c>
@@ -3077,10 +3808,13 @@
         <v>223</v>
       </c>
       <c r="E118" t="s">
-        <v>279</v>
-      </c>
-    </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.35">
+        <v>278</v>
+      </c>
+      <c r="F118" s="4" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>116</v>
       </c>
@@ -3091,10 +3825,13 @@
         <v>201</v>
       </c>
       <c r="E119" t="s">
-        <v>280</v>
-      </c>
-    </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.35">
+        <v>279</v>
+      </c>
+      <c r="F119" s="4" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>117</v>
       </c>
@@ -3104,8 +3841,11 @@
       <c r="C120" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F120" s="4" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>118</v>
       </c>
@@ -3116,10 +3856,13 @@
         <v>201</v>
       </c>
       <c r="E121" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.35">
+        <v>280</v>
+      </c>
+      <c r="F121" s="4" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>119</v>
       </c>
@@ -3129,8 +3872,11 @@
       <c r="C122" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F122" s="4" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>120</v>
       </c>
@@ -3140,8 +3886,11 @@
       <c r="C123" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F123" s="4" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>121</v>
       </c>
@@ -3151,8 +3900,11 @@
       <c r="C124" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F124" s="4" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>122</v>
       </c>
@@ -3162,8 +3914,11 @@
       <c r="C125" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F125" s="4" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>123</v>
       </c>
@@ -3174,10 +3929,13 @@
         <v>201</v>
       </c>
       <c r="E126" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.35">
+        <v>281</v>
+      </c>
+      <c r="F126" s="4" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>124</v>
       </c>
@@ -3187,8 +3945,11 @@
       <c r="C127" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F127" s="4" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>125</v>
       </c>
@@ -3198,8 +3959,11 @@
       <c r="C128" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F128" s="4" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>126</v>
       </c>
@@ -3209,8 +3973,11 @@
       <c r="C129" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F129" s="4" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A130" t="s">
         <v>127</v>
       </c>
@@ -3221,7 +3988,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>128</v>
       </c>
@@ -3232,10 +3999,13 @@
         <v>201</v>
       </c>
       <c r="E131" t="s">
-        <v>283</v>
-      </c>
-    </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.35">
+        <v>282</v>
+      </c>
+      <c r="F131" s="4" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>129</v>
       </c>
@@ -3246,10 +4016,13 @@
         <v>201</v>
       </c>
       <c r="E132" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.35">
+        <v>283</v>
+      </c>
+      <c r="F132" s="4" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>130</v>
       </c>
@@ -3262,8 +4035,11 @@
       <c r="E133">
         <v>-590</v>
       </c>
-    </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F133" s="4" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>131</v>
       </c>
@@ -3274,10 +4050,13 @@
         <v>201</v>
       </c>
       <c r="E134" t="s">
-        <v>285</v>
-      </c>
-    </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.35">
+        <v>284</v>
+      </c>
+      <c r="F134" s="4" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>132</v>
       </c>
@@ -3287,8 +4066,11 @@
       <c r="C135" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F135" s="4" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>133</v>
       </c>
@@ -3299,10 +4081,13 @@
         <v>201</v>
       </c>
       <c r="E136" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.35">
+        <v>285</v>
+      </c>
+      <c r="F136" s="4" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>134</v>
       </c>
@@ -3313,10 +4098,13 @@
         <v>201</v>
       </c>
       <c r="E137" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.35">
+        <v>286</v>
+      </c>
+      <c r="F137" s="4" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>135</v>
       </c>
@@ -3327,7 +4115,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>136</v>
       </c>
@@ -3338,10 +4126,13 @@
         <v>201</v>
       </c>
       <c r="E139" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.35">
+        <v>287</v>
+      </c>
+      <c r="F139" s="4" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>137</v>
       </c>
@@ -3352,10 +4143,10 @@
         <v>201</v>
       </c>
       <c r="E140" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.35">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>138</v>
       </c>
@@ -3365,8 +4156,11 @@
       <c r="C141" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F141" s="4" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>139</v>
       </c>
@@ -3376,8 +4170,11 @@
       <c r="C142" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F142" s="4" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>140</v>
       </c>
@@ -3391,7 +4188,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>141</v>
       </c>
@@ -3419,7 +4216,7 @@
         <v>219</v>
       </c>
       <c r="E145" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.35">
@@ -3455,7 +4252,7 @@
         <v>201</v>
       </c>
       <c r="E148" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.35">
@@ -3469,7 +4266,7 @@
         <v>201</v>
       </c>
       <c r="E149" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.35">
@@ -3519,7 +4316,7 @@
         <v>201</v>
       </c>
       <c r="E153" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.35">
@@ -3580,7 +4377,7 @@
         <v>201</v>
       </c>
       <c r="E158" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.35">
@@ -3594,7 +4391,7 @@
         <v>201</v>
       </c>
       <c r="E159" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.35">
@@ -3625,7 +4422,7 @@
         <v>224</v>
       </c>
       <c r="E161" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="162" spans="1:5" x14ac:dyDescent="0.35">
@@ -3700,7 +4497,7 @@
         <v>201</v>
       </c>
       <c r="E167" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="168" spans="1:5" x14ac:dyDescent="0.35">
@@ -3753,7 +4550,7 @@
         <v>201</v>
       </c>
       <c r="E171" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.35">
@@ -3792,7 +4589,7 @@
         <v>201</v>
       </c>
       <c r="E174" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.35">
@@ -3820,7 +4617,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="177" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
         <v>174</v>
       </c>
@@ -3834,10 +4631,10 @@
         <v>230</v>
       </c>
       <c r="E177" t="s">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="178" spans="1:6" x14ac:dyDescent="0.35">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="178" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
         <v>175</v>
       </c>
@@ -3848,7 +4645,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="179" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
         <v>176</v>
       </c>
@@ -3859,10 +4656,10 @@
         <v>201</v>
       </c>
       <c r="E179" t="s">
-        <v>301</v>
-      </c>
-    </row>
-    <row r="180" spans="1:6" x14ac:dyDescent="0.35">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="180" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
         <v>177</v>
       </c>
@@ -3876,7 +4673,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="181" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
         <v>178</v>
       </c>
@@ -3887,10 +4684,10 @@
         <v>201</v>
       </c>
       <c r="E181" t="s">
-        <v>302</v>
-      </c>
-    </row>
-    <row r="182" spans="1:6" x14ac:dyDescent="0.35">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="182" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
         <v>179</v>
       </c>
@@ -3901,10 +4698,10 @@
         <v>201</v>
       </c>
       <c r="E182" t="s">
-        <v>304</v>
-      </c>
-    </row>
-    <row r="183" spans="1:6" x14ac:dyDescent="0.35">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="183" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
         <v>180</v>
       </c>
@@ -3915,10 +4712,10 @@
         <v>201</v>
       </c>
       <c r="E183" t="s">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="184" spans="1:6" x14ac:dyDescent="0.35">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="184" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A184" t="s">
         <v>181</v>
       </c>
@@ -3929,7 +4726,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="185" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
         <v>182</v>
       </c>
@@ -3940,7 +4737,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="186" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A186" t="s">
         <v>183</v>
       </c>
@@ -3954,7 +4751,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="187" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
         <v>184</v>
       </c>
@@ -3965,7 +4762,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="188" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
         <v>185</v>
       </c>
@@ -3976,10 +4773,10 @@
         <v>201</v>
       </c>
       <c r="E188" t="s">
-        <v>305</v>
-      </c>
-    </row>
-    <row r="189" spans="1:6" x14ac:dyDescent="0.35">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="189" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
         <v>186</v>
       </c>
@@ -3993,10 +4790,10 @@
         <v>208</v>
       </c>
       <c r="E189" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="190" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.35">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="190" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A190" s="2" t="s">
         <v>187</v>
       </c>
@@ -4010,13 +4807,14 @@
         <v>231</v>
       </c>
       <c r="E190" s="2" t="s">
-        <v>307</v>
-      </c>
-      <c r="F190" s="6" t="s">
-        <v>343</v>
-      </c>
-    </row>
-    <row r="191" spans="1:6" x14ac:dyDescent="0.35">
+        <v>306</v>
+      </c>
+      <c r="F190" s="6"/>
+      <c r="G190" s="6" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="191" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A191" t="s">
         <v>188</v>
       </c>
@@ -4027,10 +4825,10 @@
         <v>201</v>
       </c>
       <c r="E191" t="s">
-        <v>308</v>
-      </c>
-    </row>
-    <row r="192" spans="1:6" x14ac:dyDescent="0.35">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="192" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
         <v>189</v>
       </c>
@@ -4041,7 +4839,7 @@
         <v>201</v>
       </c>
       <c r="E192" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.35">
@@ -4055,7 +4853,7 @@
         <v>201</v>
       </c>
       <c r="E193" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating the exclusion excel file.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FE50A3B-3A82-4AFB-946E-861862DCF278}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463933D8-C90B-4A71-BE91-2ACEE1E90667}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3680" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="470">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -996,7 +996,7 @@
     <t>-910 -2115'</t>
   </si>
   <si>
-    <t>To delete because very bad</t>
+    <t>Deleted because very bad</t>
   </si>
   <si>
     <t>9180-10400</t>
@@ -1039,9 +1039,6 @@
   </si>
   <si>
     <t>-1010</t>
-  </si>
-  <si>
-    <t>to delete because bad</t>
   </si>
   <si>
     <t>-3920 5100-7120</t>
@@ -1453,7 +1450,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1463,12 +1460,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1485,15 +1476,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
@@ -1812,8 +1801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
   <dimension ref="A1:G193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G142" sqref="G142"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1823,8 +1812,8 @@
     <col min="3" max="3" width="4.36328125" customWidth="1"/>
     <col min="4" max="4" width="18.54296875" customWidth="1"/>
     <col min="5" max="5" width="16.36328125" customWidth="1"/>
-    <col min="6" max="6" width="16.36328125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="9.36328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.36328125" style="3" customWidth="1"/>
+    <col min="7" max="7" width="9.36328125" style="3" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.35">
@@ -1843,10 +1832,10 @@
       <c r="E1" t="s">
         <v>232</v>
       </c>
-      <c r="F1" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="G1" s="4" t="s">
+      <c r="F1" s="3" t="s">
+        <v>371</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>320</v>
       </c>
     </row>
@@ -1860,10 +1849,10 @@
       <c r="C2" t="s">
         <v>201</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>373</v>
-      </c>
-      <c r="G2" s="5" t="s">
+      <c r="F2" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>321</v>
       </c>
     </row>
@@ -1877,8 +1866,8 @@
       <c r="C3" s="2" t="s">
         <v>197</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="G3" s="6"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
@@ -1896,10 +1885,10 @@
       <c r="E4" t="s">
         <v>233</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>-910</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="G4" s="4" t="s">
         <v>322</v>
       </c>
     </row>
@@ -1913,55 +1902,55 @@
       <c r="C5" t="s">
         <v>201</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>-620</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7" t="s">
+      <c r="C6" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
         <v>317</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="E7" s="3" t="s">
+      <c r="C7" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E7" s="2" t="s">
         <v>318</v>
       </c>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7" t="s">
+      <c r="F7" s="5"/>
+      <c r="G7" s="5" t="s">
         <v>323</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="F8" s="7"/>
-      <c r="G8" s="7" t="s">
+      <c r="C8" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5" t="s">
         <v>323</v>
       </c>
     </row>
@@ -1975,10 +1964,10 @@
       <c r="C9" t="s">
         <v>201</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>374</v>
-      </c>
-      <c r="G9" s="8" t="s">
+      <c r="F9" s="3" t="s">
+        <v>373</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>324</v>
       </c>
     </row>
@@ -1992,7 +1981,7 @@
       <c r="C10" t="s">
         <v>201</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="7" t="s">
         <v>325</v>
       </c>
     </row>
@@ -2006,23 +1995,25 @@
       <c r="C11" t="s">
         <v>201</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>375</v>
-      </c>
-      <c r="G11" s="9" t="s">
+      <c r="F11" s="3" t="s">
+        <v>374</v>
+      </c>
+      <c r="G11" s="7" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+    <row r="12" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="2" t="s">
         <v>310</v>
       </c>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -2040,10 +2031,10 @@
       <c r="E13" t="s">
         <v>312</v>
       </c>
-      <c r="F13" s="4" t="s">
-        <v>376</v>
-      </c>
-      <c r="G13" s="5" t="s">
+      <c r="F13" s="3" t="s">
+        <v>375</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>327</v>
       </c>
     </row>
@@ -2060,25 +2051,25 @@
       <c r="E14" t="s">
         <v>313</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>377</v>
-      </c>
-      <c r="G14" s="5" t="s">
+      <c r="F14" s="3" t="s">
+        <v>376</v>
+      </c>
+      <c r="G14" s="4" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
+    <row r="15" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C15" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7" t="s">
+      <c r="C15" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5" t="s">
         <v>323</v>
       </c>
     </row>
@@ -2095,10 +2086,10 @@
       <c r="E16" t="s">
         <v>314</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>378</v>
-      </c>
-      <c r="G16" s="4" t="s">
+      <c r="F16" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="G16" s="3" t="s">
         <v>329</v>
       </c>
     </row>
@@ -2115,39 +2106,41 @@
       <c r="E17" t="s">
         <v>315</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>379</v>
-      </c>
-      <c r="G17" s="4" t="s">
+      <c r="F17" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="G17" s="3" t="s">
         <v>330</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+    <row r="18" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="2" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+    </row>
+    <row r="19" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="E19" s="3">
+      <c r="C19" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="E19" s="2">
         <v>-640</v>
       </c>
-      <c r="F19" s="7"/>
-      <c r="G19" s="7" t="s">
+      <c r="F19" s="5"/>
+      <c r="G19" s="5" t="s">
         <v>323</v>
       </c>
     </row>
@@ -2161,10 +2154,10 @@
       <c r="C20" t="s">
         <v>201</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>380</v>
-      </c>
-      <c r="G20" s="4" t="s">
+      <c r="F20" s="3" t="s">
+        <v>379</v>
+      </c>
+      <c r="G20" s="3" t="s">
         <v>331</v>
       </c>
     </row>
@@ -2178,11 +2171,11 @@
       <c r="C21" t="s">
         <v>201</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>382</v>
-      </c>
-      <c r="G21" s="4" t="s">
+      <c r="F21" s="3" t="s">
         <v>381</v>
+      </c>
+      <c r="G21" s="3" t="s">
+        <v>380</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.35">
@@ -2195,7 +2188,7 @@
       <c r="C22" t="s">
         <v>201</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="3" t="s">
         <v>332</v>
       </c>
     </row>
@@ -2209,10 +2202,10 @@
       <c r="C23" t="s">
         <v>201</v>
       </c>
-      <c r="F23" s="4" t="s">
+      <c r="F23" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="G23" s="4" t="s">
+      <c r="G23" s="3" t="s">
         <v>333</v>
       </c>
     </row>
@@ -2232,10 +2225,10 @@
       <c r="E24" t="s">
         <v>234</v>
       </c>
-      <c r="F24" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="G24" s="4" t="s">
+      <c r="F24" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="G24" s="3" t="s">
         <v>334</v>
       </c>
     </row>
@@ -2252,7 +2245,7 @@
       <c r="D25" t="s">
         <v>205</v>
       </c>
-      <c r="G25" s="4" t="s">
+      <c r="G25" s="3" t="s">
         <v>335</v>
       </c>
     </row>
@@ -2266,10 +2259,10 @@
       <c r="C26" t="s">
         <v>201</v>
       </c>
-      <c r="F26" s="4" t="s">
+      <c r="F26" s="3" t="s">
         <v>336</v>
       </c>
-      <c r="G26" s="4" t="s">
+      <c r="G26" s="3" t="s">
         <v>336</v>
       </c>
     </row>
@@ -2283,29 +2276,29 @@
       <c r="C27" t="s">
         <v>201</v>
       </c>
-      <c r="F27" s="4" t="s">
-        <v>384</v>
-      </c>
-      <c r="G27" s="4" t="s">
+      <c r="F27" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="G27" s="3" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A28" s="3" t="s">
+    <row r="28" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>193</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>201</v>
-      </c>
-      <c r="D28" s="3" t="s">
+      <c r="B28" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D28" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7" t="s">
-        <v>338</v>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.35">
@@ -2321,11 +2314,11 @@
       <c r="E29" t="s">
         <v>235</v>
       </c>
-      <c r="F29" s="4" t="s">
-        <v>385</v>
-      </c>
-      <c r="G29" s="4" t="s">
-        <v>339</v>
+      <c r="F29" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>338</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.35">
@@ -2341,11 +2334,11 @@
       <c r="E30" t="s">
         <v>236</v>
       </c>
-      <c r="F30" s="4" t="s">
-        <v>386</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>340</v>
+      <c r="F30" s="3" t="s">
+        <v>385</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>339</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.35">
@@ -2361,11 +2354,11 @@
       <c r="E31" t="s">
         <v>237</v>
       </c>
-      <c r="F31" s="4" t="s">
-        <v>387</v>
-      </c>
-      <c r="G31" s="4" t="s">
-        <v>342</v>
+      <c r="F31" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.35">
@@ -2381,11 +2374,11 @@
       <c r="E32" t="s">
         <v>238</v>
       </c>
-      <c r="F32" s="4" t="s">
-        <v>388</v>
-      </c>
-      <c r="G32" s="4" t="s">
-        <v>343</v>
+      <c r="F32" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.35">
@@ -2401,11 +2394,11 @@
       <c r="E33" t="s">
         <v>239</v>
       </c>
-      <c r="F33" s="4" t="s">
-        <v>389</v>
-      </c>
-      <c r="G33" s="4" t="s">
-        <v>344</v>
+      <c r="F33" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>343</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
@@ -2421,11 +2414,11 @@
       <c r="E34" t="s">
         <v>240</v>
       </c>
-      <c r="F34" s="4" t="s">
-        <v>390</v>
-      </c>
-      <c r="G34" s="4" t="s">
-        <v>345</v>
+      <c r="F34" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>344</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
@@ -2438,8 +2431,8 @@
       <c r="C35" t="s">
         <v>201</v>
       </c>
-      <c r="G35" s="4" t="s">
-        <v>346</v>
+      <c r="G35" s="3" t="s">
+        <v>345</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.35">
@@ -2452,11 +2445,11 @@
       <c r="C36" t="s">
         <v>201</v>
       </c>
-      <c r="F36" s="4" t="s">
-        <v>393</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>347</v>
+      <c r="F36" s="3" t="s">
+        <v>392</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>346</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.35">
@@ -2469,11 +2462,11 @@
       <c r="C37" t="s">
         <v>201</v>
       </c>
-      <c r="F37" s="4" t="s">
-        <v>394</v>
-      </c>
-      <c r="G37" s="4" t="s">
-        <v>348</v>
+      <c r="F37" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="G37" s="3" t="s">
+        <v>347</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.35">
@@ -2509,11 +2502,11 @@
       <c r="E39">
         <v>-375</v>
       </c>
-      <c r="F39" s="4" t="s">
-        <v>395</v>
-      </c>
-      <c r="G39" s="4" t="s">
-        <v>349</v>
+      <c r="F39" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="G39" s="3" t="s">
+        <v>348</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
@@ -2529,8 +2522,8 @@
       <c r="E40" t="s">
         <v>241</v>
       </c>
-      <c r="F40" s="4" t="s">
-        <v>396</v>
+      <c r="F40" s="3" t="s">
+        <v>395</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.35">
@@ -2546,7 +2539,7 @@
       <c r="E41" t="s">
         <v>242</v>
       </c>
-      <c r="F41" s="4" t="s">
+      <c r="F41" s="3" t="s">
         <v>336</v>
       </c>
     </row>
@@ -2563,11 +2556,11 @@
       <c r="E42" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="F42" s="5" t="s">
-        <v>397</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>350</v>
+      <c r="F42" s="4" t="s">
+        <v>396</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
@@ -2583,8 +2576,8 @@
       <c r="E43" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="F43" s="5" t="s">
-        <v>398</v>
+      <c r="F43" s="4" t="s">
+        <v>397</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
@@ -2600,8 +2593,8 @@
       <c r="E44" t="s">
         <v>245</v>
       </c>
-      <c r="G44" s="4" t="s">
-        <v>351</v>
+      <c r="G44" s="3" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.35">
@@ -2617,8 +2610,8 @@
       <c r="E45" s="1">
         <v>-1840</v>
       </c>
-      <c r="F45" s="5" t="s">
-        <v>399</v>
+      <c r="F45" s="4" t="s">
+        <v>398</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.35">
@@ -2648,8 +2641,8 @@
       <c r="E47" s="1" t="s">
         <v>246</v>
       </c>
-      <c r="F47" s="5" t="s">
-        <v>400</v>
+      <c r="F47" s="4" t="s">
+        <v>399</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.35">
@@ -2663,10 +2656,10 @@
         <v>201</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>352</v>
-      </c>
-      <c r="F48" s="5" t="s">
-        <v>401</v>
+        <v>351</v>
+      </c>
+      <c r="F48" s="4" t="s">
+        <v>400</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.35">
@@ -2690,8 +2683,8 @@
       <c r="C50" t="s">
         <v>201</v>
       </c>
-      <c r="G50" s="4" t="s">
-        <v>353</v>
+      <c r="G50" s="3" t="s">
+        <v>352</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
@@ -2707,11 +2700,11 @@
       <c r="E51" t="s">
         <v>247</v>
       </c>
-      <c r="F51" s="4" t="s">
-        <v>402</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>354</v>
+      <c r="F51" s="3" t="s">
+        <v>401</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.35">
@@ -2727,11 +2720,11 @@
       <c r="E52" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="F52" s="5" t="s">
-        <v>403</v>
-      </c>
-      <c r="G52" s="4" t="s">
-        <v>355</v>
+      <c r="F52" s="4" t="s">
+        <v>402</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>354</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.35">
@@ -2747,11 +2740,11 @@
       <c r="E53" s="1" t="s">
         <v>249</v>
       </c>
-      <c r="F53" s="5" t="s">
-        <v>404</v>
-      </c>
-      <c r="G53" s="4" t="s">
-        <v>356</v>
+      <c r="F53" s="4" t="s">
+        <v>403</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>355</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.35">
@@ -2767,9 +2760,9 @@
       <c r="E54" s="1" t="s">
         <v>250</v>
       </c>
-      <c r="F54" s="5"/>
-      <c r="G54" s="4" t="s">
-        <v>357</v>
+      <c r="F54" s="4"/>
+      <c r="G54" s="3" t="s">
+        <v>356</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.35">
@@ -2785,8 +2778,8 @@
       <c r="E55" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="F55" s="4" t="s">
-        <v>358</v>
+      <c r="F55" s="3" t="s">
+        <v>357</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.35">
@@ -2802,11 +2795,11 @@
       <c r="E56" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="F56" s="5" t="s">
-        <v>405</v>
-      </c>
-      <c r="G56" s="4" t="s">
-        <v>359</v>
+      <c r="F56" s="4" t="s">
+        <v>404</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>358</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.35">
@@ -2819,7 +2812,7 @@
       <c r="C57" t="s">
         <v>201</v>
       </c>
-      <c r="F57" s="4" t="s">
+      <c r="F57" s="3" t="s">
         <v>333</v>
       </c>
     </row>
@@ -2836,7 +2829,7 @@
       <c r="E58" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="F58" s="5"/>
+      <c r="F58" s="4"/>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A59" t="s">
@@ -2848,11 +2841,11 @@
       <c r="C59" t="s">
         <v>201</v>
       </c>
-      <c r="F59" s="4" t="s">
-        <v>407</v>
-      </c>
-      <c r="G59" s="4" t="s">
+      <c r="F59" s="3" t="s">
         <v>406</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>405</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.35">
@@ -2865,11 +2858,11 @@
       <c r="C60" t="s">
         <v>201</v>
       </c>
-      <c r="F60" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="G60" s="4" t="s">
-        <v>360</v>
+      <c r="F60" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>359</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.35">
@@ -2888,8 +2881,8 @@
       <c r="E61" t="s">
         <v>254</v>
       </c>
-      <c r="G61" s="4" t="s">
-        <v>361</v>
+      <c r="G61" s="3" t="s">
+        <v>360</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.35">
@@ -2905,11 +2898,11 @@
       <c r="E62" t="s">
         <v>255</v>
       </c>
-      <c r="F62" s="4" t="s">
-        <v>411</v>
-      </c>
-      <c r="G62" s="4" t="s">
+      <c r="F62" s="3" t="s">
         <v>410</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>409</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.35">
@@ -2925,11 +2918,11 @@
       <c r="E63">
         <v>-840</v>
       </c>
-      <c r="F63" s="4" t="s">
-        <v>413</v>
-      </c>
-      <c r="G63" s="4" t="s">
+      <c r="F63" s="3" t="s">
         <v>412</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>411</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.35">
@@ -2948,11 +2941,11 @@
       <c r="E64" t="s">
         <v>256</v>
       </c>
-      <c r="F64" s="4" t="s">
-        <v>414</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>363</v>
+      <c r="F64" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>362</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.35">
@@ -2968,8 +2961,8 @@
       <c r="D65" t="s">
         <v>319</v>
       </c>
-      <c r="G65" s="4" t="s">
-        <v>364</v>
+      <c r="G65" s="3" t="s">
+        <v>363</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.35">
@@ -2982,8 +2975,8 @@
       <c r="C66" t="s">
         <v>201</v>
       </c>
-      <c r="F66" s="4" t="s">
-        <v>365</v>
+      <c r="F66" s="3" t="s">
+        <v>364</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.35">
@@ -2999,11 +2992,11 @@
       <c r="E67" t="s">
         <v>257</v>
       </c>
-      <c r="F67" s="4" t="s">
-        <v>415</v>
-      </c>
-      <c r="G67" s="4" t="s">
-        <v>366</v>
+      <c r="F67" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>365</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.35">
@@ -3019,11 +3012,11 @@
       <c r="E68">
         <v>-840</v>
       </c>
-      <c r="F68" s="4" t="s">
-        <v>416</v>
-      </c>
-      <c r="G68" s="4" t="s">
-        <v>367</v>
+      <c r="F68" s="3" t="s">
+        <v>415</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>366</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.35">
@@ -3061,11 +3054,11 @@
       <c r="C71" t="s">
         <v>201</v>
       </c>
-      <c r="F71" s="4" t="s">
-        <v>368</v>
-      </c>
-      <c r="G71" s="4" t="s">
-        <v>417</v>
+      <c r="F71" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>416</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.35">
@@ -3081,11 +3074,11 @@
       <c r="E72">
         <v>-610</v>
       </c>
-      <c r="F72" s="4" t="s">
-        <v>418</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>369</v>
+      <c r="F72" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="G72" s="3" t="s">
+        <v>368</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.35">
@@ -3098,8 +3091,8 @@
       <c r="C73" t="s">
         <v>201</v>
       </c>
-      <c r="G73" s="4" t="s">
-        <v>370</v>
+      <c r="G73" s="3" t="s">
+        <v>369</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.35">
@@ -3115,11 +3108,11 @@
       <c r="E74" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="F74" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="G74" s="4" t="s">
+      <c r="F74" s="4" t="s">
         <v>419</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>418</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.35">
@@ -3132,11 +3125,11 @@
       <c r="C75" t="s">
         <v>201</v>
       </c>
-      <c r="F75" s="4" t="s">
-        <v>422</v>
-      </c>
-      <c r="G75" s="4" t="s">
+      <c r="F75" s="3" t="s">
         <v>421</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>420</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.35">
@@ -3166,11 +3159,11 @@
       <c r="E77" t="s">
         <v>260</v>
       </c>
-      <c r="F77" s="4" t="s">
-        <v>424</v>
-      </c>
-      <c r="G77" s="4" t="s">
+      <c r="F77" s="3" t="s">
         <v>423</v>
+      </c>
+      <c r="G77" s="3" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.35">
@@ -3186,11 +3179,11 @@
       <c r="D78" t="s">
         <v>214</v>
       </c>
-      <c r="F78" s="4" t="s">
-        <v>425</v>
-      </c>
-      <c r="G78" s="4" t="s">
-        <v>371</v>
+      <c r="F78" s="3" t="s">
+        <v>424</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>370</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.35">
@@ -3206,8 +3199,8 @@
       <c r="D79" t="s">
         <v>213</v>
       </c>
-      <c r="F79" s="4" t="s">
-        <v>426</v>
+      <c r="F79" s="3" t="s">
+        <v>425</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.35">
@@ -3220,8 +3213,8 @@
       <c r="C80" t="s">
         <v>201</v>
       </c>
-      <c r="F80" s="4" t="s">
-        <v>427</v>
+      <c r="F80" s="3" t="s">
+        <v>426</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.35">
@@ -3237,8 +3230,8 @@
       <c r="D81" t="s">
         <v>215</v>
       </c>
-      <c r="F81" s="4" t="s">
-        <v>428</v>
+      <c r="F81" s="3" t="s">
+        <v>427</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.35">
@@ -3276,8 +3269,8 @@
       <c r="C84" t="s">
         <v>201</v>
       </c>
-      <c r="F84" s="4" t="s">
-        <v>429</v>
+      <c r="F84" s="3" t="s">
+        <v>428</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.35">
@@ -3296,8 +3289,8 @@
       <c r="E85" t="s">
         <v>262</v>
       </c>
-      <c r="F85" s="4" t="s">
-        <v>430</v>
+      <c r="F85" s="3" t="s">
+        <v>429</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.35">
@@ -3313,8 +3306,8 @@
       <c r="E86" t="s">
         <v>263</v>
       </c>
-      <c r="F86" s="4" t="s">
-        <v>431</v>
+      <c r="F86" s="3" t="s">
+        <v>430</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
@@ -3330,7 +3323,7 @@
       <c r="E87" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="F87" s="5"/>
+      <c r="F87" s="4"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
@@ -3342,8 +3335,8 @@
       <c r="C88" t="s">
         <v>201</v>
       </c>
-      <c r="F88" s="4" t="s">
-        <v>432</v>
+      <c r="F88" s="3" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.35">
@@ -3359,8 +3352,8 @@
       <c r="E89">
         <v>-750</v>
       </c>
-      <c r="F89" s="4" t="s">
-        <v>433</v>
+      <c r="F89" s="3" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.35">
@@ -3376,8 +3369,8 @@
       <c r="E90" s="1" t="s">
         <v>265</v>
       </c>
-      <c r="F90" s="5" t="s">
-        <v>354</v>
+      <c r="F90" s="4" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
@@ -3401,8 +3394,8 @@
       <c r="C92" t="s">
         <v>201</v>
       </c>
-      <c r="F92" s="4" t="s">
-        <v>434</v>
+      <c r="F92" s="3" t="s">
+        <v>433</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.35">
@@ -3418,8 +3411,8 @@
       <c r="E93" t="s">
         <v>266</v>
       </c>
-      <c r="F93" s="4" t="s">
-        <v>435</v>
+      <c r="F93" s="3" t="s">
+        <v>434</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
@@ -3435,8 +3428,8 @@
       <c r="D94" t="s">
         <v>216</v>
       </c>
-      <c r="F94" s="4" t="s">
-        <v>436</v>
+      <c r="F94" s="3" t="s">
+        <v>435</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
@@ -3449,8 +3442,8 @@
       <c r="C95" t="s">
         <v>201</v>
       </c>
-      <c r="F95" s="4" t="s">
-        <v>437</v>
+      <c r="F95" s="3" t="s">
+        <v>436</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.35">
@@ -3464,7 +3457,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A97" t="s">
         <v>94</v>
       </c>
@@ -3474,11 +3467,11 @@
       <c r="C97" t="s">
         <v>201</v>
       </c>
-      <c r="F97" s="4" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F97" s="3" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
         <v>95</v>
       </c>
@@ -3491,11 +3484,11 @@
       <c r="E98" t="s">
         <v>267</v>
       </c>
-      <c r="F98" s="4" t="s">
-        <v>439</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F98" s="3" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A99" t="s">
         <v>96</v>
       </c>
@@ -3512,7 +3505,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A100" t="s">
         <v>97</v>
       </c>
@@ -3522,11 +3515,11 @@
       <c r="C100" t="s">
         <v>201</v>
       </c>
-      <c r="F100" s="4" t="s">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F100" s="3" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
         <v>98</v>
       </c>
@@ -3536,11 +3529,11 @@
       <c r="C101" t="s">
         <v>201</v>
       </c>
-      <c r="F101" s="4" t="s">
-        <v>441</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F101" s="3" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A102" t="s">
         <v>99</v>
       </c>
@@ -3554,7 +3547,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A103" t="s">
         <v>100</v>
       </c>
@@ -3570,11 +3563,11 @@
       <c r="E103" t="s">
         <v>269</v>
       </c>
-      <c r="F103" s="4" t="s">
-        <v>442</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F103" s="3" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
         <v>101</v>
       </c>
@@ -3584,22 +3577,24 @@
       <c r="C104" t="s">
         <v>201</v>
       </c>
-      <c r="F104" s="4" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A105" t="s">
+      <c r="F104" s="3" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A105" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="B105" t="s">
-        <v>193</v>
-      </c>
-      <c r="C105" t="s">
+      <c r="B105" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C105" s="2" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F105" s="5"/>
+      <c r="G105" s="5"/>
+    </row>
+    <row r="106" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A106" t="s">
         <v>103</v>
       </c>
@@ -3609,11 +3604,11 @@
       <c r="C106" t="s">
         <v>201</v>
       </c>
-      <c r="F106" s="4" t="s">
-        <v>444</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F106" s="3" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A107" t="s">
         <v>104</v>
       </c>
@@ -3626,11 +3621,11 @@
       <c r="E107" t="s">
         <v>270</v>
       </c>
-      <c r="F107" s="4" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F107" s="3" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
         <v>105</v>
       </c>
@@ -3643,11 +3638,11 @@
       <c r="E108" t="s">
         <v>271</v>
       </c>
-      <c r="F108" s="4" t="s">
-        <v>446</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F108" s="3" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A109" t="s">
         <v>106</v>
       </c>
@@ -3660,11 +3655,11 @@
       <c r="E109" t="s">
         <v>272</v>
       </c>
-      <c r="F109" s="4" t="s">
-        <v>447</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F109" s="3" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
         <v>107</v>
       </c>
@@ -3677,11 +3672,11 @@
       <c r="E110" t="s">
         <v>273</v>
       </c>
-      <c r="F110" s="4" t="s">
-        <v>448</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F110" s="3" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A111" t="s">
         <v>108</v>
       </c>
@@ -3695,7 +3690,7 @@
         <v>274</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A112" t="s">
         <v>109</v>
       </c>
@@ -3705,8 +3700,8 @@
       <c r="C112" t="s">
         <v>201</v>
       </c>
-      <c r="F112" s="4" t="s">
-        <v>449</v>
+      <c r="F112" s="3" t="s">
+        <v>448</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.35">
@@ -3722,8 +3717,8 @@
       <c r="E113" t="s">
         <v>275</v>
       </c>
-      <c r="F113" s="4" t="s">
-        <v>450</v>
+      <c r="F113" s="3" t="s">
+        <v>449</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.35">
@@ -3739,8 +3734,8 @@
       <c r="E114" t="s">
         <v>276</v>
       </c>
-      <c r="F114" s="4" t="s">
-        <v>451</v>
+      <c r="F114" s="3" t="s">
+        <v>450</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.35">
@@ -3756,8 +3751,8 @@
       <c r="E115" t="s">
         <v>277</v>
       </c>
-      <c r="F115" s="4" t="s">
-        <v>362</v>
+      <c r="F115" s="3" t="s">
+        <v>361</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.35">
@@ -3773,8 +3768,8 @@
       <c r="D116" t="s">
         <v>222</v>
       </c>
-      <c r="F116" s="4" t="s">
-        <v>452</v>
+      <c r="F116" s="3" t="s">
+        <v>451</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.35">
@@ -3790,8 +3785,8 @@
       <c r="D117" t="s">
         <v>209</v>
       </c>
-      <c r="F117" s="4" t="s">
-        <v>453</v>
+      <c r="F117" s="3" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.35">
@@ -3810,8 +3805,8 @@
       <c r="E118" t="s">
         <v>278</v>
       </c>
-      <c r="F118" s="4" t="s">
-        <v>454</v>
+      <c r="F118" s="3" t="s">
+        <v>453</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.35">
@@ -3827,8 +3822,8 @@
       <c r="E119" t="s">
         <v>279</v>
       </c>
-      <c r="F119" s="4" t="s">
-        <v>409</v>
+      <c r="F119" s="3" t="s">
+        <v>408</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.35">
@@ -3841,8 +3836,8 @@
       <c r="C120" t="s">
         <v>201</v>
       </c>
-      <c r="F120" s="4" t="s">
-        <v>455</v>
+      <c r="F120" s="3" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.35">
@@ -3858,8 +3853,8 @@
       <c r="E121" t="s">
         <v>280</v>
       </c>
-      <c r="F121" s="4" t="s">
-        <v>456</v>
+      <c r="F121" s="3" t="s">
+        <v>455</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.35">
@@ -3872,8 +3867,8 @@
       <c r="C122" t="s">
         <v>201</v>
       </c>
-      <c r="F122" s="4" t="s">
-        <v>457</v>
+      <c r="F122" s="3" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.35">
@@ -3886,8 +3881,8 @@
       <c r="C123" t="s">
         <v>201</v>
       </c>
-      <c r="F123" s="4" t="s">
-        <v>458</v>
+      <c r="F123" s="3" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.35">
@@ -3900,8 +3895,8 @@
       <c r="C124" t="s">
         <v>201</v>
       </c>
-      <c r="F124" s="4" t="s">
-        <v>459</v>
+      <c r="F124" s="3" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.35">
@@ -3914,8 +3909,8 @@
       <c r="C125" t="s">
         <v>201</v>
       </c>
-      <c r="F125" s="4" t="s">
-        <v>460</v>
+      <c r="F125" s="3" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.35">
@@ -3931,8 +3926,8 @@
       <c r="E126" t="s">
         <v>281</v>
       </c>
-      <c r="F126" s="4" t="s">
-        <v>461</v>
+      <c r="F126" s="3" t="s">
+        <v>460</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.35">
@@ -3945,7 +3940,7 @@
       <c r="C127" t="s">
         <v>201</v>
       </c>
-      <c r="F127" s="4" t="s">
+      <c r="F127" s="3" t="s">
         <v>290</v>
       </c>
     </row>
@@ -3959,11 +3954,11 @@
       <c r="C128" t="s">
         <v>201</v>
       </c>
-      <c r="F128" s="4" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F128" s="3" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A129" t="s">
         <v>126</v>
       </c>
@@ -3973,22 +3968,24 @@
       <c r="C129" t="s">
         <v>201</v>
       </c>
-      <c r="F129" s="4" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A130" t="s">
+      <c r="F129" s="3" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A130" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B130" t="s">
-        <v>193</v>
-      </c>
-      <c r="C130" t="s">
+      <c r="B130" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C130" s="2" t="s">
         <v>200</v>
       </c>
-    </row>
-    <row r="131" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F130" s="5"/>
+      <c r="G130" s="5"/>
+    </row>
+    <row r="131" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
         <v>128</v>
       </c>
@@ -4001,11 +3998,11 @@
       <c r="E131" t="s">
         <v>282</v>
       </c>
-      <c r="F131" s="4" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F131" s="3" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A132" t="s">
         <v>129</v>
       </c>
@@ -4018,11 +4015,11 @@
       <c r="E132" t="s">
         <v>283</v>
       </c>
-      <c r="F132" s="4" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F132" s="3" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A133" t="s">
         <v>130</v>
       </c>
@@ -4035,11 +4032,11 @@
       <c r="E133">
         <v>-590</v>
       </c>
-      <c r="F133" s="4" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F133" s="3" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
         <v>131</v>
       </c>
@@ -4052,11 +4049,11 @@
       <c r="E134" t="s">
         <v>284</v>
       </c>
-      <c r="F134" s="4" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F134" s="3" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
         <v>132</v>
       </c>
@@ -4066,11 +4063,11 @@
       <c r="C135" t="s">
         <v>201</v>
       </c>
-      <c r="F135" s="4" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F135" s="3" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A136" t="s">
         <v>133</v>
       </c>
@@ -4083,11 +4080,11 @@
       <c r="E136" t="s">
         <v>285</v>
       </c>
-      <c r="F136" s="4" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F136" s="3" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
         <v>134</v>
       </c>
@@ -4100,11 +4097,11 @@
       <c r="E137" t="s">
         <v>286</v>
       </c>
-      <c r="F137" s="4" t="s">
-        <v>468</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F137" s="3" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
         <v>135</v>
       </c>
@@ -4115,7 +4112,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="139" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
         <v>136</v>
       </c>
@@ -4128,11 +4125,11 @@
       <c r="E139" t="s">
         <v>287</v>
       </c>
-      <c r="F139" s="4" t="s">
-        <v>469</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F139" s="3" t="s">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A140" t="s">
         <v>137</v>
       </c>
@@ -4146,7 +4143,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="141" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
         <v>138</v>
       </c>
@@ -4156,11 +4153,11 @@
       <c r="C141" t="s">
         <v>201</v>
       </c>
-      <c r="F141" s="4" t="s">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F141" s="3" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A142" t="s">
         <v>139</v>
       </c>
@@ -4170,11 +4167,11 @@
       <c r="C142" t="s">
         <v>201</v>
       </c>
-      <c r="F142" s="4" t="s">
-        <v>454</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F142" s="3" t="s">
+        <v>453</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A143" t="s">
         <v>140</v>
       </c>
@@ -4188,7 +4185,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="144" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
         <v>141</v>
       </c>
@@ -4408,7 +4405,7 @@
         <v>-440</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A161" t="s">
         <v>158</v>
       </c>
@@ -4425,7 +4422,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A162" t="s">
         <v>159</v>
       </c>
@@ -4436,7 +4433,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
         <v>160</v>
       </c>
@@ -4447,21 +4444,23 @@
         <v>201</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A164" t="s">
+    <row r="164" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A164" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="B164" t="s">
-        <v>195</v>
-      </c>
-      <c r="C164" t="s">
-        <v>201</v>
-      </c>
-      <c r="D164" t="s">
+      <c r="B164" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="C164" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D164" s="2" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F164" s="5"/>
+      <c r="G164" s="5"/>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A165" t="s">
         <v>162</v>
       </c>
@@ -4472,7 +4471,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="166" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
         <v>163</v>
       </c>
@@ -4486,7 +4485,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
         <v>164</v>
       </c>
@@ -4500,7 +4499,7 @@
         <v>296</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
         <v>165</v>
       </c>
@@ -4514,7 +4513,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A169" t="s">
         <v>166</v>
       </c>
@@ -4525,7 +4524,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A170" t="s">
         <v>167</v>
       </c>
@@ -4539,7 +4538,7 @@
         <v>227</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
         <v>168</v>
       </c>
@@ -4553,7 +4552,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="172" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
         <v>169</v>
       </c>
@@ -4567,7 +4566,7 @@
         <v>-1100</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
         <v>170</v>
       </c>
@@ -4578,7 +4577,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
         <v>171</v>
       </c>
@@ -4592,7 +4591,7 @@
         <v>298</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
         <v>172</v>
       </c>
@@ -4606,7 +4605,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
         <v>173</v>
       </c>
@@ -4809,9 +4808,9 @@
       <c r="E190" s="2" t="s">
         <v>306</v>
       </c>
-      <c r="F190" s="6"/>
-      <c r="G190" s="6" t="s">
-        <v>341</v>
+      <c r="F190" s="5"/>
+      <c r="G190" s="5" t="s">
+        <v>340</v>
       </c>
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
MAking sure up to date.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{463933D8-C90B-4A71-BE91-2ACEE1E90667}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218AA265-7629-4C88-9D8E-F36586C3983D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3680" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -1801,8 +1801,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
   <dimension ref="A1:G193"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A144" sqref="A144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Ending 2017-2018 ablation exclusions definition.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{218AA265-7629-4C88-9D8E-F36586C3983D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAF99A83-7147-4963-993B-D5F30B458657}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3680" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="470">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="894" uniqueCount="500">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -1435,6 +1435,96 @@
   </si>
   <si>
     <t>-600</t>
+  </si>
+  <si>
+    <t>-1080</t>
+  </si>
+  <si>
+    <t>7050-</t>
+  </si>
+  <si>
+    <t>-420</t>
+  </si>
+  <si>
+    <t>5300-</t>
+  </si>
+  <si>
+    <t>7560-</t>
+  </si>
+  <si>
+    <t>-430</t>
+  </si>
+  <si>
+    <t>3030-</t>
+  </si>
+  <si>
+    <t>4200-4600 4900-5040 17430-</t>
+  </si>
+  <si>
+    <t>-100 2545-</t>
+  </si>
+  <si>
+    <t>-1600</t>
+  </si>
+  <si>
+    <t>2850-</t>
+  </si>
+  <si>
+    <t>-740</t>
+  </si>
+  <si>
+    <t>8900-10600 15915-</t>
+  </si>
+  <si>
+    <t>6380-</t>
+  </si>
+  <si>
+    <t>to delete because shit</t>
+  </si>
+  <si>
+    <t>3090-</t>
+  </si>
+  <si>
+    <t>-2300</t>
+  </si>
+  <si>
+    <t>4700-</t>
+  </si>
+  <si>
+    <t>5000-</t>
+  </si>
+  <si>
+    <t>1220-1400 2370-</t>
+  </si>
+  <si>
+    <t>-390</t>
+  </si>
+  <si>
+    <t>-1350</t>
+  </si>
+  <si>
+    <t>6800-</t>
+  </si>
+  <si>
+    <t>-900 3515-3600</t>
+  </si>
+  <si>
+    <t>4320-</t>
+  </si>
+  <si>
+    <t>8100-</t>
+  </si>
+  <si>
+    <t>-3870 4275-6745 8850-9480 10390-11750</t>
+  </si>
+  <si>
+    <t>5700-</t>
+  </si>
+  <si>
+    <t>-1335</t>
+  </si>
+  <si>
+    <t>2960-</t>
   </si>
 </sst>
 </file>
@@ -1450,7 +1540,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1460,6 +1550,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1476,7 +1572,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1485,6 +1581,8 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1801,8 +1899,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
   <dimension ref="A1:G193"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A139" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A144" sqref="A144"/>
+    <sheetView tabSelected="1" topLeftCell="A172" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F193" sqref="F193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4184,6 +4282,9 @@
       <c r="D143" t="s">
         <v>218</v>
       </c>
+      <c r="F143" s="3" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A144" t="s">
@@ -4199,7 +4300,7 @@
         <v>-1600</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>142</v>
       </c>
@@ -4215,8 +4316,11 @@
       <c r="E145" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F145" s="3" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>143</v>
       </c>
@@ -4226,8 +4330,11 @@
       <c r="C146" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F146" s="3" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>144</v>
       </c>
@@ -4237,8 +4344,11 @@
       <c r="C147" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F147" s="3" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>145</v>
       </c>
@@ -4252,7 +4362,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>146</v>
       </c>
@@ -4266,7 +4376,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>147</v>
       </c>
@@ -4277,7 +4387,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>148</v>
       </c>
@@ -4287,8 +4397,11 @@
       <c r="C151" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F151" s="3" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>149</v>
       </c>
@@ -4301,8 +4414,11 @@
       <c r="D152" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F152" s="3" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>150</v>
       </c>
@@ -4316,7 +4432,7 @@
         <v>292</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>151</v>
       </c>
@@ -4330,7 +4446,7 @@
         <v>-70</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>152</v>
       </c>
@@ -4341,7 +4457,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>153</v>
       </c>
@@ -4351,8 +4467,11 @@
       <c r="C156" t="s">
         <v>201</v>
       </c>
-    </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F156" s="3" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>154</v>
       </c>
@@ -4363,7 +4482,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>155</v>
       </c>
@@ -4376,8 +4495,11 @@
       <c r="E158" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F158" s="3" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>156</v>
       </c>
@@ -4390,8 +4512,11 @@
       <c r="E159" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F159" s="3" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>157</v>
       </c>
@@ -4403,6 +4528,9 @@
       </c>
       <c r="E160">
         <v>-440</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>479</v>
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.35">
@@ -4432,6 +4560,9 @@
       <c r="C162" t="s">
         <v>201</v>
       </c>
+      <c r="F162" s="3" t="s">
+        <v>480</v>
+      </c>
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
@@ -4443,6 +4574,9 @@
       <c r="C163" t="s">
         <v>201</v>
       </c>
+      <c r="F163" s="3" t="s">
+        <v>481</v>
+      </c>
     </row>
     <row r="164" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A164" s="2" t="s">
@@ -4470,6 +4604,9 @@
       <c r="C165" t="s">
         <v>201</v>
       </c>
+      <c r="F165" s="3" t="s">
+        <v>482</v>
+      </c>
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
@@ -4484,6 +4621,9 @@
       <c r="D166" t="s">
         <v>219</v>
       </c>
+      <c r="F166" s="3" t="s">
+        <v>407</v>
+      </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A167" t="s">
@@ -4498,6 +4638,9 @@
       <c r="E167" t="s">
         <v>296</v>
       </c>
+      <c r="F167" s="3" t="s">
+        <v>483</v>
+      </c>
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A168" t="s">
@@ -4524,19 +4667,23 @@
         <v>201</v>
       </c>
     </row>
-    <row r="170" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A170" t="s">
+    <row r="170" spans="1:7" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A170" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="B170" t="s">
+      <c r="B170" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="C170" t="s">
-        <v>201</v>
-      </c>
-      <c r="D170" t="s">
+      <c r="C170" s="8" t="s">
+        <v>201</v>
+      </c>
+      <c r="D170" s="8" t="s">
         <v>227</v>
       </c>
+      <c r="F170" s="9" t="s">
+        <v>484</v>
+      </c>
+      <c r="G170" s="9"/>
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
@@ -4551,6 +4698,9 @@
       <c r="E171" t="s">
         <v>297</v>
       </c>
+      <c r="F171" s="3" t="s">
+        <v>485</v>
+      </c>
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A172" t="s">
@@ -4565,6 +4715,9 @@
       <c r="E172">
         <v>-1100</v>
       </c>
+      <c r="F172" s="3" t="s">
+        <v>486</v>
+      </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
@@ -4604,6 +4757,9 @@
       <c r="D175" t="s">
         <v>229</v>
       </c>
+      <c r="F175" s="3" t="s">
+        <v>487</v>
+      </c>
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A176" t="s">
@@ -4615,6 +4771,9 @@
       <c r="C176" t="s">
         <v>201</v>
       </c>
+      <c r="F176" s="3" t="s">
+        <v>380</v>
+      </c>
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A177" t="s">
@@ -4632,6 +4791,9 @@
       <c r="E177" t="s">
         <v>299</v>
       </c>
+      <c r="F177" s="3" t="s">
+        <v>488</v>
+      </c>
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
@@ -4643,6 +4805,9 @@
       <c r="C178" t="s">
         <v>201</v>
       </c>
+      <c r="F178" s="3" t="s">
+        <v>427</v>
+      </c>
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
@@ -4657,6 +4822,9 @@
       <c r="E179" t="s">
         <v>300</v>
       </c>
+      <c r="F179" s="3" t="s">
+        <v>489</v>
+      </c>
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A180" t="s">
@@ -4671,6 +4839,9 @@
       <c r="D180" t="s">
         <v>218</v>
       </c>
+      <c r="F180" s="3" t="s">
+        <v>490</v>
+      </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
@@ -4699,6 +4870,9 @@
       <c r="E182" t="s">
         <v>303</v>
       </c>
+      <c r="F182" s="3" t="s">
+        <v>491</v>
+      </c>
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
@@ -4724,6 +4898,9 @@
       <c r="C184" t="s">
         <v>201</v>
       </c>
+      <c r="F184" s="3" t="s">
+        <v>492</v>
+      </c>
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A185" t="s">
@@ -4749,6 +4926,9 @@
       <c r="D186" t="s">
         <v>228</v>
       </c>
+      <c r="F186" s="3" t="s">
+        <v>493</v>
+      </c>
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
@@ -4760,6 +4940,9 @@
       <c r="C187" t="s">
         <v>201</v>
       </c>
+      <c r="F187" s="3" t="s">
+        <v>494</v>
+      </c>
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
@@ -4774,6 +4957,9 @@
       <c r="E188" t="s">
         <v>304</v>
       </c>
+      <c r="F188" s="3" t="s">
+        <v>495</v>
+      </c>
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
@@ -4791,6 +4977,9 @@
       <c r="E189" t="s">
         <v>305</v>
       </c>
+      <c r="F189" s="3" t="s">
+        <v>496</v>
+      </c>
     </row>
     <row r="190" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A190" s="2" t="s">
@@ -4826,6 +5015,9 @@
       <c r="E191" t="s">
         <v>307</v>
       </c>
+      <c r="F191" s="3" t="s">
+        <v>497</v>
+      </c>
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
@@ -4840,8 +5032,11 @@
       <c r="E192" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F192" s="3" t="s">
+        <v>498</v>
+      </c>
+    </row>
+    <row r="193" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>190</v>
       </c>
@@ -4853,6 +5048,9 @@
       </c>
       <c r="E193" t="s">
         <v>309</v>
+      </c>
+      <c r="F193" s="3" t="s">
+        <v>499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correct the typo introduced in previous commit about 20170410_01_132_133.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9D36C9D-E2EF-45CD-8144-CC847D9D8C68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8245C594-0D13-4420-AAAA-EBBEF64B4811}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3680" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2670" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="537">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -1539,9 +1539,6 @@
     <t>20170331_01_033_038</t>
   </si>
   <si>
-    <t>20170410_01_130_133</t>
-  </si>
-  <si>
     <t>20170412_01_035_055</t>
   </si>
   <si>
@@ -1636,6 +1633,9 @@
   </si>
   <si>
     <t>Exclusions_1st_run</t>
+  </si>
+  <si>
+    <t>20170410_01_132_133</t>
   </si>
 </sst>
 </file>
@@ -2002,8 +2002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
   <dimension ref="A1:H194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A161" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E176" sqref="E176"/>
+    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F62" sqref="F62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2050,22 +2050,22 @@
         <v>192</v>
       </c>
       <c r="C2" t="s">
+        <v>531</v>
+      </c>
+      <c r="D2" t="s">
         <v>532</v>
-      </c>
-      <c r="D2" t="s">
-        <v>533</v>
       </c>
       <c r="E2" t="s">
         <v>497</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>534</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>535</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>536</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -2153,7 +2153,7 @@
         <v>194</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -2167,7 +2167,7 @@
         <v>194</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>306</v>
@@ -2183,7 +2183,7 @@
         <v>194</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -2254,7 +2254,7 @@
         <v>194</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -2317,7 +2317,7 @@
         <v>194</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -2391,7 +2391,7 @@
         <v>194</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F20" s="5">
         <v>-640</v>
@@ -2570,7 +2570,7 @@
         <v>193</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>206</v>
@@ -3253,7 +3253,7 @@
         <v>211</v>
       </c>
       <c r="E62" t="s">
-        <v>504</v>
+        <v>536</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>245</v>
@@ -3322,7 +3322,7 @@
         <v>304</v>
       </c>
       <c r="E65" t="s">
-        <v>505</v>
+        <v>504</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>247</v>
@@ -3348,7 +3348,7 @@
         <v>307</v>
       </c>
       <c r="E66" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="H66" s="3" t="s">
         <v>343</v>
@@ -3579,7 +3579,7 @@
         <v>212</v>
       </c>
       <c r="E78" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>250</v>
@@ -3605,7 +3605,7 @@
         <v>214</v>
       </c>
       <c r="E79" t="s">
-        <v>508</v>
+        <v>507</v>
       </c>
       <c r="G79" s="3" t="s">
         <v>404</v>
@@ -3628,7 +3628,7 @@
         <v>213</v>
       </c>
       <c r="E80" t="s">
-        <v>509</v>
+        <v>508</v>
       </c>
       <c r="G80" s="3" t="s">
         <v>405</v>
@@ -3665,7 +3665,7 @@
         <v>215</v>
       </c>
       <c r="E82" t="s">
-        <v>510</v>
+        <v>509</v>
       </c>
       <c r="G82" s="3" t="s">
         <v>407</v>
@@ -3733,7 +3733,7 @@
         <v>210</v>
       </c>
       <c r="E86" t="s">
-        <v>511</v>
+        <v>510</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>252</v>
@@ -3902,7 +3902,7 @@
         <v>216</v>
       </c>
       <c r="E95" t="s">
-        <v>512</v>
+        <v>511</v>
       </c>
       <c r="G95" s="3" t="s">
         <v>415</v>
@@ -3990,7 +3990,7 @@
         <v>217</v>
       </c>
       <c r="E100" t="s">
-        <v>513</v>
+        <v>512</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>256</v>
@@ -4044,7 +4044,7 @@
         <v>220</v>
       </c>
       <c r="E103" t="s">
-        <v>514</v>
+        <v>513</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.35">
@@ -4061,7 +4061,7 @@
         <v>221</v>
       </c>
       <c r="E104" t="s">
-        <v>515</v>
+        <v>514</v>
       </c>
       <c r="F104" s="3" t="s">
         <v>257</v>
@@ -4306,7 +4306,7 @@
         <v>222</v>
       </c>
       <c r="E117" t="s">
-        <v>516</v>
+        <v>515</v>
       </c>
       <c r="G117" s="3" t="s">
         <v>431</v>
@@ -4326,7 +4326,7 @@
         <v>209</v>
       </c>
       <c r="E118" t="s">
-        <v>517</v>
+        <v>516</v>
       </c>
       <c r="G118" s="3" t="s">
         <v>432</v>
@@ -4346,7 +4346,7 @@
         <v>223</v>
       </c>
       <c r="E119" t="s">
-        <v>518</v>
+        <v>517</v>
       </c>
       <c r="F119" s="3" t="s">
         <v>266</v>
@@ -4801,7 +4801,7 @@
         <v>218</v>
       </c>
       <c r="E144" t="s">
-        <v>519</v>
+        <v>518</v>
       </c>
       <c r="G144" s="3" t="s">
         <v>450</v>
@@ -4838,7 +4838,7 @@
         <v>219</v>
       </c>
       <c r="E146" t="s">
-        <v>520</v>
+        <v>519</v>
       </c>
       <c r="F146" s="3" t="s">
         <v>277</v>
@@ -4960,7 +4960,7 @@
         <v>210</v>
       </c>
       <c r="E153" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="G153" s="3" t="s">
         <v>455</v>
@@ -5119,7 +5119,7 @@
         <v>224</v>
       </c>
       <c r="E162" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="F162" s="3" t="s">
         <v>283</v>
@@ -5207,7 +5207,7 @@
         <v>219</v>
       </c>
       <c r="E167" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="G167" s="3" t="s">
         <v>387</v>
@@ -5247,7 +5247,7 @@
         <v>226</v>
       </c>
       <c r="E169" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.35">
@@ -5272,7 +5272,7 @@
         <v>195</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>227</v>
@@ -5366,7 +5366,7 @@
         <v>229</v>
       </c>
       <c r="E176" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
       <c r="G176" s="3" t="s">
         <v>466</v>
@@ -5403,7 +5403,7 @@
         <v>230</v>
       </c>
       <c r="E178" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
       <c r="F178" s="3" t="s">
         <v>287</v>
@@ -5463,7 +5463,7 @@
         <v>218</v>
       </c>
       <c r="E181" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="G181" s="3" t="s">
         <v>469</v>
@@ -5568,7 +5568,7 @@
         <v>228</v>
       </c>
       <c r="E187" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
       <c r="G187" s="3" t="s">
         <v>473</v>
@@ -5625,7 +5625,7 @@
         <v>208</v>
       </c>
       <c r="E190" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
       <c r="F190" s="3" t="s">
         <v>293</v>
@@ -5642,7 +5642,7 @@
         <v>195</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>231</v>

</xml_diff>

<commit_message>
Identification of fail of roll correction in 2017. 2017 to be continued and 2018 to be done.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8245C594-0D13-4420-AAAA-EBBEF64B4811}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523ADF36-6544-44CF-8047-9DEBB1D3A37D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3680" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1073" uniqueCount="537">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="540">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -954,15 +954,6 @@
     <t>Exclusions after 1st run</t>
   </si>
   <si>
-    <t>9180-10400</t>
-  </si>
-  <si>
-    <t>-5810 5825-5925 6060-</t>
-  </si>
-  <si>
-    <t>-1620 1790</t>
-  </si>
-  <si>
     <t>-360 500-650 910-1060 1260-</t>
   </si>
   <si>
@@ -972,69 +963,33 @@
     <t>-500</t>
   </si>
   <si>
-    <t>-2740 2900-3055 6780-7220 9680-9860 10470-10560 19910-19990 27330-</t>
-  </si>
-  <si>
-    <t>2240-3560 10260-</t>
-  </si>
-  <si>
     <t>2300-</t>
   </si>
   <si>
     <t>-1010</t>
   </si>
   <si>
-    <t>-3920 5100-7120</t>
-  </si>
-  <si>
     <t>-1450 1720-1880 2730-</t>
   </si>
   <si>
-    <t>4510-4950 27360-29020 29740-29910 30890-31460 35100-35700 37170-37420 38660-38900 40440-</t>
-  </si>
-  <si>
     <t>5720-6310 6540-6815</t>
   </si>
   <si>
-    <t>2560-</t>
-  </si>
-  <si>
     <t>-940 5050-5630 5810-6000 6050-6480 8150-8310 8450-11130</t>
   </si>
   <si>
     <t>-550 2060-2280 3200-3310 4260-4400 4780-4900 5280-5460</t>
   </si>
   <si>
-    <t>-170 1050-</t>
-  </si>
-  <si>
-    <t>-1890 2370-</t>
-  </si>
-  <si>
-    <t>6360-</t>
-  </si>
-  <si>
-    <t>1540-2230</t>
-  </si>
-  <si>
     <t>680-1250</t>
   </si>
   <si>
     <t>-1040 6290-</t>
   </si>
   <si>
-    <t>840-890</t>
-  </si>
-  <si>
     <t>-780</t>
   </si>
   <si>
-    <t>1160-1480 3230-3320 3700-3870 4220-4540</t>
-  </si>
-  <si>
-    <t>-1240</t>
-  </si>
-  <si>
     <t>1550-1620 1860-</t>
   </si>
   <si>
@@ -1044,9 +999,6 @@
     <t>-1370</t>
   </si>
   <si>
-    <t>3830-</t>
-  </si>
-  <si>
     <t>-270 2500-</t>
   </si>
   <si>
@@ -1062,21 +1014,12 @@
     <t>2310-</t>
   </si>
   <si>
-    <t>-500 1100-</t>
-  </si>
-  <si>
-    <t>-1420 2330-2540</t>
-  </si>
-  <si>
     <t>-830</t>
   </si>
   <si>
     <t>1010-1120 1690-1770 2160-2420</t>
   </si>
   <si>
-    <t>1350-1530</t>
-  </si>
-  <si>
     <t>-105 225-380 710-790 1310-1760</t>
   </si>
   <si>
@@ -1158,9 +1101,6 @@
     <t>1540-2230 5030-</t>
   </si>
   <si>
-    <t>-880 1490-2080 3460</t>
-  </si>
-  <si>
     <t>2600-</t>
   </si>
   <si>
@@ -1194,15 +1134,9 @@
     <t>-1270</t>
   </si>
   <si>
-    <t>-2600 4100-5800 6370-7250 11360-11820 17130-18480 19980-21440 25430-26250 28560-30485 34710-34810</t>
-  </si>
-  <si>
     <t>26460-27760 30940-32180 35380-</t>
   </si>
   <si>
-    <t>1440-1690 1850-2220 2275-2330 2920-3650 3750-4120 4190-4330 4400-</t>
-  </si>
-  <si>
     <t>-1170 2630-2900 3040-3355 4030-4120</t>
   </si>
   <si>
@@ -1215,9 +1149,6 @@
     <t>-1300</t>
   </si>
   <si>
-    <t>1790-</t>
-  </si>
-  <si>
     <t>-770</t>
   </si>
   <si>
@@ -1233,9 +1164,6 @@
     <t xml:space="preserve">-330 </t>
   </si>
   <si>
-    <t>8800-9770</t>
-  </si>
-  <si>
     <t xml:space="preserve">-1130 </t>
   </si>
   <si>
@@ -1500,24 +1428,9 @@
     <t>-700 1935-2055</t>
   </si>
   <si>
-    <t>-230 470-675 1350-1515 1680-1975 3600-</t>
-  </si>
-  <si>
-    <t>-910 -2115</t>
-  </si>
-  <si>
     <t>-800 910-990 1130-1255 1395-</t>
   </si>
   <si>
-    <t>-2850 4090-</t>
-  </si>
-  <si>
-    <t>-21200 31320-</t>
-  </si>
-  <si>
-    <t>-2480 2630-2690 3345-</t>
-  </si>
-  <si>
     <t>datetrack_tobeprocessed</t>
   </si>
   <si>
@@ -1636,6 +1549,102 @@
   </si>
   <si>
     <t>20170410_01_132_133</t>
+  </si>
+  <si>
+    <t>-100 470-675 1350-1515 1680-1975 3680-</t>
+  </si>
+  <si>
+    <t>2115-</t>
+  </si>
+  <si>
+    <t>-550</t>
+  </si>
+  <si>
+    <t>-9180 9280-9380 9540-9610 10400-</t>
+  </si>
+  <si>
+    <t>-2710 2760-2850 3140-3230 3330-3460 3560-3780 3820-3970 4100-</t>
+  </si>
+  <si>
+    <t>-7150 7230-7350 12440-25260 25390-26450 26600-26690 26830-29370 29570-29690 29880-29980 30090-30180 30350-30450 30530-30580 30820-</t>
+  </si>
+  <si>
+    <t>-2480 2630-2690 3100-3200 3345-</t>
+  </si>
+  <si>
+    <t>-5810 5825-5925 6060-9410 9550-</t>
+  </si>
+  <si>
+    <t>-1620 1790-2130 2320-2420 2530-2730 2770-2860 3060-3150 3200-3620 3770-3840 3980-4080 4230-4330 4440-4590 4730-5490 5610-</t>
+  </si>
+  <si>
+    <t>-2740 2900-3055 6880-7220 7560-7700 9690-9860 10470-10590 23700-23810 27330-</t>
+  </si>
+  <si>
+    <t>2240-3560</t>
+  </si>
+  <si>
+    <t>5100-7120 12460-</t>
+  </si>
+  <si>
+    <t>670-1120 2640-2760 4510-4950 17900-18360 27360-29020 29740-29910 30890-31460 31950-32410 39580-</t>
+  </si>
+  <si>
+    <t>2560- 4530-4610 4660-4770 4850-4890 4980-5200 6100-6230</t>
+  </si>
+  <si>
+    <t>-170</t>
+  </si>
+  <si>
+    <t>4600-4640</t>
+  </si>
+  <si>
+    <t>1190-1240</t>
+  </si>
+  <si>
+    <t>-880 1490-2080 3460-</t>
+  </si>
+  <si>
+    <t>1020-1120</t>
+  </si>
+  <si>
+    <t>5390-5510</t>
+  </si>
+  <si>
+    <t>830-880</t>
+  </si>
+  <si>
+    <t>9320-9390 11180-11260 12100-12200</t>
+  </si>
+  <si>
+    <t>1160-1480 3230-3320 4470-4540 4690-4760</t>
+  </si>
+  <si>
+    <t>1900-1945 1970-2010</t>
+  </si>
+  <si>
+    <t>-1470 3830-</t>
+  </si>
+  <si>
+    <t>-1400 1700-2515  4100-5430 6335-7770 9000-9800 11360-11820 17130-18480 19980-21440 22730-22920 25430-26250 28560-30485 34710-34810</t>
+  </si>
+  <si>
+    <t>1440-1690 1850-2220 2275-2330 2920-2980 3390-3470 3540-3650 3750-3850 3895-3990 4190-4215 4270-4330 4400-</t>
+  </si>
+  <si>
+    <t>2060-2110</t>
+  </si>
+  <si>
+    <t>1370-1420 2330-2540</t>
+  </si>
+  <si>
+    <t>1420-1490 1790-</t>
+  </si>
+  <si>
+    <t>1350-1530 1690-1840</t>
+  </si>
+  <si>
+    <t>9330-9770</t>
   </si>
 </sst>
 </file>
@@ -2002,8 +2011,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
   <dimension ref="A1:H194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F62" sqref="F62"/>
+    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I83" sqref="I83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2030,13 +2039,13 @@
         <v>202</v>
       </c>
       <c r="E1" t="s">
-        <v>497</v>
+        <v>468</v>
       </c>
       <c r="F1" s="3" t="s">
         <v>232</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>308</v>
@@ -2050,22 +2059,22 @@
         <v>192</v>
       </c>
       <c r="C2" t="s">
-        <v>531</v>
+        <v>502</v>
       </c>
       <c r="D2" t="s">
-        <v>532</v>
+        <v>503</v>
       </c>
       <c r="E2" t="s">
-        <v>497</v>
+        <v>468</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>533</v>
+        <v>504</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>534</v>
+        <v>505</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>535</v>
+        <v>506</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -2082,10 +2091,10 @@
         <v>0</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>352</v>
+        <v>333</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>491</v>
+        <v>508</v>
       </c>
     </row>
     <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2116,7 +2125,7 @@
         <v>203</v>
       </c>
       <c r="E5" t="s">
-        <v>498</v>
+        <v>469</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>233</v>
@@ -2125,7 +2134,7 @@
         <v>-910</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>492</v>
+        <v>509</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -2141,8 +2150,8 @@
       <c r="E6" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="3">
-        <v>-620</v>
+      <c r="H6" s="3" t="s">
+        <v>510</v>
       </c>
     </row>
     <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2153,7 +2162,7 @@
         <v>194</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>529</v>
+        <v>500</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -2167,7 +2176,7 @@
         <v>194</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>529</v>
+        <v>500</v>
       </c>
       <c r="F8" s="5" t="s">
         <v>306</v>
@@ -2183,7 +2192,7 @@
         <v>194</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>529</v>
+        <v>500</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -2203,10 +2212,10 @@
         <v>6</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>353</v>
+        <v>334</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>309</v>
+        <v>511</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -2223,7 +2232,7 @@
         <v>7</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>493</v>
+        <v>467</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -2240,10 +2249,10 @@
         <v>8</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>354</v>
+        <v>335</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>494</v>
+        <v>512</v>
       </c>
     </row>
     <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2254,7 +2263,7 @@
         <v>194</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>529</v>
+        <v>500</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -2274,16 +2283,16 @@
         <v>299</v>
       </c>
       <c r="E14" t="s">
-        <v>499</v>
+        <v>470</v>
       </c>
       <c r="F14" s="3" t="s">
         <v>300</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>355</v>
+        <v>336</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>495</v>
+        <v>513</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -2303,10 +2312,10 @@
         <v>301</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>356</v>
+        <v>337</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>496</v>
+        <v>514</v>
       </c>
     </row>
     <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2317,7 +2326,7 @@
         <v>194</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>529</v>
+        <v>500</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -2340,10 +2349,10 @@
         <v>302</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>357</v>
+        <v>338</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>310</v>
+        <v>515</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -2363,10 +2372,10 @@
         <v>303</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>358</v>
+        <v>339</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>311</v>
+        <v>516</v>
       </c>
     </row>
     <row r="19" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2391,7 +2400,7 @@
         <v>194</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>529</v>
+        <v>500</v>
       </c>
       <c r="F20" s="5">
         <v>-640</v>
@@ -2413,10 +2422,10 @@
         <v>17</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>359</v>
+        <v>340</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -2433,10 +2442,10 @@
         <v>18</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>361</v>
+        <v>342</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>360</v>
+        <v>341</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -2453,7 +2462,7 @@
         <v>19</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>313</v>
+        <v>310</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -2470,10 +2479,7 @@
         <v>20</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="H24" s="3" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.35">
@@ -2490,16 +2496,16 @@
         <v>204</v>
       </c>
       <c r="E25" t="s">
-        <v>500</v>
+        <v>471</v>
       </c>
       <c r="F25" s="3" t="s">
         <v>234</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>362</v>
+        <v>343</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>315</v>
+        <v>517</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -2516,10 +2522,10 @@
         <v>205</v>
       </c>
       <c r="E26" t="s">
-        <v>501</v>
+        <v>472</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>316</v>
+        <v>518</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -2536,10 +2542,7 @@
         <v>23</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="H27" s="3" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -2556,10 +2559,10 @@
         <v>24</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>363</v>
+        <v>344</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -2570,7 +2573,7 @@
         <v>193</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>529</v>
+        <v>500</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>206</v>
@@ -2596,10 +2599,10 @@
         <v>235</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>364</v>
+        <v>345</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>319</v>
+        <v>519</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -2619,10 +2622,10 @@
         <v>236</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>365</v>
+        <v>346</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -2642,10 +2645,10 @@
         <v>237</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>366</v>
+        <v>347</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>321</v>
+        <v>520</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -2665,10 +2668,10 @@
         <v>238</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>367</v>
+        <v>348</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>322</v>
+        <v>315</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -2688,10 +2691,10 @@
         <v>239</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>368</v>
+        <v>349</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>323</v>
+        <v>521</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -2711,10 +2714,10 @@
         <v>240</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>369</v>
+        <v>350</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -2731,7 +2734,7 @@
         <v>32</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -2748,10 +2751,10 @@
         <v>33</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>372</v>
+        <v>353</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>326</v>
+        <v>522</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -2768,10 +2771,7 @@
         <v>34</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>373</v>
-      </c>
-      <c r="H38" s="3" t="s">
-        <v>327</v>
+        <v>354</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -2788,7 +2788,7 @@
         <v>207</v>
       </c>
       <c r="E39" t="s">
-        <v>502</v>
+        <v>473</v>
       </c>
       <c r="F39" s="3">
         <v>-1815</v>
@@ -2808,16 +2808,16 @@
         <v>209</v>
       </c>
       <c r="E40" t="s">
-        <v>503</v>
+        <v>474</v>
       </c>
       <c r="F40" s="3">
         <v>-375</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>374</v>
+        <v>355</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>328</v>
+        <v>523</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -2837,7 +2837,7 @@
         <v>241</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>375</v>
+        <v>356</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
@@ -2857,7 +2857,10 @@
         <v>242</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>317</v>
+        <v>312</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>383</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
@@ -2874,13 +2877,13 @@
         <v>39</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>480</v>
+        <v>456</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>376</v>
+        <v>357</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>329</v>
+        <v>524</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
@@ -2897,10 +2900,10 @@
         <v>40</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>481</v>
+        <v>457</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>377</v>
+        <v>525</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
@@ -2920,7 +2923,7 @@
         <v>243</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>330</v>
+        <v>318</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
@@ -2940,7 +2943,7 @@
         <v>-1840</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>378</v>
+        <v>358</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
@@ -2974,10 +2977,13 @@
         <v>44</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>482</v>
+        <v>458</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>379</v>
+        <v>359</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>526</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
@@ -2994,10 +3000,13 @@
         <v>45</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>331</v>
+        <v>319</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>380</v>
+        <v>360</v>
+      </c>
+      <c r="H49" s="3" t="s">
+        <v>527</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
@@ -3028,7 +3037,7 @@
         <v>47</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>332</v>
+        <v>528</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
@@ -3048,10 +3057,10 @@
         <v>244</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>381</v>
+        <v>361</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>333</v>
+        <v>529</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
@@ -3068,13 +3077,13 @@
         <v>49</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>483</v>
+        <v>459</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>382</v>
+        <v>362</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>334</v>
+        <v>530</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
@@ -3091,13 +3100,10 @@
         <v>50</v>
       </c>
       <c r="F54" s="4" t="s">
-        <v>484</v>
+        <v>460</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>383</v>
-      </c>
-      <c r="H54" s="3" t="s">
-        <v>335</v>
+        <v>363</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
@@ -3114,11 +3120,11 @@
         <v>51</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>485</v>
+        <v>461</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="3" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
@@ -3135,10 +3141,13 @@
         <v>52</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>486</v>
+        <v>462</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>337</v>
+        <v>322</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>531</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
@@ -3155,13 +3164,13 @@
         <v>53</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>487</v>
+        <v>463</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>384</v>
+        <v>364</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
@@ -3178,7 +3187,7 @@
         <v>54</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>314</v>
+        <v>311</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
@@ -3195,7 +3204,7 @@
         <v>55</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>472</v>
+        <v>448</v>
       </c>
       <c r="G59" s="4"/>
     </row>
@@ -3213,10 +3222,10 @@
         <v>56</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>386</v>
+        <v>366</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>385</v>
+        <v>365</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
@@ -3233,10 +3242,10 @@
         <v>57</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>387</v>
+        <v>367</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>339</v>
+        <v>532</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
@@ -3253,13 +3262,13 @@
         <v>211</v>
       </c>
       <c r="E62" t="s">
-        <v>536</v>
+        <v>507</v>
       </c>
       <c r="F62" s="3" t="s">
         <v>245</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>340</v>
+        <v>324</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
@@ -3279,10 +3288,10 @@
         <v>246</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>390</v>
+        <v>369</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>389</v>
+        <v>533</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
@@ -3302,10 +3311,10 @@
         <v>-840</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>392</v>
+        <v>370</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>391</v>
+        <v>534</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
@@ -3322,16 +3331,16 @@
         <v>304</v>
       </c>
       <c r="E65" t="s">
-        <v>504</v>
+        <v>475</v>
       </c>
       <c r="F65" s="3" t="s">
         <v>247</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>393</v>
+        <v>371</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>342</v>
+        <v>326</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
@@ -3348,10 +3357,10 @@
         <v>307</v>
       </c>
       <c r="E66" t="s">
-        <v>505</v>
+        <v>476</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>343</v>
+        <v>327</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
@@ -3368,7 +3377,10 @@
         <v>63</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>344</v>
+        <v>328</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>535</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
@@ -3388,10 +3400,10 @@
         <v>248</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>394</v>
+        <v>372</v>
       </c>
       <c r="H68" s="3" t="s">
-        <v>345</v>
+        <v>311</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
@@ -3411,10 +3423,10 @@
         <v>-840</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>395</v>
+        <v>373</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>346</v>
+        <v>536</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
@@ -3462,10 +3474,10 @@
         <v>68</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>347</v>
+        <v>329</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>396</v>
+        <v>537</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
@@ -3485,10 +3497,10 @@
         <v>-610</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>397</v>
+        <v>374</v>
       </c>
       <c r="H73" s="3" t="s">
-        <v>348</v>
+        <v>330</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
@@ -3505,7 +3517,7 @@
         <v>70</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>349</v>
+        <v>538</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
@@ -3522,13 +3534,13 @@
         <v>71</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>488</v>
+        <v>464</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>399</v>
+        <v>376</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>398</v>
+        <v>375</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.35">
@@ -3545,10 +3557,10 @@
         <v>72</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>401</v>
+        <v>378</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>400</v>
+        <v>377</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.35">
@@ -3579,16 +3591,16 @@
         <v>212</v>
       </c>
       <c r="E78" t="s">
-        <v>506</v>
+        <v>477</v>
       </c>
       <c r="F78" s="3" t="s">
         <v>250</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>403</v>
+        <v>379</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>402</v>
+        <v>539</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
@@ -3605,13 +3617,13 @@
         <v>214</v>
       </c>
       <c r="E79" t="s">
-        <v>507</v>
+        <v>478</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>404</v>
+        <v>380</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>350</v>
+        <v>331</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.35">
@@ -3628,10 +3640,10 @@
         <v>213</v>
       </c>
       <c r="E80" t="s">
-        <v>508</v>
+        <v>479</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>405</v>
+        <v>381</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.35">
@@ -3648,7 +3660,7 @@
         <v>77</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>406</v>
+        <v>382</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.35">
@@ -3665,10 +3677,10 @@
         <v>215</v>
       </c>
       <c r="E82" t="s">
-        <v>509</v>
+        <v>480</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>407</v>
+        <v>383</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.35">
@@ -3716,7 +3728,7 @@
         <v>81</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>408</v>
+        <v>384</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.35">
@@ -3733,13 +3745,13 @@
         <v>210</v>
       </c>
       <c r="E86" t="s">
-        <v>510</v>
+        <v>481</v>
       </c>
       <c r="F86" s="3" t="s">
         <v>252</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>409</v>
+        <v>385</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.35">
@@ -3759,7 +3771,7 @@
         <v>253</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>410</v>
+        <v>386</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.35">
@@ -3776,7 +3788,7 @@
         <v>84</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>489</v>
+        <v>465</v>
       </c>
       <c r="G88" s="4"/>
     </row>
@@ -3794,7 +3806,7 @@
         <v>85</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>411</v>
+        <v>387</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.35">
@@ -3814,7 +3826,7 @@
         <v>-750</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>412</v>
+        <v>388</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.35">
@@ -3831,10 +3843,10 @@
         <v>87</v>
       </c>
       <c r="F91" s="4" t="s">
-        <v>490</v>
+        <v>466</v>
       </c>
       <c r="G91" s="4" t="s">
-        <v>333</v>
+        <v>320</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.35">
@@ -3865,7 +3877,7 @@
         <v>89</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>413</v>
+        <v>389</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.35">
@@ -3885,7 +3897,7 @@
         <v>254</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>414</v>
+        <v>390</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.35">
@@ -3902,10 +3914,10 @@
         <v>216</v>
       </c>
       <c r="E95" t="s">
-        <v>511</v>
+        <v>482</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>415</v>
+        <v>391</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.35">
@@ -3922,7 +3934,7 @@
         <v>92</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>416</v>
+        <v>392</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.35">
@@ -3953,7 +3965,7 @@
         <v>94</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>417</v>
+        <v>393</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.35">
@@ -3973,7 +3985,7 @@
         <v>255</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>418</v>
+        <v>394</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.35">
@@ -3990,7 +4002,7 @@
         <v>217</v>
       </c>
       <c r="E100" t="s">
-        <v>512</v>
+        <v>483</v>
       </c>
       <c r="F100" s="3" t="s">
         <v>256</v>
@@ -4010,7 +4022,7 @@
         <v>97</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>419</v>
+        <v>395</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.35">
@@ -4027,7 +4039,7 @@
         <v>98</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>420</v>
+        <v>396</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.35">
@@ -4044,7 +4056,7 @@
         <v>220</v>
       </c>
       <c r="E103" t="s">
-        <v>513</v>
+        <v>484</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.35">
@@ -4061,13 +4073,13 @@
         <v>221</v>
       </c>
       <c r="E104" t="s">
-        <v>514</v>
+        <v>485</v>
       </c>
       <c r="F104" s="3" t="s">
         <v>257</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>421</v>
+        <v>397</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.35">
@@ -4084,7 +4096,7 @@
         <v>101</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>422</v>
+        <v>398</v>
       </c>
     </row>
     <row r="106" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -4115,7 +4127,7 @@
         <v>103</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>423</v>
+        <v>399</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.35">
@@ -4135,7 +4147,7 @@
         <v>258</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>424</v>
+        <v>400</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.35">
@@ -4155,7 +4167,7 @@
         <v>259</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>425</v>
+        <v>401</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.35">
@@ -4175,7 +4187,7 @@
         <v>260</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>426</v>
+        <v>402</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.35">
@@ -4195,7 +4207,7 @@
         <v>261</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>427</v>
+        <v>403</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.35">
@@ -4229,7 +4241,7 @@
         <v>109</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>428</v>
+        <v>404</v>
       </c>
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.35">
@@ -4249,7 +4261,7 @@
         <v>263</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>429</v>
+        <v>405</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.35">
@@ -4269,7 +4281,7 @@
         <v>264</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>430</v>
+        <v>406</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.35">
@@ -4289,7 +4301,7 @@
         <v>265</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>341</v>
+        <v>325</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.35">
@@ -4306,10 +4318,10 @@
         <v>222</v>
       </c>
       <c r="E117" t="s">
-        <v>515</v>
+        <v>486</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>431</v>
+        <v>407</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.35">
@@ -4326,10 +4338,10 @@
         <v>209</v>
       </c>
       <c r="E118" t="s">
-        <v>516</v>
+        <v>487</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>432</v>
+        <v>408</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.35">
@@ -4346,13 +4358,13 @@
         <v>223</v>
       </c>
       <c r="E119" t="s">
-        <v>517</v>
+        <v>488</v>
       </c>
       <c r="F119" s="3" t="s">
         <v>266</v>
       </c>
       <c r="G119" s="3" t="s">
-        <v>433</v>
+        <v>409</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.35">
@@ -4372,7 +4384,7 @@
         <v>267</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>388</v>
+        <v>368</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.35">
@@ -4389,7 +4401,7 @@
         <v>117</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>434</v>
+        <v>410</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.35">
@@ -4409,7 +4421,7 @@
         <v>268</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>435</v>
+        <v>411</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.35">
@@ -4426,7 +4438,7 @@
         <v>119</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>436</v>
+        <v>412</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.35">
@@ -4443,7 +4455,7 @@
         <v>120</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>437</v>
+        <v>413</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.35">
@@ -4460,7 +4472,7 @@
         <v>121</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>438</v>
+        <v>414</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.35">
@@ -4477,7 +4489,7 @@
         <v>122</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>439</v>
+        <v>415</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.35">
@@ -4497,7 +4509,7 @@
         <v>269</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>440</v>
+        <v>416</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.35">
@@ -4531,7 +4543,7 @@
         <v>125</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>371</v>
+        <v>352</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.35">
@@ -4548,7 +4560,7 @@
         <v>126</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>441</v>
+        <v>417</v>
       </c>
     </row>
     <row r="131" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -4582,7 +4594,7 @@
         <v>270</v>
       </c>
       <c r="G132" s="3" t="s">
-        <v>370</v>
+        <v>351</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.35">
@@ -4602,7 +4614,7 @@
         <v>271</v>
       </c>
       <c r="G133" s="3" t="s">
-        <v>442</v>
+        <v>418</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.35">
@@ -4622,7 +4634,7 @@
         <v>-590</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>443</v>
+        <v>419</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.35">
@@ -4642,7 +4654,7 @@
         <v>272</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>444</v>
+        <v>420</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.35">
@@ -4659,7 +4671,7 @@
         <v>132</v>
       </c>
       <c r="G136" s="3" t="s">
-        <v>445</v>
+        <v>421</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.35">
@@ -4679,7 +4691,7 @@
         <v>273</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>446</v>
+        <v>422</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.35">
@@ -4699,7 +4711,7 @@
         <v>274</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>447</v>
+        <v>423</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.35">
@@ -4733,7 +4745,7 @@
         <v>275</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>448</v>
+        <v>424</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.35">
@@ -4767,7 +4779,7 @@
         <v>138</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>449</v>
+        <v>425</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.35">
@@ -4784,7 +4796,7 @@
         <v>139</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>433</v>
+        <v>409</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.35">
@@ -4801,10 +4813,10 @@
         <v>218</v>
       </c>
       <c r="E144" t="s">
-        <v>518</v>
+        <v>489</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>450</v>
+        <v>426</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.35">
@@ -4838,13 +4850,13 @@
         <v>219</v>
       </c>
       <c r="E146" t="s">
-        <v>519</v>
+        <v>490</v>
       </c>
       <c r="F146" s="3" t="s">
         <v>277</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>451</v>
+        <v>427</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.35">
@@ -4861,7 +4873,7 @@
         <v>143</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>452</v>
+        <v>428</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.35">
@@ -4878,7 +4890,7 @@
         <v>144</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>453</v>
+        <v>429</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.35">
@@ -4943,7 +4955,7 @@
         <v>148</v>
       </c>
       <c r="G152" s="3" t="s">
-        <v>454</v>
+        <v>430</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.35">
@@ -4960,10 +4972,10 @@
         <v>210</v>
       </c>
       <c r="E153" t="s">
-        <v>520</v>
+        <v>491</v>
       </c>
       <c r="G153" s="3" t="s">
-        <v>455</v>
+        <v>431</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.35">
@@ -5028,7 +5040,7 @@
         <v>153</v>
       </c>
       <c r="G157" s="3" t="s">
-        <v>456</v>
+        <v>432</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.35">
@@ -5062,7 +5074,7 @@
         <v>281</v>
       </c>
       <c r="G159" s="3" t="s">
-        <v>457</v>
+        <v>433</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.35">
@@ -5082,7 +5094,7 @@
         <v>282</v>
       </c>
       <c r="G160" s="3" t="s">
-        <v>458</v>
+        <v>434</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.35">
@@ -5102,7 +5114,7 @@
         <v>-440</v>
       </c>
       <c r="G161" s="3" t="s">
-        <v>459</v>
+        <v>435</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.35">
@@ -5119,7 +5131,7 @@
         <v>224</v>
       </c>
       <c r="E162" t="s">
-        <v>521</v>
+        <v>492</v>
       </c>
       <c r="F162" s="3" t="s">
         <v>283</v>
@@ -5139,7 +5151,7 @@
         <v>159</v>
       </c>
       <c r="G163" s="3" t="s">
-        <v>460</v>
+        <v>436</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.35">
@@ -5156,7 +5168,7 @@
         <v>160</v>
       </c>
       <c r="G164" s="3" t="s">
-        <v>461</v>
+        <v>437</v>
       </c>
     </row>
     <row r="165" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5190,7 +5202,7 @@
         <v>162</v>
       </c>
       <c r="G166" s="3" t="s">
-        <v>462</v>
+        <v>438</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.35">
@@ -5207,10 +5219,10 @@
         <v>219</v>
       </c>
       <c r="E167" t="s">
-        <v>522</v>
+        <v>493</v>
       </c>
       <c r="G167" s="3" t="s">
-        <v>387</v>
+        <v>367</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.35">
@@ -5230,7 +5242,7 @@
         <v>284</v>
       </c>
       <c r="G168" s="3" t="s">
-        <v>463</v>
+        <v>439</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.35">
@@ -5247,7 +5259,7 @@
         <v>226</v>
       </c>
       <c r="E169" t="s">
-        <v>523</v>
+        <v>494</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.35">
@@ -5272,7 +5284,7 @@
         <v>195</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>529</v>
+        <v>500</v>
       </c>
       <c r="D171" s="2" t="s">
         <v>227</v>
@@ -5298,7 +5310,7 @@
         <v>285</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>464</v>
+        <v>440</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.35">
@@ -5318,7 +5330,7 @@
         <v>-1100</v>
       </c>
       <c r="G173" s="3" t="s">
-        <v>465</v>
+        <v>441</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.35">
@@ -5366,10 +5378,10 @@
         <v>229</v>
       </c>
       <c r="E176" t="s">
-        <v>524</v>
+        <v>495</v>
       </c>
       <c r="G176" s="3" t="s">
-        <v>466</v>
+        <v>442</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.35">
@@ -5386,7 +5398,7 @@
         <v>173</v>
       </c>
       <c r="G177" s="3" t="s">
-        <v>360</v>
+        <v>341</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.35">
@@ -5403,13 +5415,13 @@
         <v>230</v>
       </c>
       <c r="E178" t="s">
-        <v>525</v>
+        <v>496</v>
       </c>
       <c r="F178" s="3" t="s">
         <v>287</v>
       </c>
       <c r="G178" s="3" t="s">
-        <v>467</v>
+        <v>443</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.35">
@@ -5426,7 +5438,7 @@
         <v>175</v>
       </c>
       <c r="G179" s="3" t="s">
-        <v>407</v>
+        <v>383</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.35">
@@ -5446,7 +5458,7 @@
         <v>288</v>
       </c>
       <c r="G180" s="3" t="s">
-        <v>468</v>
+        <v>444</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.35">
@@ -5463,10 +5475,10 @@
         <v>218</v>
       </c>
       <c r="E181" t="s">
-        <v>526</v>
+        <v>497</v>
       </c>
       <c r="G181" s="3" t="s">
-        <v>469</v>
+        <v>445</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.35">
@@ -5503,7 +5515,7 @@
         <v>291</v>
       </c>
       <c r="G183" s="3" t="s">
-        <v>470</v>
+        <v>446</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.35">
@@ -5537,7 +5549,7 @@
         <v>181</v>
       </c>
       <c r="G185" s="3" t="s">
-        <v>471</v>
+        <v>447</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.35">
@@ -5568,10 +5580,10 @@
         <v>228</v>
       </c>
       <c r="E187" t="s">
-        <v>527</v>
+        <v>498</v>
       </c>
       <c r="G187" s="3" t="s">
-        <v>473</v>
+        <v>449</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.35">
@@ -5588,7 +5600,7 @@
         <v>184</v>
       </c>
       <c r="G188" s="3" t="s">
-        <v>474</v>
+        <v>450</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.35">
@@ -5608,7 +5620,7 @@
         <v>292</v>
       </c>
       <c r="G189" s="3" t="s">
-        <v>475</v>
+        <v>451</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.35">
@@ -5625,13 +5637,13 @@
         <v>208</v>
       </c>
       <c r="E190" t="s">
-        <v>528</v>
+        <v>499</v>
       </c>
       <c r="F190" s="3" t="s">
         <v>293</v>
       </c>
       <c r="G190" s="3" t="s">
-        <v>476</v>
+        <v>452</v>
       </c>
     </row>
     <row r="191" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5642,7 +5654,7 @@
         <v>195</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>530</v>
+        <v>501</v>
       </c>
       <c r="D191" s="2" t="s">
         <v>231</v>
@@ -5670,7 +5682,7 @@
         <v>295</v>
       </c>
       <c r="G192" s="3" t="s">
-        <v>477</v>
+        <v>453</v>
       </c>
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.35">
@@ -5690,7 +5702,7 @@
         <v>296</v>
       </c>
       <c r="G193" s="3" t="s">
-        <v>478</v>
+        <v>454</v>
       </c>
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.35">
@@ -5710,7 +5722,7 @@
         <v>297</v>
       </c>
       <c r="G194" s="3" t="s">
-        <v>479</v>
+        <v>455</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ending 2017 exclusion defintion from outputs from MacFerrin et al., 2019. 2018 to be done.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{523ADF36-6544-44CF-8047-9DEBB1D3A37D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF2AB62-BF67-4C11-86D1-E294A88706A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3680" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="540">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="565">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -1645,6 +1645,81 @@
   </si>
   <si>
     <t>9330-9770</t>
+  </si>
+  <si>
+    <t>3910-</t>
+  </si>
+  <si>
+    <t>1270-</t>
+  </si>
+  <si>
+    <t>760-900 1155-1315 3130-3170 3250-3300</t>
+  </si>
+  <si>
+    <t>1690-1900 2750-2815 3000-3070 3580-</t>
+  </si>
+  <si>
+    <t>855-945 2570-2650</t>
+  </si>
+  <si>
+    <t>2700-2935</t>
+  </si>
+  <si>
+    <t>-1645 1770-1865 2865-2950 2970-</t>
+  </si>
+  <si>
+    <t>535-1240 3090-3230</t>
+  </si>
+  <si>
+    <t>5090-6365</t>
+  </si>
+  <si>
+    <t>2700-2850</t>
+  </si>
+  <si>
+    <t>4145-</t>
+  </si>
+  <si>
+    <t>1740-2040 2870-3930</t>
+  </si>
+  <si>
+    <t>5255-5410 15660-15790 16495-</t>
+  </si>
+  <si>
+    <t>21700-21850</t>
+  </si>
+  <si>
+    <t>-315 950-1055</t>
+  </si>
+  <si>
+    <t>-200 660-800 1560-1575</t>
+  </si>
+  <si>
+    <t>530-630</t>
+  </si>
+  <si>
+    <t>-475 1130-1170 5875-5950 6190-6340 6715-7370 7460-7780 7900-</t>
+  </si>
+  <si>
+    <t>-175 290-340 630-970 1090-1220</t>
+  </si>
+  <si>
+    <t>1720-</t>
+  </si>
+  <si>
+    <t>-240 1085-1315 1390-1430 1450-1530 1740-1810 2030-2060</t>
+  </si>
+  <si>
+    <t>3770-3900 4265-4335</t>
+  </si>
+  <si>
+    <t>-70 2050-2310</t>
+  </si>
+  <si>
+    <t>6690-6730</t>
+  </si>
+  <si>
+    <t>6480-6505 7200-7250</t>
   </si>
 </sst>
 </file>
@@ -2011,8 +2086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
   <dimension ref="A1:H194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B25" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I83" sqref="I83"/>
+    <sheetView tabSelected="1" topLeftCell="D125" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G137" sqref="G137"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2020,7 +2095,8 @@
     <col min="1" max="1" width="20.453125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
     <col min="3" max="3" width="4.36328125" customWidth="1"/>
-    <col min="4" max="5" width="18.54296875" customWidth="1"/>
+    <col min="4" max="4" width="18.54296875" customWidth="1"/>
+    <col min="5" max="5" width="20.08984375" customWidth="1"/>
     <col min="6" max="7" width="16.36328125" style="3" customWidth="1"/>
     <col min="8" max="8" width="9.36328125" style="3" bestFit="1" customWidth="1"/>
   </cols>
@@ -3645,8 +3721,11 @@
       <c r="G80" s="3" t="s">
         <v>381</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H80" s="3" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A81" t="s">
         <v>77</v>
       </c>
@@ -3663,7 +3742,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A82" t="s">
         <v>78</v>
       </c>
@@ -3682,8 +3761,11 @@
       <c r="G82" s="3" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H82" s="3" t="s">
+        <v>541</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
         <v>79</v>
       </c>
@@ -3700,7 +3782,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A84" t="s">
         <v>80</v>
       </c>
@@ -3714,7 +3796,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A85" t="s">
         <v>81</v>
       </c>
@@ -3731,7 +3813,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A86" t="s">
         <v>82</v>
       </c>
@@ -3753,8 +3835,11 @@
       <c r="G86" s="3" t="s">
         <v>385</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H86" s="3" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A87" t="s">
         <v>83</v>
       </c>
@@ -3773,8 +3858,11 @@
       <c r="G87" s="3" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H87" s="3" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A88" t="s">
         <v>84</v>
       </c>
@@ -3792,7 +3880,7 @@
       </c>
       <c r="G88" s="4"/>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A89" t="s">
         <v>85</v>
       </c>
@@ -3808,8 +3896,11 @@
       <c r="G89" s="3" t="s">
         <v>387</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H89" s="3" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A90" t="s">
         <v>86</v>
       </c>
@@ -3828,8 +3919,11 @@
       <c r="G90" s="3" t="s">
         <v>388</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H90" s="3" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
         <v>87</v>
       </c>
@@ -3848,8 +3942,11 @@
       <c r="G91" s="4" t="s">
         <v>320</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H91" s="3" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A92" t="s">
         <v>88</v>
       </c>
@@ -3862,8 +3959,11 @@
       <c r="E92" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H92" s="3" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A93" t="s">
         <v>89</v>
       </c>
@@ -3879,8 +3979,11 @@
       <c r="G93" s="3" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H93" s="3" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
         <v>90</v>
       </c>
@@ -3900,7 +4003,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
         <v>91</v>
       </c>
@@ -3920,7 +4023,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A96" t="s">
         <v>92</v>
       </c>
@@ -3950,6 +4053,9 @@
       <c r="E97" t="s">
         <v>93</v>
       </c>
+      <c r="H97" s="3" t="s">
+        <v>549</v>
+      </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A98" t="s">
@@ -4007,6 +4113,9 @@
       <c r="F100" s="3" t="s">
         <v>256</v>
       </c>
+      <c r="H100" s="3" t="s">
+        <v>550</v>
+      </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A101" t="s">
@@ -4129,6 +4238,9 @@
       <c r="G107" s="3" t="s">
         <v>399</v>
       </c>
+      <c r="H107" s="3" t="s">
+        <v>551</v>
+      </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A108" t="s">
@@ -4169,6 +4281,9 @@
       <c r="G109" s="3" t="s">
         <v>401</v>
       </c>
+      <c r="H109" s="3" t="s">
+        <v>552</v>
+      </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A110" t="s">
@@ -4227,7 +4342,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A113" t="s">
         <v>109</v>
       </c>
@@ -4244,7 +4359,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A114" t="s">
         <v>110</v>
       </c>
@@ -4264,7 +4379,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A115" t="s">
         <v>111</v>
       </c>
@@ -4283,8 +4398,11 @@
       <c r="G115" s="3" t="s">
         <v>406</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H115" s="3" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A116" t="s">
         <v>112</v>
       </c>
@@ -4304,7 +4422,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A117" t="s">
         <v>113</v>
       </c>
@@ -4323,8 +4441,11 @@
       <c r="G117" s="3" t="s">
         <v>407</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H117" s="3" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A118" t="s">
         <v>114</v>
       </c>
@@ -4344,7 +4465,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A119" t="s">
         <v>115</v>
       </c>
@@ -4366,8 +4487,11 @@
       <c r="G119" s="3" t="s">
         <v>409</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H119" s="3" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>116</v>
       </c>
@@ -4387,7 +4511,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A121" t="s">
         <v>117</v>
       </c>
@@ -4404,7 +4528,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
         <v>118</v>
       </c>
@@ -4424,7 +4548,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A123" t="s">
         <v>119</v>
       </c>
@@ -4440,8 +4564,11 @@
       <c r="G123" s="3" t="s">
         <v>412</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H123" s="3" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A124" t="s">
         <v>120</v>
       </c>
@@ -4458,7 +4585,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A125" t="s">
         <v>121</v>
       </c>
@@ -4475,7 +4602,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A126" t="s">
         <v>122</v>
       </c>
@@ -4492,7 +4619,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
         <v>123</v>
       </c>
@@ -4511,8 +4638,11 @@
       <c r="G127" s="3" t="s">
         <v>416</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H127" s="3" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A128" t="s">
         <v>124</v>
       </c>
@@ -4616,6 +4746,9 @@
       <c r="G133" s="3" t="s">
         <v>418</v>
       </c>
+      <c r="H133" s="3" t="s">
+        <v>558</v>
+      </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A134" t="s">
@@ -4636,6 +4769,9 @@
       <c r="G134" s="3" t="s">
         <v>419</v>
       </c>
+      <c r="H134" s="3" t="s">
+        <v>559</v>
+      </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
@@ -4673,6 +4809,9 @@
       <c r="G136" s="3" t="s">
         <v>421</v>
       </c>
+      <c r="H136" s="3" t="s">
+        <v>560</v>
+      </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A137" t="s">
@@ -4693,6 +4832,9 @@
       <c r="G137" s="3" t="s">
         <v>422</v>
       </c>
+      <c r="H137" s="3" t="s">
+        <v>561</v>
+      </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
@@ -4713,6 +4855,9 @@
       <c r="G138" s="3" t="s">
         <v>423</v>
       </c>
+      <c r="H138" s="3" t="s">
+        <v>562</v>
+      </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
@@ -4747,6 +4892,9 @@
       <c r="G140" s="3" t="s">
         <v>424</v>
       </c>
+      <c r="H140" s="3" t="s">
+        <v>563</v>
+      </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A141" t="s">
@@ -4763,6 +4911,9 @@
       </c>
       <c r="F141" s="3" t="s">
         <v>276</v>
+      </c>
+      <c r="H141" s="3" t="s">
+        <v>564</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Ending 2018 exclusion identification after roll correction.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF2AB62-BF67-4C11-86D1-E294A88706A7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EB42AF-F650-408D-B891-5CD83890A68F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3680" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1100" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="592">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -1707,6 +1707,9 @@
     <t>1720-</t>
   </si>
   <si>
+    <t>-240</t>
+  </si>
+  <si>
     <t>-240 1085-1315 1390-1430 1450-1530 1740-1810 2030-2060</t>
   </si>
   <si>
@@ -1720,16 +1723,100 @@
   </si>
   <si>
     <t>6480-6505 7200-7250</t>
+  </si>
+  <si>
+    <t>-7000</t>
+  </si>
+  <si>
+    <t>5680-</t>
+  </si>
+  <si>
+    <t>4330-</t>
+  </si>
+  <si>
+    <t>130-310 830-1570 1760-1860 3580-3680</t>
+  </si>
+  <si>
+    <t>-570 450-580 730-840 970-1170 1370-1510 1630-1820 1960-2080 2260-2400 2545-2690 3190-3300 3560-3660 3850-3980 4150-4320 4460-4650</t>
+  </si>
+  <si>
+    <t>920-1240 1580-1880 2820-4150 4490-4580 4750-4920 5020-5240 5340-5540 5640-6160 6610-10810 10910-11030 11280-11430</t>
+  </si>
+  <si>
+    <t>1180-1760 4830-5000</t>
+  </si>
+  <si>
+    <t>8200-</t>
+  </si>
+  <si>
+    <t>1540-1630 2120-2170</t>
+  </si>
+  <si>
+    <t>855-1350 1600-1720 2060-2210 2320-2440 2720-2880 3830-3970 10180-10290 10470-10530 13100-13160 15250-15300 15380-15430</t>
+  </si>
+  <si>
+    <t>1300-1410 1600-1740</t>
+  </si>
+  <si>
+    <t>7850-8000 8170-8310 9400-9600 9780-9870 19780-19950 21420-21600</t>
+  </si>
+  <si>
+    <t>1320-1400</t>
+  </si>
+  <si>
+    <t>-930</t>
+  </si>
+  <si>
+    <t>-355 1100-1200</t>
+  </si>
+  <si>
+    <t>100-150</t>
+  </si>
+  <si>
+    <t>5430-</t>
+  </si>
+  <si>
+    <t>1460-1580</t>
+  </si>
+  <si>
+    <t>6175-6275</t>
+  </si>
+  <si>
+    <t>-320</t>
+  </si>
+  <si>
+    <t>-100 630-710 920-1030</t>
+  </si>
+  <si>
+    <t>2930-3085</t>
+  </si>
+  <si>
+    <t>285-370</t>
+  </si>
+  <si>
+    <t>2420-2680 2830-2880 3210-3300 4140-4290</t>
+  </si>
+  <si>
+    <t>1235-1400 1515-1580</t>
+  </si>
+  <si>
+    <t>2540-2640 2860-2945 3190-3270</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1761,7 +1848,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1770,6 +1857,7 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2086,8 +2174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
   <dimension ref="A1:H194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D125" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G137" sqref="G137"/>
+    <sheetView tabSelected="1" topLeftCell="D178" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D192" sqref="D192"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -4810,7 +4898,7 @@
         <v>421</v>
       </c>
       <c r="H136" s="3" t="s">
-        <v>560</v>
+        <v>561</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.35">
@@ -4833,7 +4921,7 @@
         <v>422</v>
       </c>
       <c r="H137" s="3" t="s">
-        <v>561</v>
+        <v>562</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.35">
@@ -4856,7 +4944,7 @@
         <v>423</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>562</v>
+        <v>563</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.35">
@@ -4893,7 +4981,7 @@
         <v>424</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.35">
@@ -4913,7 +5001,7 @@
         <v>276</v>
       </c>
       <c r="H141" s="3" t="s">
-        <v>564</v>
+        <v>565</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.35">
@@ -4969,8 +5057,11 @@
       <c r="G144" s="3" t="s">
         <v>426</v>
       </c>
-    </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H144" s="3" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145" t="s">
         <v>141</v>
       </c>
@@ -4987,7 +5078,7 @@
         <v>-1600</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146" t="s">
         <v>142</v>
       </c>
@@ -5010,7 +5101,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A147" t="s">
         <v>143</v>
       </c>
@@ -5026,8 +5117,11 @@
       <c r="G147" s="3" t="s">
         <v>428</v>
       </c>
-    </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H147" s="3" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
         <v>144</v>
       </c>
@@ -5043,8 +5137,11 @@
       <c r="G148" s="3" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H148" s="3" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149" t="s">
         <v>145</v>
       </c>
@@ -5060,8 +5157,11 @@
       <c r="F149" s="3" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H149" s="3" t="s">
+        <v>569</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150" t="s">
         <v>146</v>
       </c>
@@ -5078,7 +5178,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151" t="s">
         <v>147</v>
       </c>
@@ -5092,7 +5192,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A152" t="s">
         <v>148</v>
       </c>
@@ -5108,8 +5208,11 @@
       <c r="G152" s="3" t="s">
         <v>430</v>
       </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H152" s="3" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A153" t="s">
         <v>149</v>
       </c>
@@ -5128,8 +5231,11 @@
       <c r="G153" s="3" t="s">
         <v>431</v>
       </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H153" s="3" t="s">
+        <v>571</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A154" t="s">
         <v>150</v>
       </c>
@@ -5146,7 +5252,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A155" t="s">
         <v>151</v>
       </c>
@@ -5156,14 +5262,17 @@
       <c r="C155" t="s">
         <v>201</v>
       </c>
-      <c r="E155" t="s">
+      <c r="E155" s="8" t="s">
         <v>151</v>
       </c>
       <c r="F155" s="3">
         <v>-70</v>
       </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H155" s="3" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A156" t="s">
         <v>152</v>
       </c>
@@ -5176,8 +5285,11 @@
       <c r="E156" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H156" s="3" t="s">
+        <v>573</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A157" t="s">
         <v>153</v>
       </c>
@@ -5194,7 +5306,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A158" t="s">
         <v>154</v>
       </c>
@@ -5207,8 +5319,11 @@
       <c r="E158" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H158" s="3" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A159" t="s">
         <v>155</v>
       </c>
@@ -5227,8 +5342,11 @@
       <c r="G159" s="3" t="s">
         <v>433</v>
       </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H159" s="3" t="s">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A160" t="s">
         <v>156</v>
       </c>
@@ -5246,6 +5364,9 @@
       </c>
       <c r="G160" s="3" t="s">
         <v>434</v>
+      </c>
+      <c r="H160" s="3" t="s">
+        <v>576</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.35">
@@ -5287,6 +5408,9 @@
       <c r="F162" s="3" t="s">
         <v>283</v>
       </c>
+      <c r="H162" s="3" t="s">
+        <v>577</v>
+      </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163" t="s">
@@ -5304,6 +5428,9 @@
       <c r="G163" s="3" t="s">
         <v>436</v>
       </c>
+      <c r="H163" s="3" t="s">
+        <v>578</v>
+      </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A164" t="s">
@@ -5321,6 +5448,9 @@
       <c r="G164" s="3" t="s">
         <v>437</v>
       </c>
+      <c r="H164" s="3" t="s">
+        <v>579</v>
+      </c>
     </row>
     <row r="165" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A165" s="2" t="s">
@@ -5426,6 +5556,9 @@
       <c r="E170" t="s">
         <v>166</v>
       </c>
+      <c r="H170" s="3" t="s">
+        <v>580</v>
+      </c>
     </row>
     <row r="171" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A171" s="2" t="s">
@@ -5463,6 +5596,9 @@
       <c r="G172" s="3" t="s">
         <v>440</v>
       </c>
+      <c r="H172" s="3" t="s">
+        <v>581</v>
+      </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A173" t="s">
@@ -5483,6 +5619,9 @@
       <c r="G173" s="3" t="s">
         <v>441</v>
       </c>
+      <c r="H173" s="3" t="s">
+        <v>582</v>
+      </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A174" t="s">
@@ -5497,6 +5636,9 @@
       <c r="E174" t="s">
         <v>170</v>
       </c>
+      <c r="H174" s="3" t="s">
+        <v>583</v>
+      </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
@@ -5551,6 +5693,9 @@
       <c r="G177" s="3" t="s">
         <v>341</v>
       </c>
+      <c r="H177" s="3" t="s">
+        <v>584</v>
+      </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A178" t="s">
@@ -5574,6 +5719,9 @@
       <c r="G178" s="3" t="s">
         <v>443</v>
       </c>
+      <c r="H178" s="3" t="s">
+        <v>585</v>
+      </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
@@ -5611,6 +5759,9 @@
       <c r="G180" s="3" t="s">
         <v>444</v>
       </c>
+      <c r="H180" s="3" t="s">
+        <v>586</v>
+      </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A181" t="s">
@@ -5631,6 +5782,9 @@
       <c r="G181" s="3" t="s">
         <v>445</v>
       </c>
+      <c r="H181" s="3" t="s">
+        <v>587</v>
+      </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
@@ -5716,6 +5870,9 @@
       <c r="E186" t="s">
         <v>182</v>
       </c>
+      <c r="H186" s="3" t="s">
+        <v>588</v>
+      </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A187" t="s">
@@ -5736,6 +5893,9 @@
       <c r="G187" s="3" t="s">
         <v>449</v>
       </c>
+      <c r="H187" s="3" t="s">
+        <v>589</v>
+      </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A188" t="s">
@@ -5753,6 +5913,9 @@
       <c r="G188" s="3" t="s">
         <v>450</v>
       </c>
+      <c r="H188" s="3" t="s">
+        <v>590</v>
+      </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A189" t="s">
@@ -5773,6 +5936,9 @@
       <c r="G189" s="3" t="s">
         <v>451</v>
       </c>
+      <c r="H189" s="3" t="s">
+        <v>591</v>
+      </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A190" t="s">
@@ -5836,7 +6002,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="193" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A193" t="s">
         <v>189</v>
       </c>
@@ -5856,7 +6022,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="194" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A194" t="s">
         <v>190</v>
       </c>
@@ -5874,6 +6040,9 @@
       </c>
       <c r="G194" s="3" t="s">
         <v>455</v>
+      </c>
+      <c r="H194" s="3" t="s">
+        <v>560</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correcting a mistake in exclusion_fail_roll_correction.txt
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80EB42AF-F650-408D-B891-5CD83890A68F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DE6BAC-5815-401C-AA07-848E614A50D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3680" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -1626,9 +1626,6 @@
     <t>-1470 3830-</t>
   </si>
   <si>
-    <t>-1400 1700-2515  4100-5430 6335-7770 9000-9800 11360-11820 17130-18480 19980-21440 22730-22920 25430-26250 28560-30485 34710-34810</t>
-  </si>
-  <si>
     <t>1440-1690 1850-2220 2275-2330 2920-2980 3390-3470 3540-3650 3750-3850 3895-3990 4190-4215 4270-4330 4400-</t>
   </si>
   <si>
@@ -1801,6 +1798,9 @@
   </si>
   <si>
     <t>2540-2640 2860-2945 3190-3270</t>
+  </si>
+  <si>
+    <t>-1400 1700-2515 4100-5430 6335-7770 9000-9800 11360-11820 17130-18480 19980-21440 22730-22920 25430-26250 28560-30485 34710-34810</t>
   </si>
 </sst>
 </file>
@@ -2174,8 +2174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
   <dimension ref="A1:H194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D178" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D192" sqref="D192"/>
+    <sheetView tabSelected="1" topLeftCell="D58" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H63" sqref="H63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3455,7 +3455,7 @@
         <v>369</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>533</v>
+        <v>591</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
@@ -3478,7 +3478,7 @@
         <v>370</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
@@ -3544,7 +3544,7 @@
         <v>328</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
@@ -3590,7 +3590,7 @@
         <v>373</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
@@ -3641,7 +3641,7 @@
         <v>329</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
@@ -3681,7 +3681,7 @@
         <v>70</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
@@ -3764,7 +3764,7 @@
         <v>379</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
@@ -3810,7 +3810,7 @@
         <v>381</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.35">
@@ -3850,7 +3850,7 @@
         <v>383</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.35">
@@ -3924,7 +3924,7 @@
         <v>385</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.35">
@@ -3947,7 +3947,7 @@
         <v>386</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.35">
@@ -3985,7 +3985,7 @@
         <v>387</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.35">
@@ -4008,7 +4008,7 @@
         <v>388</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.35">
@@ -4031,7 +4031,7 @@
         <v>320</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.35">
@@ -4048,7 +4048,7 @@
         <v>88</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.35">
@@ -4068,7 +4068,7 @@
         <v>389</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.35">
@@ -4142,7 +4142,7 @@
         <v>93</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.35">
@@ -4202,7 +4202,7 @@
         <v>256</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.35">
@@ -4327,7 +4327,7 @@
         <v>399</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.35">
@@ -4370,7 +4370,7 @@
         <v>401</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.35">
@@ -4487,7 +4487,7 @@
         <v>406</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.35">
@@ -4530,7 +4530,7 @@
         <v>407</v>
       </c>
       <c r="H117" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.35">
@@ -4576,7 +4576,7 @@
         <v>409</v>
       </c>
       <c r="H119" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.35">
@@ -4653,7 +4653,7 @@
         <v>412</v>
       </c>
       <c r="H123" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.35">
@@ -4727,7 +4727,7 @@
         <v>416</v>
       </c>
       <c r="H127" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.35">
@@ -4835,7 +4835,7 @@
         <v>418</v>
       </c>
       <c r="H133" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.35">
@@ -4858,7 +4858,7 @@
         <v>419</v>
       </c>
       <c r="H134" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.35">
@@ -4898,7 +4898,7 @@
         <v>421</v>
       </c>
       <c r="H136" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.35">
@@ -4921,7 +4921,7 @@
         <v>422</v>
       </c>
       <c r="H137" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.35">
@@ -4944,7 +4944,7 @@
         <v>423</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.35">
@@ -4981,7 +4981,7 @@
         <v>424</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.35">
@@ -5001,7 +5001,7 @@
         <v>276</v>
       </c>
       <c r="H141" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.35">
@@ -5058,7 +5058,7 @@
         <v>426</v>
       </c>
       <c r="H144" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.35">
@@ -5118,7 +5118,7 @@
         <v>428</v>
       </c>
       <c r="H147" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.35">
@@ -5138,7 +5138,7 @@
         <v>429</v>
       </c>
       <c r="H148" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.35">
@@ -5158,7 +5158,7 @@
         <v>278</v>
       </c>
       <c r="H149" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.35">
@@ -5209,7 +5209,7 @@
         <v>430</v>
       </c>
       <c r="H152" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.35">
@@ -5232,7 +5232,7 @@
         <v>431</v>
       </c>
       <c r="H153" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.35">
@@ -5269,7 +5269,7 @@
         <v>-70</v>
       </c>
       <c r="H155" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.35">
@@ -5286,7 +5286,7 @@
         <v>152</v>
       </c>
       <c r="H156" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.35">
@@ -5320,7 +5320,7 @@
         <v>154</v>
       </c>
       <c r="H158" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.35">
@@ -5343,7 +5343,7 @@
         <v>433</v>
       </c>
       <c r="H159" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.35">
@@ -5366,7 +5366,7 @@
         <v>434</v>
       </c>
       <c r="H160" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.35">
@@ -5409,7 +5409,7 @@
         <v>283</v>
       </c>
       <c r="H162" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.35">
@@ -5429,7 +5429,7 @@
         <v>436</v>
       </c>
       <c r="H163" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.35">
@@ -5449,7 +5449,7 @@
         <v>437</v>
       </c>
       <c r="H164" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="165" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5557,7 +5557,7 @@
         <v>166</v>
       </c>
       <c r="H170" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="171" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5597,7 +5597,7 @@
         <v>440</v>
       </c>
       <c r="H172" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.35">
@@ -5620,7 +5620,7 @@
         <v>441</v>
       </c>
       <c r="H173" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.35">
@@ -5637,7 +5637,7 @@
         <v>170</v>
       </c>
       <c r="H174" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.35">
@@ -5694,7 +5694,7 @@
         <v>341</v>
       </c>
       <c r="H177" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.35">
@@ -5720,7 +5720,7 @@
         <v>443</v>
       </c>
       <c r="H178" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.35">
@@ -5760,7 +5760,7 @@
         <v>444</v>
       </c>
       <c r="H180" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.35">
@@ -5783,7 +5783,7 @@
         <v>445</v>
       </c>
       <c r="H181" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.35">
@@ -5871,7 +5871,7 @@
         <v>182</v>
       </c>
       <c r="H186" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.35">
@@ -5894,7 +5894,7 @@
         <v>449</v>
       </c>
       <c r="H187" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.35">
@@ -5914,7 +5914,7 @@
         <v>450</v>
       </c>
       <c r="H188" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.35">
@@ -5937,7 +5937,7 @@
         <v>451</v>
       </c>
       <c r="H189" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.35">
@@ -6042,7 +6042,7 @@
         <v>455</v>
       </c>
       <c r="H194" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Correcting a typo in exclusions_fail_roll_correction.txt
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24DE6BAC-5815-401C-AA07-848E614A50D0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9556048-A4C4-47F9-8A3F-7BF853F8D907}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3680" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -1590,9 +1590,6 @@
     <t>670-1120 2640-2760 4510-4950 17900-18360 27360-29020 29740-29910 30890-31460 31950-32410 39580-</t>
   </si>
   <si>
-    <t>2560- 4530-4610 4660-4770 4850-4890 4980-5200 6100-6230</t>
-  </si>
-  <si>
     <t>-170</t>
   </si>
   <si>
@@ -1801,6 +1798,9 @@
   </si>
   <si>
     <t>-1400 1700-2515 4100-5430 6335-7770 9000-9800 11360-11820 17130-18480 19980-21440 22730-22920 25430-26250 28560-30485 34710-34810</t>
+  </si>
+  <si>
+    <t>4530-4610 4660-4770 4850-4890 4980-5200 6100-6230</t>
   </si>
 </sst>
 </file>
@@ -2174,8 +2174,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
   <dimension ref="A1:H194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" topLeftCell="D22" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H34" sqref="H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2858,7 +2858,7 @@
         <v>349</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>521</v>
+        <v>591</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -2918,7 +2918,7 @@
         <v>353</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -2981,7 +2981,7 @@
         <v>355</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -3047,7 +3047,7 @@
         <v>357</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>524</v>
+        <v>523</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
@@ -3067,7 +3067,7 @@
         <v>457</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>525</v>
+        <v>524</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
@@ -3147,7 +3147,7 @@
         <v>359</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>526</v>
+        <v>525</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
@@ -3170,7 +3170,7 @@
         <v>360</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
@@ -3201,7 +3201,7 @@
         <v>47</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>528</v>
+        <v>527</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
@@ -3224,7 +3224,7 @@
         <v>361</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>529</v>
+        <v>528</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
@@ -3247,7 +3247,7 @@
         <v>362</v>
       </c>
       <c r="H53" s="3" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
@@ -3311,7 +3311,7 @@
         <v>322</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>531</v>
+        <v>530</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
@@ -3409,7 +3409,7 @@
         <v>367</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>532</v>
+        <v>531</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
@@ -3455,7 +3455,7 @@
         <v>369</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
@@ -3478,7 +3478,7 @@
         <v>370</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>533</v>
+        <v>532</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
@@ -3544,7 +3544,7 @@
         <v>328</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
@@ -3590,7 +3590,7 @@
         <v>373</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>535</v>
+        <v>534</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
@@ -3641,7 +3641,7 @@
         <v>329</v>
       </c>
       <c r="H72" s="3" t="s">
-        <v>536</v>
+        <v>535</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
@@ -3681,7 +3681,7 @@
         <v>70</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>537</v>
+        <v>536</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
@@ -3764,7 +3764,7 @@
         <v>379</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
@@ -3810,7 +3810,7 @@
         <v>381</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.35">
@@ -3850,7 +3850,7 @@
         <v>383</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>540</v>
+        <v>539</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.35">
@@ -3924,7 +3924,7 @@
         <v>385</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>541</v>
+        <v>540</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.35">
@@ -3947,7 +3947,7 @@
         <v>386</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>542</v>
+        <v>541</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.35">
@@ -3985,7 +3985,7 @@
         <v>387</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.35">
@@ -4008,7 +4008,7 @@
         <v>388</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>544</v>
+        <v>543</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.35">
@@ -4031,7 +4031,7 @@
         <v>320</v>
       </c>
       <c r="H91" s="3" t="s">
-        <v>545</v>
+        <v>544</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.35">
@@ -4048,7 +4048,7 @@
         <v>88</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>546</v>
+        <v>545</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.35">
@@ -4068,7 +4068,7 @@
         <v>389</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.35">
@@ -4142,7 +4142,7 @@
         <v>93</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.35">
@@ -4202,7 +4202,7 @@
         <v>256</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>549</v>
+        <v>548</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.35">
@@ -4327,7 +4327,7 @@
         <v>399</v>
       </c>
       <c r="H107" s="3" t="s">
-        <v>550</v>
+        <v>549</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.35">
@@ -4370,7 +4370,7 @@
         <v>401</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>551</v>
+        <v>550</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.35">
@@ -4487,7 +4487,7 @@
         <v>406</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.35">
@@ -4530,7 +4530,7 @@
         <v>407</v>
       </c>
       <c r="H117" s="3" t="s">
-        <v>553</v>
+        <v>552</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.35">
@@ -4576,7 +4576,7 @@
         <v>409</v>
       </c>
       <c r="H119" s="3" t="s">
-        <v>554</v>
+        <v>553</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.35">
@@ -4653,7 +4653,7 @@
         <v>412</v>
       </c>
       <c r="H123" s="3" t="s">
-        <v>555</v>
+        <v>554</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.35">
@@ -4727,7 +4727,7 @@
         <v>416</v>
       </c>
       <c r="H127" s="3" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.35">
@@ -4835,7 +4835,7 @@
         <v>418</v>
       </c>
       <c r="H133" s="3" t="s">
-        <v>557</v>
+        <v>556</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.35">
@@ -4858,7 +4858,7 @@
         <v>419</v>
       </c>
       <c r="H134" s="3" t="s">
-        <v>558</v>
+        <v>557</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.35">
@@ -4898,7 +4898,7 @@
         <v>421</v>
       </c>
       <c r="H136" s="3" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.35">
@@ -4921,7 +4921,7 @@
         <v>422</v>
       </c>
       <c r="H137" s="3" t="s">
-        <v>561</v>
+        <v>560</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.35">
@@ -4944,7 +4944,7 @@
         <v>423</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.35">
@@ -4981,7 +4981,7 @@
         <v>424</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.35">
@@ -5001,7 +5001,7 @@
         <v>276</v>
       </c>
       <c r="H141" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.35">
@@ -5058,7 +5058,7 @@
         <v>426</v>
       </c>
       <c r="H144" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.35">
@@ -5118,7 +5118,7 @@
         <v>428</v>
       </c>
       <c r="H147" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.35">
@@ -5138,7 +5138,7 @@
         <v>429</v>
       </c>
       <c r="H148" s="3" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.35">
@@ -5158,7 +5158,7 @@
         <v>278</v>
       </c>
       <c r="H149" s="3" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.35">
@@ -5209,7 +5209,7 @@
         <v>430</v>
       </c>
       <c r="H152" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.35">
@@ -5232,7 +5232,7 @@
         <v>431</v>
       </c>
       <c r="H153" s="3" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.35">
@@ -5269,7 +5269,7 @@
         <v>-70</v>
       </c>
       <c r="H155" s="3" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.35">
@@ -5286,7 +5286,7 @@
         <v>152</v>
       </c>
       <c r="H156" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.35">
@@ -5320,7 +5320,7 @@
         <v>154</v>
       </c>
       <c r="H158" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.35">
@@ -5343,7 +5343,7 @@
         <v>433</v>
       </c>
       <c r="H159" s="3" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.35">
@@ -5366,7 +5366,7 @@
         <v>434</v>
       </c>
       <c r="H160" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.35">
@@ -5409,7 +5409,7 @@
         <v>283</v>
       </c>
       <c r="H162" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.35">
@@ -5429,7 +5429,7 @@
         <v>436</v>
       </c>
       <c r="H163" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.35">
@@ -5449,7 +5449,7 @@
         <v>437</v>
       </c>
       <c r="H164" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
     </row>
     <row r="165" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5557,7 +5557,7 @@
         <v>166</v>
       </c>
       <c r="H170" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="171" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
@@ -5597,7 +5597,7 @@
         <v>440</v>
       </c>
       <c r="H172" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.35">
@@ -5620,7 +5620,7 @@
         <v>441</v>
       </c>
       <c r="H173" s="3" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.35">
@@ -5637,7 +5637,7 @@
         <v>170</v>
       </c>
       <c r="H174" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.35">
@@ -5694,7 +5694,7 @@
         <v>341</v>
       </c>
       <c r="H177" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.35">
@@ -5720,7 +5720,7 @@
         <v>443</v>
       </c>
       <c r="H178" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.35">
@@ -5760,7 +5760,7 @@
         <v>444</v>
       </c>
       <c r="H180" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.35">
@@ -5783,7 +5783,7 @@
         <v>445</v>
       </c>
       <c r="H181" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.35">
@@ -5871,7 +5871,7 @@
         <v>182</v>
       </c>
       <c r="H186" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.35">
@@ -5894,7 +5894,7 @@
         <v>449</v>
       </c>
       <c r="H187" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.35">
@@ -5914,7 +5914,7 @@
         <v>450</v>
       </c>
       <c r="H188" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.35">
@@ -5937,7 +5937,7 @@
         <v>451</v>
       </c>
       <c r="H189" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.35">
@@ -6042,7 +6042,7 @@
         <v>455</v>
       </c>
       <c r="H194" s="3" t="s">
-        <v>559</v>
+        <v>558</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Identification of dry firn exclusions in 2017. To be continued.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9556048-A4C4-47F9-8A3F-7BF853F8D907}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217D0D81-2BF4-4EF1-9DF5-144A5098E2A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14380" windowHeight="3680" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3675" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1127" uniqueCount="592">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="646">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -1801,6 +1801,168 @@
   </si>
   <si>
     <t>4530-4610 4660-4770 4850-4890 4980-5200 6100-6230</t>
+  </si>
+  <si>
+    <t>Dry firn and other exclusions</t>
+  </si>
+  <si>
+    <t>dry_firn_and_other_exclusions</t>
+  </si>
+  <si>
+    <t>1340-</t>
+  </si>
+  <si>
+    <t>1880-</t>
+  </si>
+  <si>
+    <t>30580-30700 30780-30820</t>
+  </si>
+  <si>
+    <t>1150-</t>
+  </si>
+  <si>
+    <t>1590-</t>
+  </si>
+  <si>
+    <t>3050-6595 7210-7370 7700-8240 8425-8540 8870-9380 9523-9690 10400-10960 11250-11320 25980-</t>
+  </si>
+  <si>
+    <t>-2240 5980-</t>
+  </si>
+  <si>
+    <t>to delete</t>
+  </si>
+  <si>
+    <t>-3960 5555-5620 15260-16100 16390-17100 23260-24360 27240-27350 29910-30560 31870-31940</t>
+  </si>
+  <si>
+    <t>8400-</t>
+  </si>
+  <si>
+    <t>-750</t>
+  </si>
+  <si>
+    <t>-1885</t>
+  </si>
+  <si>
+    <t>-1850 1918-</t>
+  </si>
+  <si>
+    <t>-610 3215-</t>
+  </si>
+  <si>
+    <t>to delete though slabs at the surface …</t>
+  </si>
+  <si>
+    <t>-1440</t>
+  </si>
+  <si>
+    <t>1320-3625</t>
+  </si>
+  <si>
+    <t>2750-3000</t>
+  </si>
+  <si>
+    <t>470-680 1690-</t>
+  </si>
+  <si>
+    <t>2400-3500</t>
+  </si>
+  <si>
+    <t>2200-3400 4245-4670 5060-5510</t>
+  </si>
+  <si>
+    <t>880-</t>
+  </si>
+  <si>
+    <t>to delete though slabs at the surface but signal too noisy</t>
+  </si>
+  <si>
+    <t>1540-</t>
+  </si>
+  <si>
+    <t>-2010 2340-</t>
+  </si>
+  <si>
+    <t>-2015</t>
+  </si>
+  <si>
+    <t>-1810</t>
+  </si>
+  <si>
+    <t>2820-</t>
+  </si>
+  <si>
+    <t>-875</t>
+  </si>
+  <si>
+    <t>22920-33600</t>
+  </si>
+  <si>
+    <t>4120-4360</t>
+  </si>
+  <si>
+    <t>21500-21770 24650-26450 26730-</t>
+  </si>
+  <si>
+    <t>-5650</t>
+  </si>
+  <si>
+    <t>-1235</t>
+  </si>
+  <si>
+    <t>needs rescaling</t>
+  </si>
+  <si>
+    <t>2330-</t>
+  </si>
+  <si>
+    <t>1160-</t>
+  </si>
+  <si>
+    <t>-1855</t>
+  </si>
+  <si>
+    <t>-1020 2710-3990</t>
+  </si>
+  <si>
+    <t>-1975</t>
+  </si>
+  <si>
+    <t>5740-</t>
+  </si>
+  <si>
+    <t>370-850 1755-5670</t>
+  </si>
+  <si>
+    <t>2040-</t>
+  </si>
+  <si>
+    <t>-800</t>
+  </si>
+  <si>
+    <t>-260 480-</t>
+  </si>
+  <si>
+    <t>5595-</t>
+  </si>
+  <si>
+    <t>-870 1785-</t>
+  </si>
+  <si>
+    <t>-3930</t>
+  </si>
+  <si>
+    <t>-2700 4040-7200</t>
+  </si>
+  <si>
+    <t>2815-3465 3500-</t>
+  </si>
+  <si>
+    <t>-2295</t>
+  </si>
+  <si>
+    <t>1470-2935</t>
   </si>
 </sst>
 </file>
@@ -1822,7 +1984,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1832,6 +1994,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1848,7 +2022,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -1858,6 +2032,12 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2172,24 +2352,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
-  <dimension ref="A1:H194"/>
+  <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D22" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H34" sqref="H34"/>
+    <sheetView tabSelected="1" topLeftCell="D62" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I92" sqref="I92"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="20.42578125" customWidth="1"/>
     <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="4.36328125" customWidth="1"/>
-    <col min="4" max="4" width="18.54296875" customWidth="1"/>
-    <col min="5" max="5" width="20.08984375" customWidth="1"/>
-    <col min="6" max="7" width="16.36328125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="9.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="4.42578125" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" customWidth="1"/>
+    <col min="6" max="7" width="16.42578125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="9.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>191</v>
       </c>
@@ -2214,8 +2395,11 @@
       <c r="H1" s="3" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" s="3" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>191</v>
       </c>
@@ -2240,8 +2424,11 @@
       <c r="H2" s="3" t="s">
         <v>506</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I2" s="3" t="s">
+        <v>593</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2260,8 +2447,11 @@
       <c r="H3" s="4" t="s">
         <v>508</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="I3" s="3" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -2274,8 +2464,9 @@
       <c r="F4" s="5"/>
       <c r="G4" s="5"/>
       <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I4" s="5"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2300,25 +2491,33 @@
       <c r="H5" s="4" t="s">
         <v>509</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="I5" s="3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
-        <v>193</v>
-      </c>
-      <c r="C6" t="s">
-        <v>201</v>
-      </c>
-      <c r="E6" t="s">
+      <c r="B6" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E6" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="H6" s="10" t="s">
         <v>510</v>
       </c>
-    </row>
-    <row r="7" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="I6" s="10" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -2331,8 +2530,9 @@
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
       <c r="H7" s="5"/>
-    </row>
-    <row r="8" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="I7" s="5"/>
+    </row>
+    <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>305</v>
       </c>
@@ -2347,8 +2547,9 @@
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
-    </row>
-    <row r="9" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="I8" s="5"/>
+    </row>
+    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -2361,8 +2562,9 @@
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
       <c r="H9" s="5"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I9" s="5"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -2382,7 +2584,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -2399,7 +2601,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2419,7 +2621,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="13" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -2432,8 +2634,9 @@
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
       <c r="H13" s="5"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I13" s="5"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -2458,8 +2661,11 @@
       <c r="H14" s="4" t="s">
         <v>513</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I14" s="3" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -2482,7 +2688,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="16" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
@@ -2495,8 +2701,9 @@
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
       <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I16" s="5"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -2519,7 +2726,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>14</v>
       </c>
@@ -2542,7 +2749,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="19" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>15</v>
       </c>
@@ -2555,8 +2762,9 @@
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
       <c r="H19" s="5"/>
-    </row>
-    <row r="20" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="I19" s="5"/>
+    </row>
+    <row r="20" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>16</v>
       </c>
@@ -2571,8 +2779,9 @@
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I20" s="5"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>17</v>
       </c>
@@ -2592,7 +2801,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>18</v>
       </c>
@@ -2611,8 +2820,11 @@
       <c r="H22" s="3" t="s">
         <v>341</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I22" s="3">
+        <v>-1263</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>19</v>
       </c>
@@ -2628,8 +2840,11 @@
       <c r="H23" s="3" t="s">
         <v>310</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I23" s="3" t="s">
+        <v>597</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>20</v>
       </c>
@@ -2645,8 +2860,11 @@
       <c r="G24" s="3" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I24" s="3" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>21</v>
       </c>
@@ -2671,8 +2889,11 @@
       <c r="H25" s="3" t="s">
         <v>517</v>
       </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I25" s="3" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>22</v>
       </c>
@@ -2691,8 +2912,11 @@
       <c r="H26" s="3" t="s">
         <v>518</v>
       </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I26" s="4" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>23</v>
       </c>
@@ -2708,28 +2932,35 @@
       <c r="G27" s="3" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
+      <c r="I27" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="B28" t="s">
-        <v>193</v>
-      </c>
-      <c r="C28" t="s">
-        <v>201</v>
-      </c>
-      <c r="E28" t="s">
+      <c r="B28" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C28" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E28" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="G28" s="3" t="s">
+      <c r="F28" s="10"/>
+      <c r="G28" s="10" t="s">
         <v>344</v>
       </c>
-      <c r="H28" s="3" t="s">
+      <c r="H28" s="10" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="I28" s="10" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>25</v>
       </c>
@@ -2745,8 +2976,9 @@
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
       <c r="H29" s="5"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I29" s="5"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -2768,8 +3000,11 @@
       <c r="H30" s="3" t="s">
         <v>519</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I30" s="3">
+        <v>-7120</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>27</v>
       </c>
@@ -2792,7 +3027,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>28</v>
       </c>
@@ -2814,8 +3049,11 @@
       <c r="H32" s="3" t="s">
         <v>520</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I32" s="4" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>29</v>
       </c>
@@ -2838,7 +3076,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -2861,7 +3099,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>31</v>
       </c>
@@ -2883,25 +3121,33 @@
       <c r="H35" s="3" t="s">
         <v>316</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
+      <c r="I35" s="3" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="B36" t="s">
-        <v>193</v>
-      </c>
-      <c r="C36" t="s">
-        <v>201</v>
-      </c>
-      <c r="E36" t="s">
+      <c r="B36" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C36" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E36" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="H36" s="3" t="s">
+      <c r="F36" s="10"/>
+      <c r="G36" s="10"/>
+      <c r="H36" s="10" t="s">
         <v>317</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I36" s="10" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>33</v>
       </c>
@@ -2920,8 +3166,11 @@
       <c r="H37" s="3" t="s">
         <v>521</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I37" s="3" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>34</v>
       </c>
@@ -2937,8 +3186,11 @@
       <c r="G38" s="3" t="s">
         <v>354</v>
       </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I38" s="3" t="s">
+        <v>605</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>35</v>
       </c>
@@ -2957,8 +3209,11 @@
       <c r="F39" s="3">
         <v>-1815</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I39" s="3" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>36</v>
       </c>
@@ -2983,28 +3238,35 @@
       <c r="H40" s="3" t="s">
         <v>522</v>
       </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A41" t="s">
+      <c r="I40" s="4" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B41" t="s">
-        <v>193</v>
-      </c>
-      <c r="C41" t="s">
+      <c r="B41" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C41" s="9" t="s">
         <v>198</v>
       </c>
-      <c r="E41" t="s">
+      <c r="E41" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="F41" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="G41" s="3" t="s">
+      <c r="G41" s="10" t="s">
         <v>356</v>
       </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H41" s="10"/>
+      <c r="I41" s="10" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>38</v>
       </c>
@@ -3026,8 +3288,11 @@
       <c r="H42" s="3" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I42" s="3" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>39</v>
       </c>
@@ -3049,8 +3314,11 @@
       <c r="H43" s="3" t="s">
         <v>523</v>
       </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I43" s="3" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>40</v>
       </c>
@@ -3069,8 +3337,11 @@
       <c r="G44" s="4" t="s">
         <v>524</v>
       </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I44" s="3" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>41</v>
       </c>
@@ -3089,8 +3360,11 @@
       <c r="H45" s="3" t="s">
         <v>318</v>
       </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I45" s="3" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>42</v>
       </c>
@@ -3110,7 +3384,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>43</v>
       </c>
@@ -3127,7 +3401,7 @@
         <v>-625</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>44</v>
       </c>
@@ -3149,8 +3423,11 @@
       <c r="H48" s="3" t="s">
         <v>525</v>
       </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I48" s="3" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>45</v>
       </c>
@@ -3172,22 +3449,31 @@
       <c r="H49" s="3" t="s">
         <v>526</v>
       </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A50" t="s">
+      <c r="I49" s="3" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B50" t="s">
-        <v>193</v>
-      </c>
-      <c r="C50" t="s">
-        <v>201</v>
-      </c>
-      <c r="E50" t="s">
+      <c r="B50" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C50" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E50" s="9" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="F50" s="10"/>
+      <c r="G50" s="10"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="10" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>47</v>
       </c>
@@ -3203,8 +3489,11 @@
       <c r="H51" s="3" t="s">
         <v>527</v>
       </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I51" s="3" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>48</v>
       </c>
@@ -3227,7 +3516,7 @@
         <v>528</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>49</v>
       </c>
@@ -3250,27 +3539,31 @@
         <v>529</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A54" t="s">
+    <row r="54" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="B54" t="s">
-        <v>193</v>
-      </c>
-      <c r="C54" t="s">
-        <v>201</v>
-      </c>
-      <c r="E54" t="s">
+      <c r="B54" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C54" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E54" s="9" t="s">
         <v>50</v>
       </c>
-      <c r="F54" s="4" t="s">
+      <c r="F54" s="11" t="s">
         <v>460</v>
       </c>
-      <c r="G54" s="4" t="s">
+      <c r="G54" s="11" t="s">
         <v>363</v>
       </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="H54" s="10"/>
+      <c r="I54" s="10" t="s">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>51</v>
       </c>
@@ -3290,8 +3583,11 @@
       <c r="H55" s="3" t="s">
         <v>321</v>
       </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I55" s="3" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>52</v>
       </c>
@@ -3313,8 +3609,11 @@
       <c r="H56" s="3" t="s">
         <v>530</v>
       </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I56" s="3" t="s">
+        <v>618</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>53</v>
       </c>
@@ -3336,8 +3635,11 @@
       <c r="H57" s="3" t="s">
         <v>323</v>
       </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I57" s="3" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>54</v>
       </c>
@@ -3354,7 +3656,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>55</v>
       </c>
@@ -3372,7 +3674,7 @@
       </c>
       <c r="G59" s="4"/>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>56</v>
       </c>
@@ -3391,8 +3693,11 @@
       <c r="H60" s="3" t="s">
         <v>365</v>
       </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I60" s="3" t="s">
+        <v>620</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>57</v>
       </c>
@@ -3411,8 +3716,11 @@
       <c r="H61" s="3" t="s">
         <v>531</v>
       </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I61" s="3" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>58</v>
       </c>
@@ -3434,8 +3742,11 @@
       <c r="H62" s="3" t="s">
         <v>324</v>
       </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I62" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>59</v>
       </c>
@@ -3457,8 +3768,11 @@
       <c r="H63" s="3" t="s">
         <v>590</v>
       </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I63" s="3" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>60</v>
       </c>
@@ -3480,8 +3794,11 @@
       <c r="H64" s="3" t="s">
         <v>532</v>
       </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I64" s="3" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>61</v>
       </c>
@@ -3506,8 +3823,11 @@
       <c r="H65" s="3" t="s">
         <v>326</v>
       </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I65" s="3" t="s">
+        <v>625</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>62</v>
       </c>
@@ -3526,8 +3846,11 @@
       <c r="H66" s="3" t="s">
         <v>327</v>
       </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I66" s="3" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>63</v>
       </c>
@@ -3546,31 +3869,37 @@
       <c r="H67" s="3" t="s">
         <v>533</v>
       </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A68" t="s">
+      <c r="I67" s="3" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="B68" t="s">
-        <v>193</v>
-      </c>
-      <c r="C68" t="s">
-        <v>201</v>
-      </c>
-      <c r="E68" t="s">
+      <c r="B68" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="C68" s="12" t="s">
+        <v>201</v>
+      </c>
+      <c r="E68" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="F68" s="3" t="s">
+      <c r="F68" s="13" t="s">
         <v>248</v>
       </c>
-      <c r="G68" s="3" t="s">
+      <c r="G68" s="13" t="s">
         <v>372</v>
       </c>
-      <c r="H68" s="3" t="s">
+      <c r="H68" s="13" t="s">
         <v>311</v>
       </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I68" s="13" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>65</v>
       </c>
@@ -3592,39 +3921,53 @@
       <c r="H69" s="3" t="s">
         <v>534</v>
       </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A70" t="s">
+      <c r="I69" s="3" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="B70" t="s">
-        <v>193</v>
-      </c>
-      <c r="C70" t="s">
-        <v>201</v>
-      </c>
-      <c r="E70" t="s">
+      <c r="B70" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C70" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E70" s="9" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A71" t="s">
+      <c r="F70" s="10"/>
+      <c r="G70" s="10"/>
+      <c r="H70" s="10"/>
+      <c r="I70" s="10" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="B71" t="s">
-        <v>193</v>
-      </c>
-      <c r="C71" t="s">
-        <v>201</v>
-      </c>
-      <c r="E71" t="s">
+      <c r="B71" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C71" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E71" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="F71" s="3" t="s">
+      <c r="F71" s="10" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G71" s="10"/>
+      <c r="H71" s="10"/>
+      <c r="I71" s="10" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>68</v>
       </c>
@@ -3643,31 +3986,37 @@
       <c r="H72" s="3" t="s">
         <v>535</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A73" t="s">
+      <c r="I72" s="3" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="B73" t="s">
-        <v>193</v>
-      </c>
-      <c r="C73" t="s">
-        <v>201</v>
-      </c>
-      <c r="E73" t="s">
+      <c r="B73" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E73" s="9" t="s">
         <v>69</v>
       </c>
-      <c r="F73" s="3">
+      <c r="F73" s="10">
         <v>-610</v>
       </c>
-      <c r="G73" s="3" t="s">
+      <c r="G73" s="10" t="s">
         <v>374</v>
       </c>
-      <c r="H73" s="3" t="s">
+      <c r="H73" s="10" t="s">
         <v>330</v>
       </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I73" s="10" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>70</v>
       </c>
@@ -3683,8 +4032,11 @@
       <c r="H74" s="3" t="s">
         <v>536</v>
       </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I74" s="3" t="s">
+        <v>631</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>71</v>
       </c>
@@ -3706,8 +4058,11 @@
       <c r="H75" s="3" t="s">
         <v>375</v>
       </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I75" s="3" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>72</v>
       </c>
@@ -3727,7 +4082,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>73</v>
       </c>
@@ -3740,8 +4095,11 @@
       <c r="E77" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I77" s="3" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>74</v>
       </c>
@@ -3766,8 +4124,11 @@
       <c r="H78" s="3" t="s">
         <v>537</v>
       </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I78" s="3" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>75</v>
       </c>
@@ -3789,8 +4150,11 @@
       <c r="H79" s="3" t="s">
         <v>331</v>
       </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I79" s="3" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>76</v>
       </c>
@@ -3812,8 +4176,11 @@
       <c r="H80" s="3" t="s">
         <v>538</v>
       </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I80" s="3" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>77</v>
       </c>
@@ -3829,8 +4196,11 @@
       <c r="G81" s="3" t="s">
         <v>382</v>
       </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I81" s="3" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>78</v>
       </c>
@@ -3852,8 +4222,11 @@
       <c r="H82" s="3" t="s">
         <v>539</v>
       </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I82" s="3" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>79</v>
       </c>
@@ -3869,8 +4242,11 @@
       <c r="F83" s="3" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I83" s="3" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>80</v>
       </c>
@@ -3883,8 +4259,11 @@
       <c r="E84" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I84" s="3" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>81</v>
       </c>
@@ -3900,8 +4279,11 @@
       <c r="G85" s="3" t="s">
         <v>384</v>
       </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I85" s="3" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>82</v>
       </c>
@@ -3926,8 +4308,11 @@
       <c r="H86" s="3" t="s">
         <v>540</v>
       </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I86" s="3" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>83</v>
       </c>
@@ -3949,26 +4334,33 @@
       <c r="H87" s="3" t="s">
         <v>541</v>
       </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A88" t="s">
+      <c r="I87" s="14" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B88" t="s">
-        <v>193</v>
-      </c>
-      <c r="C88" t="s">
-        <v>201</v>
-      </c>
-      <c r="E88" t="s">
+      <c r="B88" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C88" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E88" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="F88" s="4" t="s">
+      <c r="F88" s="11" t="s">
         <v>465</v>
       </c>
-      <c r="G88" s="4"/>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G88" s="11"/>
+      <c r="H88" s="10"/>
+      <c r="I88" s="10" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>85</v>
       </c>
@@ -3987,8 +4379,11 @@
       <c r="H89" s="3" t="s">
         <v>542</v>
       </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I89" s="3" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>86</v>
       </c>
@@ -4010,31 +4405,37 @@
       <c r="H90" s="3" t="s">
         <v>543</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A91" t="s">
+      <c r="I90" s="3" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B91" t="s">
-        <v>193</v>
-      </c>
-      <c r="C91" t="s">
-        <v>201</v>
-      </c>
-      <c r="E91" t="s">
+      <c r="B91" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C91" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="E91" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="F91" s="4" t="s">
+      <c r="F91" s="11" t="s">
         <v>466</v>
       </c>
-      <c r="G91" s="4" t="s">
+      <c r="G91" s="11" t="s">
         <v>320</v>
       </c>
-      <c r="H91" s="3" t="s">
+      <c r="H91" s="10" t="s">
         <v>544</v>
       </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I91" s="10" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>88</v>
       </c>
@@ -4051,7 +4452,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>89</v>
       </c>
@@ -4071,7 +4472,7 @@
         <v>546</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>90</v>
       </c>
@@ -4091,7 +4492,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>91</v>
       </c>
@@ -4111,7 +4512,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>92</v>
       </c>
@@ -4128,7 +4529,7 @@
         <v>392</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>93</v>
       </c>
@@ -4145,7 +4546,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>94</v>
       </c>
@@ -4162,7 +4563,7 @@
         <v>393</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>95</v>
       </c>
@@ -4182,7 +4583,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>96</v>
       </c>
@@ -4205,7 +4606,7 @@
         <v>548</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>97</v>
       </c>
@@ -4222,7 +4623,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>98</v>
       </c>
@@ -4239,7 +4640,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>99</v>
       </c>
@@ -4256,7 +4657,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>100</v>
       </c>
@@ -4279,7 +4680,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>101</v>
       </c>
@@ -4296,7 +4697,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="106" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>102</v>
       </c>
@@ -4309,8 +4710,9 @@
       <c r="F106" s="5"/>
       <c r="G106" s="5"/>
       <c r="H106" s="5"/>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I106" s="5"/>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>103</v>
       </c>
@@ -4330,7 +4732,7 @@
         <v>549</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>104</v>
       </c>
@@ -4350,7 +4752,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>105</v>
       </c>
@@ -4373,7 +4775,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>106</v>
       </c>
@@ -4393,7 +4795,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>107</v>
       </c>
@@ -4413,7 +4815,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>108</v>
       </c>
@@ -4430,7 +4832,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>109</v>
       </c>
@@ -4447,7 +4849,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>110</v>
       </c>
@@ -4467,7 +4869,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>111</v>
       </c>
@@ -4490,7 +4892,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>112</v>
       </c>
@@ -4510,7 +4912,7 @@
         <v>325</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>113</v>
       </c>
@@ -4533,7 +4935,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>114</v>
       </c>
@@ -4553,7 +4955,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>115</v>
       </c>
@@ -4579,7 +4981,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>116</v>
       </c>
@@ -4599,7 +5001,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>117</v>
       </c>
@@ -4616,7 +5018,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>118</v>
       </c>
@@ -4636,7 +5038,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>119</v>
       </c>
@@ -4656,7 +5058,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>120</v>
       </c>
@@ -4673,7 +5075,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>121</v>
       </c>
@@ -4690,7 +5092,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>122</v>
       </c>
@@ -4707,7 +5109,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>123</v>
       </c>
@@ -4730,7 +5132,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>124</v>
       </c>
@@ -4747,7 +5149,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>125</v>
       </c>
@@ -4764,7 +5166,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>126</v>
       </c>
@@ -4781,7 +5183,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="131" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>127</v>
       </c>
@@ -4794,8 +5196,9 @@
       <c r="F131" s="5"/>
       <c r="G131" s="5"/>
       <c r="H131" s="5"/>
-    </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I131" s="5"/>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>128</v>
       </c>
@@ -4815,7 +5218,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>129</v>
       </c>
@@ -4838,7 +5241,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>130</v>
       </c>
@@ -4861,7 +5264,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>131</v>
       </c>
@@ -4881,7 +5284,7 @@
         <v>420</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>132</v>
       </c>
@@ -4901,7 +5304,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>133</v>
       </c>
@@ -4924,7 +5327,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>134</v>
       </c>
@@ -4947,7 +5350,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>135</v>
       </c>
@@ -4961,7 +5364,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>136</v>
       </c>
@@ -4984,7 +5387,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>137</v>
       </c>
@@ -5004,7 +5407,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>138</v>
       </c>
@@ -5021,7 +5424,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>139</v>
       </c>
@@ -5038,7 +5441,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>140</v>
       </c>
@@ -5061,7 +5464,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>141</v>
       </c>
@@ -5078,7 +5481,7 @@
         <v>-1600</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>142</v>
       </c>
@@ -5101,7 +5504,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>143</v>
       </c>
@@ -5121,7 +5524,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>144</v>
       </c>
@@ -5141,7 +5544,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>145</v>
       </c>
@@ -5161,7 +5564,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>146</v>
       </c>
@@ -5178,7 +5581,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>147</v>
       </c>
@@ -5192,7 +5595,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>148</v>
       </c>
@@ -5212,7 +5615,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>149</v>
       </c>
@@ -5235,7 +5638,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>150</v>
       </c>
@@ -5252,7 +5655,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>151</v>
       </c>
@@ -5272,7 +5675,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>152</v>
       </c>
@@ -5289,7 +5692,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>153</v>
       </c>
@@ -5306,7 +5709,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>154</v>
       </c>
@@ -5323,7 +5726,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>155</v>
       </c>
@@ -5346,7 +5749,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>156</v>
       </c>
@@ -5369,7 +5772,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>157</v>
       </c>
@@ -5389,7 +5792,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>158</v>
       </c>
@@ -5412,7 +5815,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>159</v>
       </c>
@@ -5432,7 +5835,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>160</v>
       </c>
@@ -5452,7 +5855,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="165" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="165" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>161</v>
       </c>
@@ -5468,8 +5871,9 @@
       <c r="F165" s="5"/>
       <c r="G165" s="5"/>
       <c r="H165" s="5"/>
-    </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I165" s="5"/>
+    </row>
+    <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>162</v>
       </c>
@@ -5486,7 +5890,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>163</v>
       </c>
@@ -5506,7 +5910,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>164</v>
       </c>
@@ -5526,7 +5930,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>165</v>
       </c>
@@ -5543,7 +5947,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>166</v>
       </c>
@@ -5560,7 +5964,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="171" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="171" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A171" s="2" t="s">
         <v>167</v>
       </c>
@@ -5576,8 +5980,9 @@
       <c r="F171" s="5"/>
       <c r="G171" s="5"/>
       <c r="H171" s="5"/>
-    </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I171" s="5"/>
+    </row>
+    <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>168</v>
       </c>
@@ -5600,7 +6005,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>169</v>
       </c>
@@ -5623,7 +6028,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>170</v>
       </c>
@@ -5640,7 +6045,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>171</v>
       </c>
@@ -5657,7 +6062,7 @@
         <v>286</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>172</v>
       </c>
@@ -5677,7 +6082,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="177" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>173</v>
       </c>
@@ -5697,7 +6102,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="178" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>174</v>
       </c>
@@ -5723,7 +6128,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="179" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>175</v>
       </c>
@@ -5740,7 +6145,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="180" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>176</v>
       </c>
@@ -5763,7 +6168,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="181" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>177</v>
       </c>
@@ -5786,7 +6191,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="182" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>178</v>
       </c>
@@ -5803,7 +6208,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="183" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>179</v>
       </c>
@@ -5823,7 +6228,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="184" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>180</v>
       </c>
@@ -5840,7 +6245,7 @@
         <v>290</v>
       </c>
     </row>
-    <row r="185" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>181</v>
       </c>
@@ -5857,7 +6262,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="186" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>182</v>
       </c>
@@ -5874,7 +6279,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="187" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>183</v>
       </c>
@@ -5897,7 +6302,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="188" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>184</v>
       </c>
@@ -5917,7 +6322,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="189" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>185</v>
       </c>
@@ -5940,7 +6345,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="190" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>186</v>
       </c>
@@ -5963,7 +6368,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="191" spans="1:8" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="191" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
         <v>187</v>
       </c>
@@ -5981,8 +6386,9 @@
       </c>
       <c r="G191" s="5"/>
       <c r="H191" s="5"/>
-    </row>
-    <row r="192" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I191" s="5"/>
+    </row>
+    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>188</v>
       </c>
@@ -6002,7 +6408,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>189</v>
       </c>
@@ -6022,7 +6428,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>190</v>
       </c>

</xml_diff>

<commit_message>
Ending 2017 dry firn identification exclusions.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{217D0D81-2BF4-4EF1-9DF5-144A5098E2A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0F1F30-C698-4217-AC6C-6C3425510643}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3675" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1190" uniqueCount="646">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="678">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -621,9 +621,6 @@
     <t>No because of fail in surface identification, did not want to spend too much time on it knowing this region has been flown over in at leat one other 2017 date</t>
   </si>
   <si>
-    <t>Yes, -inf in data but replaces by NaNs, ok</t>
-  </si>
-  <si>
     <t>No, bad echo, even on images in CReSIS repository</t>
   </si>
   <si>
@@ -1239,9 +1236,6 @@
     <t>-1030 2810-3610 6570-6900 7920-8630</t>
   </si>
   <si>
-    <t>4390-</t>
-  </si>
-  <si>
     <t>-1570 4093-4170</t>
   </si>
   <si>
@@ -1269,9 +1263,6 @@
     <t>-40</t>
   </si>
   <si>
-    <t>2380-</t>
-  </si>
-  <si>
     <t>-530</t>
   </si>
   <si>
@@ -1830,9 +1821,6 @@
     <t>-2240 5980-</t>
   </si>
   <si>
-    <t>to delete</t>
-  </si>
-  <si>
     <t>-3960 5555-5620 15260-16100 16390-17100 23260-24360 27240-27350 29910-30560 31870-31940</t>
   </si>
   <si>
@@ -1851,9 +1839,6 @@
     <t>-610 3215-</t>
   </si>
   <si>
-    <t>to delete though slabs at the surface …</t>
-  </si>
-  <si>
     <t>-1440</t>
   </si>
   <si>
@@ -1875,9 +1860,6 @@
     <t>880-</t>
   </si>
   <si>
-    <t>to delete though slabs at the surface but signal too noisy</t>
-  </si>
-  <si>
     <t>1540-</t>
   </si>
   <si>
@@ -1911,9 +1893,6 @@
     <t>-1235</t>
   </si>
   <si>
-    <t>needs rescaling</t>
-  </si>
-  <si>
     <t>2330-</t>
   </si>
   <si>
@@ -1963,6 +1942,123 @@
   </si>
   <si>
     <t>1470-2935</t>
+  </si>
+  <si>
+    <t>-1280 1450-1870 2070-2545 3220-3380</t>
+  </si>
+  <si>
+    <t>3600-3800 4120-7340 8225-</t>
+  </si>
+  <si>
+    <t>-3130</t>
+  </si>
+  <si>
+    <t>8085-</t>
+  </si>
+  <si>
+    <t>-4090</t>
+  </si>
+  <si>
+    <t>1510-</t>
+  </si>
+  <si>
+    <t>-1670</t>
+  </si>
+  <si>
+    <t>2700-</t>
+  </si>
+  <si>
+    <t>-1750</t>
+  </si>
+  <si>
+    <t>3855-</t>
+  </si>
+  <si>
+    <t>-1280 1600-1760</t>
+  </si>
+  <si>
+    <t>3200-</t>
+  </si>
+  <si>
+    <t>5350-</t>
+  </si>
+  <si>
+    <t>2250-2870</t>
+  </si>
+  <si>
+    <t>5490-9045 9600-14320</t>
+  </si>
+  <si>
+    <t>10060-</t>
+  </si>
+  <si>
+    <t>-650 5015-5500 5665-5965 6740-7390 7685-8320 8480-</t>
+  </si>
+  <si>
+    <t>8960-9280 9570-</t>
+  </si>
+  <si>
+    <t>-1145 13500-17060 17630-21850</t>
+  </si>
+  <si>
+    <t>2660-</t>
+  </si>
+  <si>
+    <t>3020-3375 3780-3990 5530-6020 23460-</t>
+  </si>
+  <si>
+    <t>-645 835-1305</t>
+  </si>
+  <si>
+    <t>3770-</t>
+  </si>
+  <si>
+    <t>2900-</t>
+  </si>
+  <si>
+    <t>3520-</t>
+  </si>
+  <si>
+    <t>2950-</t>
+  </si>
+  <si>
+    <t>7410-</t>
+  </si>
+  <si>
+    <t>3600-</t>
+  </si>
+  <si>
+    <t>810-1115</t>
+  </si>
+  <si>
+    <t>1080-1440</t>
+  </si>
+  <si>
+    <t>2580-2675 4355-</t>
+  </si>
+  <si>
+    <t>5060-5800 6200-7700 8000-</t>
+  </si>
+  <si>
+    <t>-1410 1770-2330 7460-</t>
+  </si>
+  <si>
+    <t>-160 220-</t>
+  </si>
+  <si>
+    <t>-520 720-2105 2250-2805 2985-3600 4550-4960</t>
+  </si>
+  <si>
+    <t>-500 1480-1660</t>
+  </si>
+  <si>
+    <t>deleted after dry firn identification</t>
+  </si>
+  <si>
+    <t>deleted after dry firn identification though slabs at the surface …</t>
+  </si>
+  <si>
+    <t>Yes, -inf in data but replaces by NaNs, ok - deleted after dry firn identification though slabs at the surface …</t>
   </si>
 </sst>
 </file>
@@ -1984,7 +2080,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1994,18 +2090,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2022,7 +2106,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -2032,12 +2116,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2354,8 +2435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D62" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I92" sqref="I92"/>
+    <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I136" sqref="I136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2381,22 +2462,22 @@
         <v>196</v>
       </c>
       <c r="D1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="E1" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>592</v>
+        <v>589</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2407,25 +2488,25 @@
         <v>192</v>
       </c>
       <c r="C2" t="s">
+        <v>499</v>
+      </c>
+      <c r="D2" t="s">
+        <v>500</v>
+      </c>
+      <c r="E2" t="s">
+        <v>465</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>502</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" s="3" t="s">
         <v>503</v>
       </c>
-      <c r="E2" t="s">
-        <v>468</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>506</v>
-      </c>
       <c r="I2" s="3" t="s">
-        <v>593</v>
+        <v>590</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2436,19 +2517,19 @@
         <v>193</v>
       </c>
       <c r="C3" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E3" t="s">
         <v>0</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>594</v>
+        <v>591</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2474,47 +2555,41 @@
         <v>193</v>
       </c>
       <c r="C5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E5" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="G5" s="3">
         <v>-910</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>595</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="9" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C6" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E6" s="9" t="s">
-        <v>3</v>
-      </c>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10" t="s">
-        <v>510</v>
-      </c>
-      <c r="I6" s="10" t="s">
-        <v>601</v>
+      <c r="B6" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5" t="s">
+        <v>507</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2525,7 +2600,7 @@
         <v>194</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="F7" s="5"/>
       <c r="G7" s="5"/>
@@ -2534,16 +2609,16 @@
     </row>
     <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>194</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="5"/>
@@ -2557,7 +2632,7 @@
         <v>194</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="F9" s="5"/>
       <c r="G9" s="5"/>
@@ -2572,16 +2647,16 @@
         <v>194</v>
       </c>
       <c r="C10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E10" t="s">
         <v>6</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="H10" s="6" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
@@ -2592,13 +2667,13 @@
         <v>194</v>
       </c>
       <c r="C11" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E11" t="s">
         <v>7</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -2609,16 +2684,16 @@
         <v>194</v>
       </c>
       <c r="C12" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E12" t="s">
         <v>8</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
     </row>
     <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2629,7 +2704,7 @@
         <v>194</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="F13" s="5"/>
       <c r="G13" s="5"/>
@@ -2644,25 +2719,25 @@
         <v>194</v>
       </c>
       <c r="C14" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D14" t="s">
+        <v>298</v>
+      </c>
+      <c r="E14" t="s">
+        <v>467</v>
+      </c>
+      <c r="F14" s="3" t="s">
         <v>299</v>
       </c>
-      <c r="E14" t="s">
-        <v>470</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>300</v>
-      </c>
       <c r="G14" s="3" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="H14" s="4" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>596</v>
+        <v>593</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2673,19 +2748,19 @@
         <v>194</v>
       </c>
       <c r="C15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
     </row>
     <row r="16" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2696,7 +2771,7 @@
         <v>194</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="F16" s="5"/>
       <c r="G16" s="5"/>
@@ -2711,19 +2786,19 @@
         <v>194</v>
       </c>
       <c r="C17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E17" t="s">
         <v>13</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -2734,19 +2809,19 @@
         <v>194</v>
       </c>
       <c r="C18" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E18" t="s">
         <v>14</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2757,7 +2832,7 @@
         <v>194</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
@@ -2772,7 +2847,7 @@
         <v>194</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="F20" s="5">
         <v>-640</v>
@@ -2789,16 +2864,16 @@
         <v>193</v>
       </c>
       <c r="C21" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E21" t="s">
         <v>17</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2809,16 +2884,16 @@
         <v>193</v>
       </c>
       <c r="C22" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E22" t="s">
         <v>18</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="I22" s="3">
         <v>-1263</v>
@@ -2832,16 +2907,16 @@
         <v>193</v>
       </c>
       <c r="C23" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E23" t="s">
         <v>19</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>597</v>
+        <v>594</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -2852,16 +2927,16 @@
         <v>193</v>
       </c>
       <c r="C24" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E24" t="s">
         <v>20</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>598</v>
+        <v>595</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2872,25 +2947,25 @@
         <v>193</v>
       </c>
       <c r="C25" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D25" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E25" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2901,19 +2976,19 @@
         <v>193</v>
       </c>
       <c r="C26" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D26" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="E26" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2924,40 +2999,34 @@
         <v>193</v>
       </c>
       <c r="C27" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E27" t="s">
         <v>23</v>
       </c>
       <c r="G27" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C28" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="H28" s="5" t="s">
         <v>312</v>
-      </c>
-      <c r="I27" s="3" t="s">
-        <v>341</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C28" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E28" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="F28" s="10"/>
-      <c r="G28" s="10" t="s">
-        <v>344</v>
-      </c>
-      <c r="H28" s="10" t="s">
-        <v>313</v>
-      </c>
-      <c r="I28" s="10" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2968,10 +3037,10 @@
         <v>193</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
@@ -2986,19 +3055,19 @@
         <v>193</v>
       </c>
       <c r="C30" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E30" t="s">
         <v>26</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="I30" s="3">
         <v>-7120</v>
@@ -3012,19 +3081,19 @@
         <v>193</v>
       </c>
       <c r="C31" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E31" t="s">
         <v>27</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -3035,22 +3104,22 @@
         <v>193</v>
       </c>
       <c r="C32" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E32" t="s">
         <v>28</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3061,19 +3130,19 @@
         <v>193</v>
       </c>
       <c r="C33" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E33" t="s">
         <v>29</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
@@ -3084,19 +3153,19 @@
         <v>193</v>
       </c>
       <c r="C34" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E34" t="s">
         <v>30</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>591</v>
+        <v>588</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -3107,44 +3176,38 @@
         <v>193</v>
       </c>
       <c r="C35" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E35" t="s">
         <v>31</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="H35" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C36" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
+      <c r="H36" s="5" t="s">
         <v>316</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>603</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B36" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C36" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E36" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="F36" s="10"/>
-      <c r="G36" s="10"/>
-      <c r="H36" s="10" t="s">
-        <v>317</v>
-      </c>
-      <c r="I36" s="10" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -3155,19 +3218,19 @@
         <v>193</v>
       </c>
       <c r="C37" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E37" t="s">
         <v>33</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>604</v>
+        <v>600</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -3178,16 +3241,16 @@
         <v>193</v>
       </c>
       <c r="C38" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E38" t="s">
         <v>34</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -3198,19 +3261,19 @@
         <v>193</v>
       </c>
       <c r="C39" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D39" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="E39" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="F39" s="3">
         <v>-1815</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -3221,50 +3284,45 @@
         <v>193</v>
       </c>
       <c r="C40" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D40" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E40" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="F40" s="3">
         <v>-375</v>
       </c>
       <c r="G40" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>519</v>
+      </c>
+      <c r="I40" s="4" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>677</v>
+      </c>
+      <c r="F41" s="5" t="s">
+        <v>240</v>
+      </c>
+      <c r="G41" s="5" t="s">
         <v>355</v>
       </c>
-      <c r="H40" s="3" t="s">
-        <v>522</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>607</v>
-      </c>
-    </row>
-    <row r="41" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B41" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C41" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>241</v>
-      </c>
-      <c r="G41" s="10" t="s">
-        <v>356</v>
-      </c>
-      <c r="H41" s="10"/>
-      <c r="I41" s="10" t="s">
-        <v>608</v>
-      </c>
+      <c r="H41" s="5"/>
+      <c r="I41" s="5"/>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
@@ -3274,22 +3332,22 @@
         <v>193</v>
       </c>
       <c r="C42" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E42" t="s">
         <v>38</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>609</v>
+        <v>604</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3300,22 +3358,22 @@
         <v>193</v>
       </c>
       <c r="C43" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E43" t="s">
         <v>39</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>610</v>
+        <v>605</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3326,19 +3384,19 @@
         <v>193</v>
       </c>
       <c r="C44" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E44" t="s">
         <v>40</v>
       </c>
       <c r="F44" s="4" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>611</v>
+        <v>606</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3349,19 +3407,19 @@
         <v>193</v>
       </c>
       <c r="C45" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E45" t="s">
         <v>41</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>612</v>
+        <v>607</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -3372,7 +3430,7 @@
         <v>193</v>
       </c>
       <c r="C46" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E46" t="s">
         <v>42</v>
@@ -3381,7 +3439,7 @@
         <v>-1840</v>
       </c>
       <c r="G46" s="4" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -3392,7 +3450,7 @@
         <v>193</v>
       </c>
       <c r="C47" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E47" t="s">
         <v>43</v>
@@ -3409,22 +3467,22 @@
         <v>193</v>
       </c>
       <c r="C48" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E48" t="s">
         <v>44</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>613</v>
+        <v>608</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3435,43 +3493,37 @@
         <v>193</v>
       </c>
       <c r="C49" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E49" t="s">
         <v>45</v>
       </c>
       <c r="F49" s="4" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="H49" s="3" t="s">
-        <v>526</v>
+        <v>523</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>614</v>
-      </c>
-    </row>
-    <row r="50" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="9" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B50" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C50" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E50" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="F50" s="10"/>
-      <c r="G50" s="10"/>
-      <c r="H50" s="10"/>
-      <c r="I50" s="10" t="s">
-        <v>601</v>
-      </c>
+      <c r="B50" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
+      <c r="H50" s="5"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -3481,16 +3533,16 @@
         <v>193</v>
       </c>
       <c r="C51" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E51" t="s">
         <v>47</v>
       </c>
       <c r="H51" s="3" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>615</v>
+        <v>610</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -3501,19 +3553,19 @@
         <v>193</v>
       </c>
       <c r="C52" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E52" t="s">
         <v>48</v>
       </c>
       <c r="F52" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="H52" s="3" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -3524,44 +3576,38 @@
         <v>193</v>
       </c>
       <c r="C53" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E53" t="s">
         <v>49</v>
       </c>
       <c r="F53" s="4" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="G53" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C54" s="5" t="s">
+        <v>676</v>
+      </c>
+      <c r="F54" s="11" t="s">
+        <v>457</v>
+      </c>
+      <c r="G54" s="11" t="s">
         <v>362</v>
       </c>
-      <c r="H53" s="3" t="s">
-        <v>529</v>
-      </c>
-    </row>
-    <row r="54" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="B54" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C54" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E54" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="F54" s="11" t="s">
-        <v>460</v>
-      </c>
-      <c r="G54" s="11" t="s">
-        <v>363</v>
-      </c>
-      <c r="H54" s="10"/>
-      <c r="I54" s="10" t="s">
-        <v>616</v>
-      </c>
+      <c r="H54" s="5"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
@@ -3571,20 +3617,20 @@
         <v>193</v>
       </c>
       <c r="C55" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E55" t="s">
         <v>51</v>
       </c>
       <c r="F55" s="4" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="G55" s="4"/>
       <c r="H55" s="3" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>617</v>
+        <v>611</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3595,22 +3641,22 @@
         <v>193</v>
       </c>
       <c r="C56" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E56" t="s">
         <v>52</v>
       </c>
       <c r="F56" s="4" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="H56" s="3" t="s">
-        <v>530</v>
+        <v>527</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>618</v>
+        <v>612</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3621,22 +3667,22 @@
         <v>193</v>
       </c>
       <c r="C57" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E57" t="s">
         <v>53</v>
       </c>
       <c r="F57" s="4" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="H57" s="3" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>619</v>
+        <v>613</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -3647,13 +3693,13 @@
         <v>193</v>
       </c>
       <c r="C58" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E58" t="s">
         <v>54</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -3664,13 +3710,13 @@
         <v>193</v>
       </c>
       <c r="C59" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E59" t="s">
         <v>55</v>
       </c>
       <c r="F59" s="4" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="G59" s="4"/>
     </row>
@@ -3682,19 +3728,19 @@
         <v>193</v>
       </c>
       <c r="C60" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E60" t="s">
         <v>56</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="H60" s="3" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>620</v>
+        <v>614</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3705,19 +3751,19 @@
         <v>193</v>
       </c>
       <c r="C61" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E61" t="s">
         <v>57</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="H61" s="3" t="s">
-        <v>531</v>
+        <v>528</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>621</v>
+        <v>615</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3728,22 +3774,22 @@
         <v>193</v>
       </c>
       <c r="C62" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D62" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E62" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
       <c r="F62" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>622</v>
+        <v>616</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3754,22 +3800,22 @@
         <v>193</v>
       </c>
       <c r="C63" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E63" t="s">
         <v>59</v>
       </c>
       <c r="F63" s="3" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>590</v>
+        <v>587</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>623</v>
+        <v>617</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3780,7 +3826,7 @@
         <v>193</v>
       </c>
       <c r="C64" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E64" t="s">
         <v>60</v>
@@ -3789,13 +3835,13 @@
         <v>-840</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>532</v>
+        <v>529</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>624</v>
+        <v>618</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3806,25 +3852,25 @@
         <v>193</v>
       </c>
       <c r="C65" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D65" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="E65" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="F65" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H65" s="3" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>625</v>
+        <v>619</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3835,19 +3881,19 @@
         <v>193</v>
       </c>
       <c r="C66" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D66" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E66" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="H66" s="3" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>626</v>
+        <v>620</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3858,46 +3904,44 @@
         <v>193</v>
       </c>
       <c r="C67" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E67" t="s">
         <v>63</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="H67" s="3" t="s">
-        <v>533</v>
+        <v>530</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" s="12" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="12" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="B68" s="12" t="s">
-        <v>193</v>
-      </c>
-      <c r="C68" s="12" t="s">
-        <v>201</v>
-      </c>
-      <c r="E68" s="12" t="s">
+      <c r="B68" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C68" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="E68" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="F68" s="13" t="s">
-        <v>248</v>
-      </c>
-      <c r="G68" s="13" t="s">
-        <v>372</v>
-      </c>
-      <c r="H68" s="13" t="s">
-        <v>311</v>
-      </c>
-      <c r="I68" s="13" t="s">
-        <v>628</v>
-      </c>
+      <c r="F68" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="G68" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="H68" s="6" t="s">
+        <v>310</v>
+      </c>
+      <c r="I68" s="6"/>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
@@ -3907,7 +3951,7 @@
         <v>193</v>
       </c>
       <c r="C69" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E69" t="s">
         <v>65</v>
@@ -3916,56 +3960,44 @@
         <v>-840</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H69" s="3" t="s">
-        <v>534</v>
+        <v>531</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="9" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="B70" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C70" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E70" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F70" s="10"/>
-      <c r="G70" s="10"/>
-      <c r="H70" s="10"/>
-      <c r="I70" s="10" t="s">
-        <v>601</v>
-      </c>
-    </row>
-    <row r="71" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="9" t="s">
+      <c r="B70" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="F70" s="5"/>
+      <c r="G70" s="5"/>
+      <c r="H70" s="5"/>
+    </row>
+    <row r="71" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B71" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C71" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E71" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="F71" s="10" t="s">
-        <v>249</v>
-      </c>
-      <c r="G71" s="10"/>
-      <c r="H71" s="10"/>
-      <c r="I71" s="10" t="s">
-        <v>601</v>
-      </c>
+      <c r="B71" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="F71" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="G71" s="5"/>
+      <c r="H71" s="5"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
@@ -3975,45 +4007,39 @@
         <v>193</v>
       </c>
       <c r="C72" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E72" t="s">
         <v>68</v>
       </c>
       <c r="G72" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>532</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>623</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B73" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="F73" s="5">
+        <v>-610</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="H73" s="5" t="s">
         <v>329</v>
-      </c>
-      <c r="H72" s="3" t="s">
-        <v>535</v>
-      </c>
-      <c r="I72" s="3" t="s">
-        <v>630</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="B73" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C73" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E73" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="F73" s="10">
-        <v>-610</v>
-      </c>
-      <c r="G73" s="10" t="s">
-        <v>374</v>
-      </c>
-      <c r="H73" s="10" t="s">
-        <v>330</v>
-      </c>
-      <c r="I73" s="10" t="s">
-        <v>601</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -4024,16 +4050,16 @@
         <v>193</v>
       </c>
       <c r="C74" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E74" t="s">
         <v>70</v>
       </c>
       <c r="H74" s="3" t="s">
-        <v>536</v>
+        <v>533</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>631</v>
+        <v>624</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -4044,22 +4070,22 @@
         <v>193</v>
       </c>
       <c r="C75" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E75" t="s">
         <v>71</v>
       </c>
       <c r="F75" s="4" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H75" s="3" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>632</v>
+        <v>625</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -4070,16 +4096,16 @@
         <v>193</v>
       </c>
       <c r="C76" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E76" t="s">
         <v>72</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H76" s="3" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -4090,13 +4116,13 @@
         <v>193</v>
       </c>
       <c r="C77" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E77" t="s">
         <v>73</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>633</v>
+        <v>626</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -4107,25 +4133,25 @@
         <v>193</v>
       </c>
       <c r="C78" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D78" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E78" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="F78" s="3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H78" s="3" t="s">
-        <v>537</v>
+        <v>534</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>634</v>
+        <v>627</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -4136,22 +4162,22 @@
         <v>193</v>
       </c>
       <c r="C79" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D79" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="E79" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H79" s="3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>635</v>
+        <v>628</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -4162,22 +4188,22 @@
         <v>193</v>
       </c>
       <c r="C80" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D80" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E80" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H80" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>636</v>
+        <v>629</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -4188,16 +4214,16 @@
         <v>193</v>
       </c>
       <c r="C81" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E81" t="s">
         <v>77</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>637</v>
+        <v>630</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -4208,22 +4234,22 @@
         <v>193</v>
       </c>
       <c r="C82" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D82" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E82" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H82" s="3" t="s">
-        <v>539</v>
+        <v>536</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>638</v>
+        <v>631</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -4234,16 +4260,16 @@
         <v>193</v>
       </c>
       <c r="C83" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E83" t="s">
         <v>79</v>
       </c>
       <c r="F83" s="3" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>639</v>
+        <v>632</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -4254,13 +4280,13 @@
         <v>193</v>
       </c>
       <c r="C84" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E84" t="s">
         <v>80</v>
       </c>
       <c r="I84" s="3" t="s">
-        <v>640</v>
+        <v>633</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -4271,16 +4297,16 @@
         <v>193</v>
       </c>
       <c r="C85" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E85" t="s">
         <v>81</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>641</v>
+        <v>634</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -4291,25 +4317,25 @@
         <v>193</v>
       </c>
       <c r="C86" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D86" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E86" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="F86" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="H86" s="3" t="s">
-        <v>540</v>
+        <v>537</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>642</v>
+        <v>635</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -4320,45 +4346,39 @@
         <v>193</v>
       </c>
       <c r="C87" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E87" t="s">
         <v>83</v>
       </c>
       <c r="F87" s="3" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H87" s="3" t="s">
-        <v>541</v>
-      </c>
-      <c r="I87" s="14" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="88" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A88" s="9" t="s">
+        <v>538</v>
+      </c>
+      <c r="I87" s="9" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A88" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="B88" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C88" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E88" s="9" t="s">
-        <v>84</v>
+      <c r="B88" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C88" s="5" t="s">
+        <v>675</v>
       </c>
       <c r="F88" s="11" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="G88" s="11"/>
-      <c r="H88" s="10"/>
-      <c r="I88" s="10" t="s">
-        <v>601</v>
-      </c>
+      <c r="H88" s="5"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
@@ -4368,19 +4388,19 @@
         <v>193</v>
       </c>
       <c r="C89" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E89" t="s">
         <v>85</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="H89" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>644</v>
+        <v>637</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -4391,7 +4411,7 @@
         <v>193</v>
       </c>
       <c r="C90" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E90" t="s">
         <v>86</v>
@@ -4400,39 +4420,33 @@
         <v>-750</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="H90" s="3" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="91" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="9" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B91" s="9" t="s">
-        <v>193</v>
-      </c>
-      <c r="C91" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="E91" s="9" t="s">
-        <v>87</v>
+      <c r="B91" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C91" s="5" t="s">
+        <v>675</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
       <c r="G91" s="11" t="s">
-        <v>320</v>
-      </c>
-      <c r="H91" s="10" t="s">
-        <v>544</v>
-      </c>
-      <c r="I91" s="10" t="s">
-        <v>601</v>
+        <v>319</v>
+      </c>
+      <c r="H91" s="5" t="s">
+        <v>541</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -4443,13 +4457,16 @@
         <v>193</v>
       </c>
       <c r="C92" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E92" t="s">
         <v>88</v>
       </c>
       <c r="H92" s="3" t="s">
-        <v>545</v>
+        <v>542</v>
+      </c>
+      <c r="I92" s="3" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -4460,16 +4477,19 @@
         <v>193</v>
       </c>
       <c r="C93" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E93" t="s">
         <v>89</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="H93" s="3" t="s">
-        <v>546</v>
+        <v>543</v>
+      </c>
+      <c r="I93" s="3" t="s">
+        <v>640</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -4480,16 +4500,19 @@
         <v>193</v>
       </c>
       <c r="C94" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E94" t="s">
         <v>90</v>
       </c>
       <c r="F94" s="3" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>390</v>
+        <v>389</v>
+      </c>
+      <c r="I94" s="3" t="s">
+        <v>641</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -4500,16 +4523,19 @@
         <v>193</v>
       </c>
       <c r="C95" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D95" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E95" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>391</v>
+        <v>390</v>
+      </c>
+      <c r="I95" s="3" t="s">
+        <v>642</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -4520,13 +4546,16 @@
         <v>193</v>
       </c>
       <c r="C96" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E96" t="s">
         <v>92</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>392</v>
+        <v>391</v>
+      </c>
+      <c r="I96" s="3" t="s">
+        <v>643</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -4537,13 +4566,16 @@
         <v>193</v>
       </c>
       <c r="C97" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E97" t="s">
         <v>93</v>
       </c>
       <c r="H97" s="3" t="s">
-        <v>547</v>
+        <v>544</v>
+      </c>
+      <c r="I97" s="3" t="s">
+        <v>644</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -4554,13 +4586,16 @@
         <v>193</v>
       </c>
       <c r="C98" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E98" t="s">
         <v>94</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>393</v>
+        <v>392</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>645</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -4571,16 +4606,19 @@
         <v>193</v>
       </c>
       <c r="C99" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E99" t="s">
         <v>95</v>
       </c>
       <c r="F99" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
+      </c>
+      <c r="I99" s="3" t="s">
+        <v>646</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -4591,19 +4629,22 @@
         <v>193</v>
       </c>
       <c r="C100" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D100" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="E100" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="F100" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="H100" s="3" t="s">
-        <v>548</v>
+        <v>545</v>
+      </c>
+      <c r="I100" s="3" t="s">
+        <v>647</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -4614,13 +4655,16 @@
         <v>193</v>
       </c>
       <c r="C101" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E101" t="s">
         <v>97</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
+      </c>
+      <c r="I101" s="3" t="s">
+        <v>648</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -4631,13 +4675,16 @@
         <v>193</v>
       </c>
       <c r="C102" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E102" t="s">
         <v>98</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>396</v>
+        <v>395</v>
+      </c>
+      <c r="I102" s="3" t="s">
+        <v>649</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -4648,13 +4695,16 @@
         <v>193</v>
       </c>
       <c r="C103" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D103" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E103" t="s">
-        <v>484</v>
+        <v>481</v>
+      </c>
+      <c r="I103" s="3" t="s">
+        <v>650</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -4665,19 +4715,22 @@
         <v>193</v>
       </c>
       <c r="C104" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D104" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="E104" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
       <c r="F104" s="3" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>397</v>
+        <v>396</v>
+      </c>
+      <c r="I104" s="3" t="s">
+        <v>312</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -4688,13 +4741,16 @@
         <v>193</v>
       </c>
       <c r="C105" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E105" t="s">
         <v>101</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>398</v>
+        <v>397</v>
+      </c>
+      <c r="I105" s="3" t="s">
+        <v>651</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4705,52 +4761,58 @@
         <v>193</v>
       </c>
       <c r="C106" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="F106" s="5"/>
       <c r="G106" s="5"/>
       <c r="H106" s="5"/>
       <c r="I106" s="5"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+    <row r="107" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="B107" t="s">
-        <v>193</v>
-      </c>
-      <c r="C107" t="s">
-        <v>201</v>
-      </c>
-      <c r="E107" t="s">
+      <c r="B107" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C107" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="E107" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="G107" s="3" t="s">
+      <c r="F107" s="6"/>
+      <c r="G107" s="6" t="s">
+        <v>398</v>
+      </c>
+      <c r="H107" s="6" t="s">
+        <v>546</v>
+      </c>
+      <c r="I107" s="6" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B108" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C108" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="E108" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="F108" s="6" t="s">
+        <v>257</v>
+      </c>
+      <c r="G108" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="H107" s="3" t="s">
-        <v>549</v>
-      </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
-        <v>104</v>
-      </c>
-      <c r="B108" t="s">
-        <v>193</v>
-      </c>
-      <c r="C108" t="s">
-        <v>201</v>
-      </c>
-      <c r="E108" t="s">
-        <v>104</v>
-      </c>
-      <c r="F108" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="G108" s="3" t="s">
-        <v>400</v>
-      </c>
+      <c r="H108" s="6"/>
+      <c r="I108" s="6"/>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
@@ -4760,19 +4822,22 @@
         <v>193</v>
       </c>
       <c r="C109" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E109" t="s">
         <v>105</v>
       </c>
       <c r="F109" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="H109" s="3" t="s">
-        <v>550</v>
+        <v>547</v>
+      </c>
+      <c r="I109" s="3" t="s">
+        <v>653</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -4783,16 +4848,16 @@
         <v>193</v>
       </c>
       <c r="C110" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E110" t="s">
         <v>106</v>
       </c>
       <c r="F110" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -4803,16 +4868,19 @@
         <v>193</v>
       </c>
       <c r="C111" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E111" t="s">
         <v>107</v>
       </c>
       <c r="F111" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>403</v>
+        <v>402</v>
+      </c>
+      <c r="I111" s="3" t="s">
+        <v>654</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -4823,16 +4891,19 @@
         <v>193</v>
       </c>
       <c r="C112" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E112" t="s">
         <v>108</v>
       </c>
       <c r="F112" s="3" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
+        <v>261</v>
+      </c>
+      <c r="I112" s="3" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>109</v>
       </c>
@@ -4840,16 +4911,16 @@
         <v>193</v>
       </c>
       <c r="C113" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E113" t="s">
         <v>109</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>110</v>
       </c>
@@ -4857,19 +4928,22 @@
         <v>193</v>
       </c>
       <c r="C114" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E114" t="s">
         <v>110</v>
       </c>
       <c r="F114" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
+        <v>403</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>111</v>
       </c>
@@ -4877,22 +4951,25 @@
         <v>193</v>
       </c>
       <c r="C115" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E115" t="s">
         <v>111</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H115" s="3" t="s">
-        <v>551</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
+        <v>548</v>
+      </c>
+      <c r="I115" s="3" t="s">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>112</v>
       </c>
@@ -4900,19 +4977,22 @@
         <v>193</v>
       </c>
       <c r="C116" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E116" t="s">
         <v>112</v>
       </c>
       <c r="F116" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>325</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
+        <v>324</v>
+      </c>
+      <c r="I116" s="3" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>113</v>
       </c>
@@ -4920,22 +5000,22 @@
         <v>193</v>
       </c>
       <c r="C117" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D117" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="E117" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
       <c r="G117" s="3" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H117" s="3" t="s">
-        <v>552</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>114</v>
       </c>
@@ -4943,45 +5023,49 @@
         <v>193</v>
       </c>
       <c r="C118" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D118" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="E118" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="G118" s="3" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+        <v>406</v>
+      </c>
+      <c r="I118" s="3" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="10" t="s">
         <v>115</v>
       </c>
-      <c r="B119" t="s">
-        <v>193</v>
-      </c>
-      <c r="C119" t="s">
-        <v>201</v>
-      </c>
-      <c r="D119" t="s">
-        <v>223</v>
-      </c>
-      <c r="E119" t="s">
-        <v>488</v>
-      </c>
-      <c r="F119" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="G119" s="3" t="s">
-        <v>409</v>
-      </c>
-      <c r="H119" s="3" t="s">
-        <v>553</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B119" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C119" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="D119" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="E119" s="10" t="s">
+        <v>485</v>
+      </c>
+      <c r="F119" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G119" s="6" t="s">
+        <v>407</v>
+      </c>
+      <c r="H119" s="6" t="s">
+        <v>550</v>
+      </c>
+      <c r="I119" s="6"/>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>116</v>
       </c>
@@ -4989,19 +5073,22 @@
         <v>193</v>
       </c>
       <c r="C120" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E120" t="s">
         <v>116</v>
       </c>
       <c r="F120" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G120" s="3" t="s">
-        <v>368</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
+        <v>367</v>
+      </c>
+      <c r="I120" s="3" t="s">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>117</v>
       </c>
@@ -5009,16 +5096,19 @@
         <v>193</v>
       </c>
       <c r="C121" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E121" t="s">
         <v>117</v>
       </c>
       <c r="G121" s="3" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
+        <v>408</v>
+      </c>
+      <c r="I121" s="3" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>118</v>
       </c>
@@ -5026,19 +5116,22 @@
         <v>193</v>
       </c>
       <c r="C122" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E122" t="s">
         <v>118</v>
       </c>
       <c r="F122" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="G122" s="3" t="s">
-        <v>411</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
+        <v>409</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>119</v>
       </c>
@@ -5046,19 +5139,22 @@
         <v>193</v>
       </c>
       <c r="C123" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E123" t="s">
         <v>119</v>
       </c>
       <c r="G123" s="3" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="H123" s="3" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
+        <v>551</v>
+      </c>
+      <c r="I123" s="3" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>120</v>
       </c>
@@ -5066,16 +5162,19 @@
         <v>193</v>
       </c>
       <c r="C124" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E124" t="s">
         <v>120</v>
       </c>
       <c r="G124" s="3" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
+        <v>411</v>
+      </c>
+      <c r="I124" s="3" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>121</v>
       </c>
@@ -5083,16 +5182,16 @@
         <v>193</v>
       </c>
       <c r="C125" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E125" t="s">
         <v>121</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>122</v>
       </c>
@@ -5100,16 +5199,19 @@
         <v>193</v>
       </c>
       <c r="C126" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E126" t="s">
         <v>122</v>
       </c>
       <c r="G126" s="3" t="s">
-        <v>415</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
+        <v>412</v>
+      </c>
+      <c r="I126" s="3" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>123</v>
       </c>
@@ -5117,22 +5219,25 @@
         <v>193</v>
       </c>
       <c r="C127" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E127" t="s">
         <v>123</v>
       </c>
       <c r="F127" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="G127" s="3" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="H127" s="3" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
+        <v>552</v>
+      </c>
+      <c r="I127" s="3" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>124</v>
       </c>
@@ -5140,13 +5245,13 @@
         <v>193</v>
       </c>
       <c r="C128" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E128" t="s">
         <v>124</v>
       </c>
       <c r="G128" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -5157,13 +5262,16 @@
         <v>193</v>
       </c>
       <c r="C129" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E129" t="s">
         <v>125</v>
       </c>
       <c r="G129" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
+      </c>
+      <c r="I129" s="3" t="s">
+        <v>666</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -5174,13 +5282,13 @@
         <v>193</v>
       </c>
       <c r="C130" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E130" t="s">
         <v>126</v>
       </c>
       <c r="G130" s="3" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
     </row>
     <row r="131" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -5191,7 +5299,7 @@
         <v>193</v>
       </c>
       <c r="C131" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F131" s="5"/>
       <c r="G131" s="5"/>
@@ -5206,39 +5314,39 @@
         <v>193</v>
       </c>
       <c r="C132" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E132" t="s">
         <v>128</v>
       </c>
       <c r="F132" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="I132" s="3" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A133" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B133" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C133" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="F133" s="5" t="s">
         <v>270</v>
       </c>
-      <c r="G132" s="3" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
-        <v>129</v>
-      </c>
-      <c r="B133" t="s">
-        <v>193</v>
-      </c>
-      <c r="C133" t="s">
-        <v>201</v>
-      </c>
-      <c r="E133" t="s">
-        <v>129</v>
-      </c>
-      <c r="F133" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="G133" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="H133" s="3" t="s">
-        <v>556</v>
+      <c r="G133" s="5" t="s">
+        <v>415</v>
+      </c>
+      <c r="H133" s="5" t="s">
+        <v>553</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -5249,7 +5357,7 @@
         <v>193</v>
       </c>
       <c r="C134" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E134" t="s">
         <v>130</v>
@@ -5258,10 +5366,13 @@
         <v>-590</v>
       </c>
       <c r="G134" s="3" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="H134" s="3" t="s">
-        <v>557</v>
+        <v>554</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>668</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -5272,37 +5383,42 @@
         <v>193</v>
       </c>
       <c r="C135" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E135" t="s">
         <v>131</v>
       </c>
       <c r="F135" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="G135" s="3" t="s">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+        <v>417</v>
+      </c>
+      <c r="I135" s="3" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="B136" t="s">
-        <v>193</v>
-      </c>
-      <c r="C136" t="s">
-        <v>201</v>
-      </c>
-      <c r="E136" t="s">
+      <c r="B136" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C136" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="E136" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="G136" s="3" t="s">
-        <v>421</v>
-      </c>
-      <c r="H136" s="3" t="s">
-        <v>559</v>
-      </c>
+      <c r="F136" s="6"/>
+      <c r="G136" s="6" t="s">
+        <v>418</v>
+      </c>
+      <c r="H136" s="6" t="s">
+        <v>556</v>
+      </c>
+      <c r="I136" s="6"/>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
@@ -5312,19 +5428,22 @@
         <v>193</v>
       </c>
       <c r="C137" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E137" t="s">
         <v>133</v>
       </c>
       <c r="F137" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G137" s="3" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="H137" s="3" t="s">
-        <v>560</v>
+        <v>557</v>
+      </c>
+      <c r="I137" s="3" t="s">
+        <v>670</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -5335,33 +5454,42 @@
         <v>193</v>
       </c>
       <c r="C138" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E138" t="s">
         <v>134</v>
       </c>
       <c r="F138" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G138" s="3" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
       <c r="H138" s="3" t="s">
-        <v>561</v>
-      </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+        <v>558</v>
+      </c>
+      <c r="I138" s="3" t="s">
+        <v>671</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="B139" t="s">
-        <v>193</v>
-      </c>
-      <c r="C139" t="s">
-        <v>201</v>
-      </c>
-      <c r="E139" t="s">
+      <c r="B139" s="10" t="s">
+        <v>193</v>
+      </c>
+      <c r="C139" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="E139" s="10" t="s">
         <v>135</v>
+      </c>
+      <c r="F139" s="6"/>
+      <c r="G139" s="6"/>
+      <c r="H139" s="6"/>
+      <c r="I139" s="6" t="s">
+        <v>672</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -5372,19 +5500,22 @@
         <v>193</v>
       </c>
       <c r="C140" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E140" t="s">
         <v>136</v>
       </c>
       <c r="F140" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="G140" s="3" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="H140" s="3" t="s">
-        <v>562</v>
+        <v>559</v>
+      </c>
+      <c r="I140" s="3" t="s">
+        <v>673</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
@@ -5395,16 +5526,16 @@
         <v>193</v>
       </c>
       <c r="C141" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E141" t="s">
         <v>137</v>
       </c>
       <c r="F141" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="H141" s="3" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
@@ -5415,13 +5546,13 @@
         <v>193</v>
       </c>
       <c r="C142" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E142" t="s">
         <v>138</v>
       </c>
       <c r="G142" s="3" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
@@ -5432,13 +5563,16 @@
         <v>193</v>
       </c>
       <c r="C143" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E143" t="s">
         <v>139</v>
       </c>
       <c r="G143" s="3" t="s">
-        <v>409</v>
+        <v>407</v>
+      </c>
+      <c r="I143" s="3" t="s">
+        <v>674</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
@@ -5449,19 +5583,19 @@
         <v>195</v>
       </c>
       <c r="C144" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D144" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E144" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
       <c r="G144" s="3" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
       <c r="H144" s="3" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.25">
@@ -5472,7 +5606,7 @@
         <v>195</v>
       </c>
       <c r="C145" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E145" t="s">
         <v>141</v>
@@ -5489,19 +5623,19 @@
         <v>195</v>
       </c>
       <c r="C146" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D146" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E146" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
       <c r="F146" s="3" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="G146" s="3" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.25">
@@ -5512,16 +5646,16 @@
         <v>195</v>
       </c>
       <c r="C147" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E147" t="s">
         <v>143</v>
       </c>
       <c r="G147" s="3" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="H147" s="3" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.25">
@@ -5532,16 +5666,16 @@
         <v>195</v>
       </c>
       <c r="C148" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E148" t="s">
         <v>144</v>
       </c>
       <c r="G148" s="3" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="H148" s="3" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.25">
@@ -5552,16 +5686,16 @@
         <v>195</v>
       </c>
       <c r="C149" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E149" t="s">
         <v>145</v>
       </c>
       <c r="F149" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="H149" s="3" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.25">
@@ -5572,13 +5706,13 @@
         <v>195</v>
       </c>
       <c r="C150" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E150" t="s">
         <v>146</v>
       </c>
       <c r="F150" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.25">
@@ -5589,7 +5723,7 @@
         <v>195</v>
       </c>
       <c r="C151" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E151" t="s">
         <v>147</v>
@@ -5603,16 +5737,16 @@
         <v>195</v>
       </c>
       <c r="C152" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E152" t="s">
         <v>148</v>
       </c>
       <c r="G152" s="3" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="H152" s="3" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.25">
@@ -5623,19 +5757,19 @@
         <v>195</v>
       </c>
       <c r="C153" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D153" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E153" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="G153" s="3" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="H153" s="3" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.25">
@@ -5646,13 +5780,13 @@
         <v>195</v>
       </c>
       <c r="C154" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E154" t="s">
         <v>150</v>
       </c>
       <c r="F154" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.25">
@@ -5663,7 +5797,7 @@
         <v>195</v>
       </c>
       <c r="C155" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E155" s="8" t="s">
         <v>151</v>
@@ -5672,7 +5806,7 @@
         <v>-70</v>
       </c>
       <c r="H155" s="3" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.25">
@@ -5683,13 +5817,13 @@
         <v>195</v>
       </c>
       <c r="C156" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E156" t="s">
         <v>152</v>
       </c>
       <c r="H156" s="3" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.25">
@@ -5700,13 +5834,13 @@
         <v>195</v>
       </c>
       <c r="C157" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E157" t="s">
         <v>153</v>
       </c>
       <c r="G157" s="3" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.25">
@@ -5717,13 +5851,13 @@
         <v>195</v>
       </c>
       <c r="C158" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E158" t="s">
         <v>154</v>
       </c>
       <c r="H158" s="3" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.25">
@@ -5734,19 +5868,19 @@
         <v>195</v>
       </c>
       <c r="C159" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E159" t="s">
         <v>155</v>
       </c>
       <c r="F159" s="3" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="G159" s="3" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="H159" s="3" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.25">
@@ -5757,19 +5891,19 @@
         <v>195</v>
       </c>
       <c r="C160" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E160" t="s">
         <v>156</v>
       </c>
       <c r="F160" s="3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="G160" s="3" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="H160" s="3" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
@@ -5780,7 +5914,7 @@
         <v>195</v>
       </c>
       <c r="C161" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E161" t="s">
         <v>157</v>
@@ -5789,7 +5923,7 @@
         <v>-440</v>
       </c>
       <c r="G161" s="3" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -5800,19 +5934,19 @@
         <v>195</v>
       </c>
       <c r="C162" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D162" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="E162" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="F162" s="3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="H162" s="3" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
@@ -5823,16 +5957,16 @@
         <v>195</v>
       </c>
       <c r="C163" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E163" t="s">
         <v>159</v>
       </c>
       <c r="G163" s="3" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="H163" s="3" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
@@ -5843,16 +5977,16 @@
         <v>195</v>
       </c>
       <c r="C164" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E164" t="s">
         <v>160</v>
       </c>
       <c r="G164" s="3" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="H164" s="3" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
     </row>
     <row r="165" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -5863,10 +5997,10 @@
         <v>195</v>
       </c>
       <c r="C165" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D165" s="2" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="F165" s="5"/>
       <c r="G165" s="5"/>
@@ -5881,13 +6015,13 @@
         <v>195</v>
       </c>
       <c r="C166" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E166" t="s">
         <v>162</v>
       </c>
       <c r="G166" s="3" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
@@ -5898,16 +6032,16 @@
         <v>195</v>
       </c>
       <c r="C167" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D167" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="E167" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="G167" s="3" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
@@ -5918,16 +6052,16 @@
         <v>195</v>
       </c>
       <c r="C168" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E168" t="s">
         <v>164</v>
       </c>
       <c r="F168" s="3" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G168" s="3" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
@@ -5938,13 +6072,13 @@
         <v>195</v>
       </c>
       <c r="C169" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D169" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="E169" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -5955,13 +6089,13 @@
         <v>195</v>
       </c>
       <c r="C170" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E170" t="s">
         <v>166</v>
       </c>
       <c r="H170" s="3" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
     </row>
     <row r="171" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -5972,10 +6106,10 @@
         <v>195</v>
       </c>
       <c r="C171" s="2" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="D171" s="2" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F171" s="5"/>
       <c r="G171" s="5"/>
@@ -5990,19 +6124,19 @@
         <v>195</v>
       </c>
       <c r="C172" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E172" t="s">
         <v>168</v>
       </c>
       <c r="F172" s="3" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="G172" s="3" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
       <c r="H172" s="3" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -6013,7 +6147,7 @@
         <v>195</v>
       </c>
       <c r="C173" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E173" t="s">
         <v>169</v>
@@ -6022,10 +6156,10 @@
         <v>-1100</v>
       </c>
       <c r="G173" s="3" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
       <c r="H173" s="3" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
@@ -6036,13 +6170,13 @@
         <v>195</v>
       </c>
       <c r="C174" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E174" t="s">
         <v>170</v>
       </c>
       <c r="H174" s="3" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
@@ -6053,13 +6187,13 @@
         <v>195</v>
       </c>
       <c r="C175" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E175" t="s">
         <v>171</v>
       </c>
       <c r="F175" s="3" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
@@ -6070,16 +6204,16 @@
         <v>195</v>
       </c>
       <c r="C176" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D176" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="E176" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="G176" s="3" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
@@ -6090,16 +6224,16 @@
         <v>195</v>
       </c>
       <c r="C177" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E177" t="s">
         <v>173</v>
       </c>
       <c r="G177" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="H177" s="3" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
@@ -6110,22 +6244,22 @@
         <v>195</v>
       </c>
       <c r="C178" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D178" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E178" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="F178" s="3" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="G178" s="3" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="H178" s="3" t="s">
-        <v>583</v>
+        <v>580</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
@@ -6136,13 +6270,13 @@
         <v>195</v>
       </c>
       <c r="C179" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E179" t="s">
         <v>175</v>
       </c>
       <c r="G179" s="3" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
@@ -6153,19 +6287,19 @@
         <v>195</v>
       </c>
       <c r="C180" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E180" t="s">
         <v>176</v>
       </c>
       <c r="F180" s="3" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="G180" s="3" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
       <c r="H180" s="3" t="s">
-        <v>584</v>
+        <v>581</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
@@ -6176,19 +6310,19 @@
         <v>195</v>
       </c>
       <c r="C181" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D181" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="E181" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="G181" s="3" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="H181" s="3" t="s">
-        <v>585</v>
+        <v>582</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
@@ -6199,13 +6333,13 @@
         <v>195</v>
       </c>
       <c r="C182" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E182" t="s">
         <v>178</v>
       </c>
       <c r="F182" s="3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
@@ -6216,16 +6350,16 @@
         <v>195</v>
       </c>
       <c r="C183" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E183" t="s">
         <v>179</v>
       </c>
       <c r="F183" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="G183" s="3" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
@@ -6236,13 +6370,13 @@
         <v>195</v>
       </c>
       <c r="C184" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E184" t="s">
         <v>180</v>
       </c>
       <c r="F184" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
@@ -6253,13 +6387,13 @@
         <v>195</v>
       </c>
       <c r="C185" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E185" t="s">
         <v>181</v>
       </c>
       <c r="G185" s="3" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
@@ -6270,13 +6404,13 @@
         <v>195</v>
       </c>
       <c r="C186" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E186" t="s">
         <v>182</v>
       </c>
       <c r="H186" s="3" t="s">
-        <v>586</v>
+        <v>583</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
@@ -6287,19 +6421,19 @@
         <v>195</v>
       </c>
       <c r="C187" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D187" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="E187" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="G187" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="H187" s="3" t="s">
-        <v>587</v>
+        <v>584</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
@@ -6310,16 +6444,16 @@
         <v>195</v>
       </c>
       <c r="C188" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E188" t="s">
         <v>184</v>
       </c>
       <c r="G188" s="3" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="H188" s="3" t="s">
-        <v>588</v>
+        <v>585</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
@@ -6330,19 +6464,19 @@
         <v>195</v>
       </c>
       <c r="C189" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E189" t="s">
         <v>185</v>
       </c>
       <c r="F189" s="3" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="G189" s="3" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="H189" s="3" t="s">
-        <v>589</v>
+        <v>586</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
@@ -6353,19 +6487,19 @@
         <v>195</v>
       </c>
       <c r="C190" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D190" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="E190" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="F190" s="3" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="G190" s="3" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="191" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6376,13 +6510,13 @@
         <v>195</v>
       </c>
       <c r="C191" s="2" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="D191" s="2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="F191" s="5" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="G191" s="5"/>
       <c r="H191" s="5"/>
@@ -6396,16 +6530,16 @@
         <v>195</v>
       </c>
       <c r="C192" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E192" t="s">
         <v>188</v>
       </c>
       <c r="F192" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="G192" s="3" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.25">
@@ -6416,16 +6550,16 @@
         <v>195</v>
       </c>
       <c r="C193" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E193" t="s">
         <v>189</v>
       </c>
       <c r="F193" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="G193" s="3" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.25">
@@ -6436,19 +6570,19 @@
         <v>195</v>
       </c>
       <c r="C194" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E194" t="s">
         <v>190</v>
       </c>
       <c r="F194" s="3" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="G194" s="3" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="H194" s="3" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updating exclusion files after 2017 dry firn exclusions identification.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE0F1F30-C698-4217-AC6C-6C3425510643}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5BA314-F17A-4BF2-A356-66F1DFE1BB9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3675" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -2435,8 +2435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A87" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I136" sqref="I136"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2591,6 +2591,7 @@
       <c r="H6" s="5" t="s">
         <v>507</v>
       </c>
+      <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
@@ -3028,6 +3029,7 @@
       <c r="H28" s="5" t="s">
         <v>312</v>
       </c>
+      <c r="I28" s="5"/>
     </row>
     <row r="29" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
@@ -3209,6 +3211,7 @@
       <c r="H36" s="5" t="s">
         <v>316</v>
       </c>
+      <c r="I36" s="5"/>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
@@ -3524,6 +3527,7 @@
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
       <c r="H50" s="5"/>
+      <c r="I50" s="5"/>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
@@ -3608,6 +3612,7 @@
         <v>362</v>
       </c>
       <c r="H54" s="5"/>
+      <c r="I54" s="5"/>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
@@ -3982,6 +3987,7 @@
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
       <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
     </row>
     <row r="71" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
@@ -3998,6 +4004,7 @@
       </c>
       <c r="G71" s="5"/>
       <c r="H71" s="5"/>
+      <c r="I71" s="5"/>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
@@ -4041,6 +4048,7 @@
       <c r="H73" s="5" t="s">
         <v>329</v>
       </c>
+      <c r="I73" s="5"/>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
@@ -4379,6 +4387,7 @@
       </c>
       <c r="G88" s="11"/>
       <c r="H88" s="5"/>
+      <c r="I88" s="5"/>
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
@@ -4448,6 +4457,7 @@
       <c r="H91" s="5" t="s">
         <v>541</v>
       </c>
+      <c r="I91" s="5"/>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
@@ -5348,6 +5358,7 @@
       <c r="H133" s="5" t="s">
         <v>553</v>
       </c>
+      <c r="I133" s="5"/>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134" t="s">

</xml_diff>

<commit_message>
Identification of exclusions of dry firn for 2018.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA5BA314-F17A-4BF2-A356-66F1DFE1BB9C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AD0CEB-B17F-453F-8C2E-FA830829E3ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3675" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="705">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -2059,6 +2059,87 @@
   </si>
   <si>
     <t>Yes, -inf in data but replaces by NaNs, ok - deleted after dry firn identification though slabs at the surface …</t>
+  </si>
+  <si>
+    <t>-2040</t>
+  </si>
+  <si>
+    <t>3370-</t>
+  </si>
+  <si>
+    <t>-1725</t>
+  </si>
+  <si>
+    <t>810-</t>
+  </si>
+  <si>
+    <t>8155-</t>
+  </si>
+  <si>
+    <t>-5500</t>
+  </si>
+  <si>
+    <t>-2180 2460-2550 4150-4270 4750-10810 12700-</t>
+  </si>
+  <si>
+    <t>-3240</t>
+  </si>
+  <si>
+    <t>-1095 1290-</t>
+  </si>
+  <si>
+    <t>300-</t>
+  </si>
+  <si>
+    <t>3045-</t>
+  </si>
+  <si>
+    <t>-18830 19610-19950 43260-</t>
+  </si>
+  <si>
+    <t>-1250</t>
+  </si>
+  <si>
+    <t>10600-</t>
+  </si>
+  <si>
+    <t>-410</t>
+  </si>
+  <si>
+    <t>2060-</t>
+  </si>
+  <si>
+    <t>4530-</t>
+  </si>
+  <si>
+    <t>-1580</t>
+  </si>
+  <si>
+    <t>-1500</t>
+  </si>
+  <si>
+    <t>-1450</t>
+  </si>
+  <si>
+    <t>3375-3510 3695-</t>
+  </si>
+  <si>
+    <t>-540</t>
+  </si>
+  <si>
+    <t>10470-10760 11500-</t>
+  </si>
+  <si>
+    <t>2390-3600 3700-</t>
+  </si>
+  <si>
+    <t>11750-12750 12945-</t>
+  </si>
+  <si>
+    <t>-2720 2915-</t>
+  </si>
+  <si>
+    <t>4165-</t>
   </si>
 </sst>
 </file>
@@ -2115,10 +2196,10 @@
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2435,8 +2516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D190" sqref="D190"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3605,10 +3686,10 @@
       <c r="C54" s="5" t="s">
         <v>676</v>
       </c>
-      <c r="F54" s="11" t="s">
+      <c r="F54" s="10" t="s">
         <v>457</v>
       </c>
-      <c r="G54" s="11" t="s">
+      <c r="G54" s="10" t="s">
         <v>362</v>
       </c>
       <c r="H54" s="5"/>
@@ -3924,17 +4005,17 @@
         <v>621</v>
       </c>
     </row>
-    <row r="68" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="10" t="s">
+    <row r="68" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B68" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="C68" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="E68" s="10" t="s">
+      <c r="B68" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C68" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E68" s="9" t="s">
         <v>64</v>
       </c>
       <c r="F68" s="6" t="s">
@@ -4368,7 +4449,7 @@
       <c r="H87" s="3" t="s">
         <v>538</v>
       </c>
-      <c r="I87" s="9" t="s">
+      <c r="I87" s="8" t="s">
         <v>636</v>
       </c>
     </row>
@@ -4382,10 +4463,10 @@
       <c r="C88" s="5" t="s">
         <v>675</v>
       </c>
-      <c r="F88" s="11" t="s">
+      <c r="F88" s="10" t="s">
         <v>462</v>
       </c>
-      <c r="G88" s="11"/>
+      <c r="G88" s="10"/>
       <c r="H88" s="5"/>
       <c r="I88" s="5"/>
     </row>
@@ -4448,10 +4529,10 @@
       <c r="C91" s="5" t="s">
         <v>675</v>
       </c>
-      <c r="F91" s="11" t="s">
+      <c r="F91" s="10" t="s">
         <v>463</v>
       </c>
-      <c r="G91" s="11" t="s">
+      <c r="G91" s="10" t="s">
         <v>319</v>
       </c>
       <c r="H91" s="5" t="s">
@@ -4778,17 +4859,17 @@
       <c r="H106" s="5"/>
       <c r="I106" s="5"/>
     </row>
-    <row r="107" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="10" t="s">
+    <row r="107" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A107" s="9" t="s">
         <v>103</v>
       </c>
-      <c r="B107" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="C107" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="E107" s="10" t="s">
+      <c r="B107" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E107" s="9" t="s">
         <v>103</v>
       </c>
       <c r="F107" s="6"/>
@@ -4802,17 +4883,17 @@
         <v>652</v>
       </c>
     </row>
-    <row r="108" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="10" t="s">
+    <row r="108" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A108" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="B108" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="C108" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="E108" s="10" t="s">
+      <c r="B108" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C108" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E108" s="9" t="s">
         <v>104</v>
       </c>
       <c r="F108" s="6" t="s">
@@ -5048,20 +5129,20 @@
         <v>622</v>
       </c>
     </row>
-    <row r="119" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A119" s="10" t="s">
+    <row r="119" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A119" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="B119" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="C119" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="D119" s="10" t="s">
+      <c r="B119" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C119" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D119" s="9" t="s">
         <v>222</v>
       </c>
-      <c r="E119" s="10" t="s">
+      <c r="E119" s="9" t="s">
         <v>485</v>
       </c>
       <c r="F119" s="6" t="s">
@@ -5409,17 +5490,17 @@
         <v>669</v>
       </c>
     </row>
-    <row r="136" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A136" s="10" t="s">
+    <row r="136" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A136" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="B136" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="C136" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="E136" s="10" t="s">
+      <c r="B136" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C136" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E136" s="9" t="s">
         <v>132</v>
       </c>
       <c r="F136" s="6"/>
@@ -5483,17 +5564,17 @@
         <v>671</v>
       </c>
     </row>
-    <row r="139" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A139" s="10" t="s">
+    <row r="139" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A139" s="9" t="s">
         <v>135</v>
       </c>
-      <c r="B139" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="C139" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="E139" s="10" t="s">
+      <c r="B139" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="C139" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E139" s="9" t="s">
         <v>135</v>
       </c>
       <c r="F139" s="6"/>
@@ -5586,47 +5667,49 @@
         <v>674</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A144" t="s">
+    <row r="144" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="9" t="s">
         <v>140</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B144" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="C144" t="s">
-        <v>200</v>
-      </c>
-      <c r="D144" t="s">
+      <c r="C144" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="D144" s="9" t="s">
         <v>217</v>
       </c>
-      <c r="E144" t="s">
+      <c r="E144" s="9" t="s">
         <v>486</v>
       </c>
-      <c r="G144" s="3" t="s">
+      <c r="F144" s="6"/>
+      <c r="G144" s="6" t="s">
         <v>423</v>
       </c>
-      <c r="H144" s="3" t="s">
+      <c r="H144" s="6" t="s">
         <v>561</v>
       </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A145" t="s">
+      <c r="I144" s="6"/>
+    </row>
+    <row r="145" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A145" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B145" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C145" t="s">
-        <v>200</v>
-      </c>
-      <c r="E145" t="s">
-        <v>141</v>
-      </c>
-      <c r="F145" s="3">
+      <c r="C145" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="F145" s="5">
         <v>-1600</v>
       </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G145" s="5"/>
+      <c r="H145" s="5"/>
+      <c r="I145" s="5"/>
+    </row>
+    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>142</v>
       </c>
@@ -5648,8 +5731,11 @@
       <c r="G146" s="3" t="s">
         <v>424</v>
       </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I146" s="3" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>143</v>
       </c>
@@ -5668,8 +5754,11 @@
       <c r="H147" s="3" t="s">
         <v>562</v>
       </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I147" s="3" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>144</v>
       </c>
@@ -5688,8 +5777,11 @@
       <c r="H148" s="3" t="s">
         <v>563</v>
       </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I148" s="3" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>145</v>
       </c>
@@ -5708,8 +5800,11 @@
       <c r="H149" s="3" t="s">
         <v>564</v>
       </c>
-    </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I149" s="3" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>146</v>
       </c>
@@ -5725,8 +5820,11 @@
       <c r="F150" s="3" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I150" s="3" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>147</v>
       </c>
@@ -5739,8 +5837,11 @@
       <c r="E151" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I151" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>148</v>
       </c>
@@ -5759,8 +5860,11 @@
       <c r="H152" s="3" t="s">
         <v>565</v>
       </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I152" s="3" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>149</v>
       </c>
@@ -5782,8 +5886,11 @@
       <c r="H153" s="3" t="s">
         <v>566</v>
       </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I153" s="3" t="s">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>150</v>
       </c>
@@ -5800,44 +5907,48 @@
         <v>279</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A155" t="s">
+    <row r="155" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B155" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="C155" t="s">
-        <v>200</v>
-      </c>
-      <c r="E155" s="8" t="s">
+      <c r="C155" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E155" s="11" t="s">
         <v>151</v>
       </c>
-      <c r="F155" s="3">
+      <c r="F155" s="6">
         <v>-70</v>
       </c>
-      <c r="H155" s="3" t="s">
+      <c r="G155" s="6"/>
+      <c r="H155" s="6" t="s">
         <v>567</v>
       </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A156" t="s">
+      <c r="I155" s="6" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="156" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B156" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C156" t="s">
-        <v>200</v>
-      </c>
-      <c r="E156" t="s">
-        <v>152</v>
-      </c>
-      <c r="H156" s="3" t="s">
+      <c r="C156" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="F156" s="5"/>
+      <c r="G156" s="5"/>
+      <c r="H156" s="5" t="s">
         <v>568</v>
       </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I156" s="5"/>
+    </row>
+    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>153</v>
       </c>
@@ -5853,8 +5964,11 @@
       <c r="G157" s="3" t="s">
         <v>429</v>
       </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I157" s="3" t="s">
+        <v>686</v>
+      </c>
+    </row>
+    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>154</v>
       </c>
@@ -5870,52 +5984,57 @@
       <c r="H158" s="3" t="s">
         <v>569</v>
       </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A159" t="s">
+      <c r="I158" s="3" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="159" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="C159" t="s">
-        <v>200</v>
-      </c>
-      <c r="E159" t="s">
+      <c r="C159" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E159" s="9" t="s">
         <v>155</v>
       </c>
-      <c r="F159" s="3" t="s">
+      <c r="F159" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="G159" s="3" t="s">
+      <c r="G159" s="6" t="s">
         <v>430</v>
       </c>
-      <c r="H159" s="3" t="s">
+      <c r="H159" s="6" t="s">
         <v>570</v>
       </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A160" t="s">
+      <c r="I159" s="6"/>
+    </row>
+    <row r="160" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="B160" t="s">
+      <c r="B160" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="C160" t="s">
-        <v>200</v>
-      </c>
-      <c r="E160" t="s">
+      <c r="C160" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E160" s="9" t="s">
         <v>156</v>
       </c>
-      <c r="F160" s="3" t="s">
+      <c r="F160" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="G160" s="3" t="s">
+      <c r="G160" s="6" t="s">
         <v>431</v>
       </c>
-      <c r="H160" s="3" t="s">
+      <c r="H160" s="6" t="s">
         <v>571</v>
       </c>
+      <c r="I160" s="6"/>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
@@ -5936,6 +6055,9 @@
       <c r="G161" s="3" t="s">
         <v>432</v>
       </c>
+      <c r="I161" s="3" t="s">
+        <v>688</v>
+      </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
@@ -5959,6 +6081,9 @@
       <c r="H162" s="3" t="s">
         <v>572</v>
       </c>
+      <c r="I162" s="3" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
@@ -5979,26 +6104,28 @@
       <c r="H163" s="3" t="s">
         <v>573</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A164" t="s">
+      <c r="I163" s="3" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="164" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
         <v>160</v>
       </c>
-      <c r="B164" t="s">
+      <c r="B164" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="C164" t="s">
-        <v>200</v>
-      </c>
-      <c r="E164" t="s">
-        <v>160</v>
-      </c>
-      <c r="G164" s="3" t="s">
+      <c r="C164" s="5" t="s">
+        <v>675</v>
+      </c>
+      <c r="F164" s="5"/>
+      <c r="G164" s="5" t="s">
         <v>434</v>
       </c>
-      <c r="H164" s="3" t="s">
+      <c r="H164" s="5" t="s">
         <v>574</v>
       </c>
+      <c r="I164" s="5"/>
     </row>
     <row r="165" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
@@ -6034,6 +6161,9 @@
       <c r="G166" s="3" t="s">
         <v>435</v>
       </c>
+      <c r="I166" s="3" t="s">
+        <v>691</v>
+      </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
@@ -6074,6 +6204,9 @@
       <c r="G168" s="3" t="s">
         <v>436</v>
       </c>
+      <c r="I168" s="3" t="s">
+        <v>340</v>
+      </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
@@ -6107,6 +6240,9 @@
       </c>
       <c r="H170" s="3" t="s">
         <v>575</v>
+      </c>
+      <c r="I170" s="3" t="s">
+        <v>692</v>
       </c>
     </row>
     <row r="171" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6149,6 +6285,9 @@
       <c r="H172" s="3" t="s">
         <v>576</v>
       </c>
+      <c r="I172" s="3" t="s">
+        <v>693</v>
+      </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
@@ -6172,6 +6311,9 @@
       <c r="H173" s="3" t="s">
         <v>577</v>
       </c>
+      <c r="I173" s="3" t="s">
+        <v>694</v>
+      </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
@@ -6189,6 +6331,9 @@
       <c r="H174" s="3" t="s">
         <v>578</v>
       </c>
+      <c r="I174" s="3" t="s">
+        <v>695</v>
+      </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
@@ -6206,6 +6351,9 @@
       <c r="F175" s="3" t="s">
         <v>285</v>
       </c>
+      <c r="I175" s="3" t="s">
+        <v>696</v>
+      </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
@@ -6226,6 +6374,9 @@
       <c r="G176" s="3" t="s">
         <v>439</v>
       </c>
+      <c r="I176" s="3" t="s">
+        <v>697</v>
+      </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
@@ -6272,6 +6423,9 @@
       <c r="H178" s="3" t="s">
         <v>580</v>
       </c>
+      <c r="I178" s="3" t="s">
+        <v>694</v>
+      </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
@@ -6290,28 +6444,29 @@
         <v>382</v>
       </c>
     </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A180" t="s">
+    <row r="180" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="B180" t="s">
+      <c r="B180" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="C180" t="s">
-        <v>200</v>
-      </c>
-      <c r="E180" t="s">
+      <c r="C180" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="E180" s="9" t="s">
         <v>176</v>
       </c>
-      <c r="F180" s="3" t="s">
+      <c r="F180" s="6" t="s">
         <v>287</v>
       </c>
-      <c r="G180" s="3" t="s">
+      <c r="G180" s="6" t="s">
         <v>441</v>
       </c>
-      <c r="H180" s="3" t="s">
+      <c r="H180" s="6" t="s">
         <v>581</v>
       </c>
+      <c r="I180" s="6"/>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
@@ -6335,6 +6490,9 @@
       <c r="H181" s="3" t="s">
         <v>582</v>
       </c>
+      <c r="I181" s="3" t="s">
+        <v>698</v>
+      </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
@@ -6352,6 +6510,9 @@
       <c r="F182" s="3" t="s">
         <v>288</v>
       </c>
+      <c r="I182" s="3" t="s">
+        <v>699</v>
+      </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
@@ -6372,6 +6533,9 @@
       <c r="G183" s="3" t="s">
         <v>443</v>
       </c>
+      <c r="I183" s="3" t="s">
+        <v>700</v>
+      </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
@@ -6446,6 +6610,9 @@
       <c r="H187" s="3" t="s">
         <v>584</v>
       </c>
+      <c r="I187" s="3" t="s">
+        <v>701</v>
+      </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
@@ -6512,6 +6679,9 @@
       <c r="G190" s="3" t="s">
         <v>449</v>
       </c>
+      <c r="I190" s="3" t="s">
+        <v>702</v>
+      </c>
     </row>
     <row r="191" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
@@ -6552,8 +6722,11 @@
       <c r="G192" s="3" t="s">
         <v>450</v>
       </c>
-    </row>
-    <row r="193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I192" s="3" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>189</v>
       </c>
@@ -6572,8 +6745,11 @@
       <c r="G193" s="3" t="s">
         <v>451</v>
       </c>
-    </row>
-    <row r="194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I193" s="3" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>190</v>
       </c>

</xml_diff>

<commit_message>
New round of dry firn exclusions identification for 2017.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5AD0CEB-B17F-453F-8C2E-FA830829E3ED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7423F77D-6880-4637-8C18-717888BAA05B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3675" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -1806,9 +1806,6 @@
     <t>1880-</t>
   </si>
   <si>
-    <t>30580-30700 30780-30820</t>
-  </si>
-  <si>
     <t>1150-</t>
   </si>
   <si>
@@ -1818,12 +1815,6 @@
     <t>3050-6595 7210-7370 7700-8240 8425-8540 8870-9380 9523-9690 10400-10960 11250-11320 25980-</t>
   </si>
   <si>
-    <t>-2240 5980-</t>
-  </si>
-  <si>
-    <t>-3960 5555-5620 15260-16100 16390-17100 23260-24360 27240-27350 29910-30560 31870-31940</t>
-  </si>
-  <si>
     <t>8400-</t>
   </si>
   <si>
@@ -1842,21 +1833,12 @@
     <t>-1440</t>
   </si>
   <si>
-    <t>1320-3625</t>
-  </si>
-  <si>
     <t>2750-3000</t>
   </si>
   <si>
     <t>470-680 1690-</t>
   </si>
   <si>
-    <t>2400-3500</t>
-  </si>
-  <si>
-    <t>2200-3400 4245-4670 5060-5510</t>
-  </si>
-  <si>
     <t>880-</t>
   </si>
   <si>
@@ -1869,18 +1851,9 @@
     <t>-2015</t>
   </si>
   <si>
-    <t>-1810</t>
-  </si>
-  <si>
-    <t>2820-</t>
-  </si>
-  <si>
     <t>-875</t>
   </si>
   <si>
-    <t>22920-33600</t>
-  </si>
-  <si>
     <t>4120-4360</t>
   </si>
   <si>
@@ -1890,9 +1863,6 @@
     <t>-5650</t>
   </si>
   <si>
-    <t>-1235</t>
-  </si>
-  <si>
     <t>2330-</t>
   </si>
   <si>
@@ -1911,9 +1881,6 @@
     <t>5740-</t>
   </si>
   <si>
-    <t>370-850 1755-5670</t>
-  </si>
-  <si>
     <t>2040-</t>
   </si>
   <si>
@@ -1923,33 +1890,21 @@
     <t>-260 480-</t>
   </si>
   <si>
-    <t>5595-</t>
-  </si>
-  <si>
     <t>-870 1785-</t>
   </si>
   <si>
     <t>-3930</t>
   </si>
   <si>
-    <t>-2700 4040-7200</t>
-  </si>
-  <si>
     <t>2815-3465 3500-</t>
   </si>
   <si>
-    <t>-2295</t>
-  </si>
-  <si>
     <t>1470-2935</t>
   </si>
   <si>
     <t>-1280 1450-1870 2070-2545 3220-3380</t>
   </si>
   <si>
-    <t>3600-3800 4120-7340 8225-</t>
-  </si>
-  <si>
     <t>-3130</t>
   </si>
   <si>
@@ -1959,42 +1914,21 @@
     <t>-4090</t>
   </si>
   <si>
-    <t>1510-</t>
-  </si>
-  <si>
     <t>-1670</t>
   </si>
   <si>
-    <t>2700-</t>
-  </si>
-  <si>
     <t>-1750</t>
   </si>
   <si>
     <t>3855-</t>
   </si>
   <si>
-    <t>-1280 1600-1760</t>
-  </si>
-  <si>
-    <t>3200-</t>
-  </si>
-  <si>
-    <t>5350-</t>
-  </si>
-  <si>
-    <t>2250-2870</t>
-  </si>
-  <si>
     <t>5490-9045 9600-14320</t>
   </si>
   <si>
     <t>10060-</t>
   </si>
   <si>
-    <t>-650 5015-5500 5665-5965 6740-7390 7685-8320 8480-</t>
-  </si>
-  <si>
     <t>8960-9280 9570-</t>
   </si>
   <si>
@@ -2140,6 +2074,72 @@
   </si>
   <si>
     <t>4165-</t>
+  </si>
+  <si>
+    <t>12440-25268 30580-30700 30780-30820</t>
+  </si>
+  <si>
+    <t>-2240 5355-5445 5980-</t>
+  </si>
+  <si>
+    <t>-8340</t>
+  </si>
+  <si>
+    <t>-3960 5555-5800 15260-16100 16390-17100 23260-24360 26940-27000 27240-27350 29910-30560 30620-30730 30860-30890 31460-31470 31830-31940</t>
+  </si>
+  <si>
+    <t>1260-3640 3790-3930</t>
+  </si>
+  <si>
+    <t>2400-3590</t>
+  </si>
+  <si>
+    <t>2200-3400 4170-4670 5060-5510</t>
+  </si>
+  <si>
+    <t>-1810 1860-1870 2030-2040</t>
+  </si>
+  <si>
+    <t>2670-2720 2820-</t>
+  </si>
+  <si>
+    <t>22920-33610</t>
+  </si>
+  <si>
+    <t>-1382</t>
+  </si>
+  <si>
+    <t>370-895 1755-5670</t>
+  </si>
+  <si>
+    <t>5250-</t>
+  </si>
+  <si>
+    <t>-2950 4040-7200</t>
+  </si>
+  <si>
+    <t>-2650</t>
+  </si>
+  <si>
+    <t>1550-2620 3600-7340 8225-</t>
+  </si>
+  <si>
+    <t>1250-</t>
+  </si>
+  <si>
+    <t>2690-</t>
+  </si>
+  <si>
+    <t>-1940</t>
+  </si>
+  <si>
+    <t>5275-</t>
+  </si>
+  <si>
+    <t>2040-2053 2250-2870</t>
+  </si>
+  <si>
+    <t>-650 1695-2110 5015-5500 5665-5965 6740-7390 7685-8320 8480-</t>
   </si>
 </sst>
 </file>
@@ -2516,8 +2516,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A127" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D190" sqref="D190"/>
+    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G138" sqref="G138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2665,7 +2665,7 @@
         <v>193</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>675</v>
+        <v>653</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -2819,7 +2819,7 @@
         <v>510</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>593</v>
+        <v>683</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2998,7 +2998,7 @@
         <v>309</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3018,7 +3018,7 @@
         <v>310</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -3047,7 +3047,7 @@
         <v>514</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -3070,7 +3070,7 @@
         <v>515</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>597</v>
+        <v>684</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -3101,7 +3101,7 @@
         <v>193</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>675</v>
+        <v>653</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5" t="s">
@@ -3152,8 +3152,8 @@
       <c r="H30" s="3" t="s">
         <v>516</v>
       </c>
-      <c r="I30" s="3">
-        <v>-7120</v>
+      <c r="I30" s="3" t="s">
+        <v>685</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -3202,7 +3202,7 @@
         <v>517</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>598</v>
+        <v>686</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3274,7 +3274,7 @@
         <v>315</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>599</v>
+        <v>596</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3285,7 +3285,7 @@
         <v>193</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>675</v>
+        <v>653</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -3314,7 +3314,7 @@
         <v>518</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>600</v>
+        <v>597</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -3334,7 +3334,7 @@
         <v>353</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -3357,7 +3357,7 @@
         <v>-1815</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -3386,7 +3386,7 @@
         <v>519</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>603</v>
+        <v>600</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3397,7 +3397,7 @@
         <v>193</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>677</v>
+        <v>655</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>240</v>
@@ -3431,7 +3431,7 @@
         <v>382</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>604</v>
+        <v>601</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3457,7 +3457,7 @@
         <v>520</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>605</v>
+        <v>687</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3480,7 +3480,7 @@
         <v>521</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3503,7 +3503,7 @@
         <v>317</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -3566,7 +3566,7 @@
         <v>522</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>608</v>
+        <v>688</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3592,7 +3592,7 @@
         <v>523</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>609</v>
+        <v>689</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3603,7 +3603,7 @@
         <v>193</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>675</v>
+        <v>653</v>
       </c>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
@@ -3627,7 +3627,7 @@
         <v>524</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>610</v>
+        <v>604</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -3684,7 +3684,7 @@
         <v>193</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>676</v>
+        <v>654</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>457</v>
@@ -3716,7 +3716,7 @@
         <v>320</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>611</v>
+        <v>605</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3742,7 +3742,7 @@
         <v>527</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>612</v>
+        <v>606</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3768,7 +3768,7 @@
         <v>322</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>613</v>
+        <v>607</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -3826,7 +3826,7 @@
         <v>364</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>614</v>
+        <v>690</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3849,7 +3849,7 @@
         <v>528</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>615</v>
+        <v>691</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3875,7 +3875,7 @@
         <v>323</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>616</v>
+        <v>608</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3901,7 +3901,7 @@
         <v>587</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>617</v>
+        <v>692</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3927,7 +3927,7 @@
         <v>529</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>618</v>
+        <v>609</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3956,7 +3956,7 @@
         <v>325</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>619</v>
+        <v>610</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3979,7 +3979,7 @@
         <v>326</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>620</v>
+        <v>611</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -4002,7 +4002,7 @@
         <v>530</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>621</v>
+        <v>693</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4052,7 +4052,7 @@
         <v>531</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>622</v>
+        <v>612</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4063,7 +4063,7 @@
         <v>193</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>675</v>
+        <v>653</v>
       </c>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
@@ -4078,7 +4078,7 @@
         <v>193</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>675</v>
+        <v>653</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>248</v>
@@ -4107,7 +4107,7 @@
         <v>532</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>623</v>
+        <v>613</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4118,7 +4118,7 @@
         <v>193</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>675</v>
+        <v>653</v>
       </c>
       <c r="F73" s="5">
         <v>-610</v>
@@ -4148,7 +4148,7 @@
         <v>533</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>624</v>
+        <v>614</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -4174,7 +4174,7 @@
         <v>374</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>625</v>
+        <v>615</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -4211,7 +4211,7 @@
         <v>73</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>626</v>
+        <v>616</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -4240,7 +4240,7 @@
         <v>534</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>627</v>
+        <v>617</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -4266,7 +4266,7 @@
         <v>330</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>628</v>
+        <v>694</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -4292,7 +4292,7 @@
         <v>535</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>629</v>
+        <v>618</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -4312,7 +4312,7 @@
         <v>381</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>630</v>
+        <v>619</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -4338,7 +4338,7 @@
         <v>536</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>631</v>
+        <v>620</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -4358,24 +4358,24 @@
         <v>250</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>632</v>
-      </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+        <v>695</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="B84" t="s">
-        <v>193</v>
-      </c>
-      <c r="C84" t="s">
-        <v>200</v>
-      </c>
-      <c r="E84" t="s">
-        <v>80</v>
-      </c>
-      <c r="I84" s="3" t="s">
-        <v>633</v>
+      <c r="B84" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>653</v>
+      </c>
+      <c r="F84" s="5"/>
+      <c r="G84" s="5"/>
+      <c r="H84" s="5"/>
+      <c r="I84" s="5" t="s">
+        <v>621</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -4395,7 +4395,7 @@
         <v>383</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>634</v>
+        <v>622</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -4424,7 +4424,7 @@
         <v>537</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>635</v>
+        <v>696</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -4450,7 +4450,7 @@
         <v>538</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>636</v>
+        <v>623</v>
       </c>
     </row>
     <row r="88" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4461,7 +4461,7 @@
         <v>193</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>675</v>
+        <v>653</v>
       </c>
       <c r="F88" s="10" t="s">
         <v>462</v>
@@ -4490,7 +4490,7 @@
         <v>539</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>637</v>
+        <v>697</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -4516,7 +4516,7 @@
         <v>540</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>638</v>
+        <v>624</v>
       </c>
     </row>
     <row r="91" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4527,7 +4527,7 @@
         <v>193</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>675</v>
+        <v>653</v>
       </c>
       <c r="F91" s="10" t="s">
         <v>463</v>
@@ -4557,7 +4557,7 @@
         <v>542</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>639</v>
+        <v>625</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -4580,7 +4580,7 @@
         <v>543</v>
       </c>
       <c r="I93" s="3" t="s">
-        <v>640</v>
+        <v>698</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -4603,7 +4603,7 @@
         <v>389</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>641</v>
+        <v>626</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -4626,7 +4626,7 @@
         <v>390</v>
       </c>
       <c r="I95" s="3" t="s">
-        <v>642</v>
+        <v>627</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -4646,7 +4646,7 @@
         <v>391</v>
       </c>
       <c r="I96" s="3" t="s">
-        <v>643</v>
+        <v>628</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -4666,7 +4666,7 @@
         <v>544</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>644</v>
+        <v>699</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -4686,7 +4686,7 @@
         <v>392</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>645</v>
+        <v>629</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -4709,7 +4709,7 @@
         <v>393</v>
       </c>
       <c r="I99" s="3" t="s">
-        <v>646</v>
+        <v>700</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -4735,7 +4735,7 @@
         <v>545</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>647</v>
+        <v>630</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -4755,7 +4755,7 @@
         <v>394</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>648</v>
+        <v>631</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -4775,7 +4775,7 @@
         <v>395</v>
       </c>
       <c r="I102" s="3" t="s">
-        <v>649</v>
+        <v>701</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -4795,7 +4795,7 @@
         <v>481</v>
       </c>
       <c r="I103" s="3" t="s">
-        <v>650</v>
+        <v>452</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -4841,7 +4841,7 @@
         <v>397</v>
       </c>
       <c r="I105" s="3" t="s">
-        <v>651</v>
+        <v>702</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4880,7 +4880,7 @@
         <v>546</v>
       </c>
       <c r="I107" s="6" t="s">
-        <v>652</v>
+        <v>703</v>
       </c>
     </row>
     <row r="108" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4928,7 +4928,7 @@
         <v>547</v>
       </c>
       <c r="I109" s="3" t="s">
-        <v>653</v>
+        <v>632</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -4971,7 +4971,7 @@
         <v>402</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>654</v>
+        <v>633</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -4991,7 +4991,7 @@
         <v>261</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>655</v>
+        <v>704</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -5031,7 +5031,7 @@
         <v>403</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>656</v>
+        <v>634</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -5057,7 +5057,7 @@
         <v>548</v>
       </c>
       <c r="I115" s="3" t="s">
-        <v>657</v>
+        <v>635</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -5080,7 +5080,7 @@
         <v>324</v>
       </c>
       <c r="I116" s="3" t="s">
-        <v>658</v>
+        <v>636</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -5126,7 +5126,7 @@
         <v>406</v>
       </c>
       <c r="I118" s="3" t="s">
-        <v>622</v>
+        <v>612</v>
       </c>
     </row>
     <row r="119" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -5176,7 +5176,7 @@
         <v>367</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>659</v>
+        <v>637</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -5196,7 +5196,7 @@
         <v>408</v>
       </c>
       <c r="I121" s="3" t="s">
-        <v>660</v>
+        <v>638</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -5219,7 +5219,7 @@
         <v>409</v>
       </c>
       <c r="I122" s="3" t="s">
-        <v>661</v>
+        <v>639</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -5262,7 +5262,7 @@
         <v>411</v>
       </c>
       <c r="I124" s="3" t="s">
-        <v>662</v>
+        <v>640</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -5279,7 +5279,7 @@
         <v>121</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>663</v>
+        <v>641</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -5299,7 +5299,7 @@
         <v>412</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>664</v>
+        <v>642</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -5325,7 +5325,7 @@
         <v>552</v>
       </c>
       <c r="I127" s="3" t="s">
-        <v>665</v>
+        <v>643</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -5362,7 +5362,7 @@
         <v>351</v>
       </c>
       <c r="I129" s="3" t="s">
-        <v>666</v>
+        <v>644</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -5417,7 +5417,7 @@
         <v>350</v>
       </c>
       <c r="I132" s="3" t="s">
-        <v>667</v>
+        <v>645</v>
       </c>
     </row>
     <row r="133" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -5428,7 +5428,7 @@
         <v>193</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>675</v>
+        <v>653</v>
       </c>
       <c r="F133" s="5" t="s">
         <v>270</v>
@@ -5464,7 +5464,7 @@
         <v>554</v>
       </c>
       <c r="I134" s="3" t="s">
-        <v>668</v>
+        <v>646</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -5487,7 +5487,7 @@
         <v>417</v>
       </c>
       <c r="I135" s="3" t="s">
-        <v>669</v>
+        <v>647</v>
       </c>
     </row>
     <row r="136" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -5535,7 +5535,7 @@
         <v>557</v>
       </c>
       <c r="I137" s="3" t="s">
-        <v>670</v>
+        <v>648</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -5561,7 +5561,7 @@
         <v>558</v>
       </c>
       <c r="I138" s="3" t="s">
-        <v>671</v>
+        <v>649</v>
       </c>
     </row>
     <row r="139" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -5581,7 +5581,7 @@
       <c r="G139" s="6"/>
       <c r="H139" s="6"/>
       <c r="I139" s="6" t="s">
-        <v>672</v>
+        <v>650</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -5607,7 +5607,7 @@
         <v>559</v>
       </c>
       <c r="I140" s="3" t="s">
-        <v>673</v>
+        <v>651</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
@@ -5664,7 +5664,7 @@
         <v>407</v>
       </c>
       <c r="I143" s="3" t="s">
-        <v>674</v>
+        <v>652</v>
       </c>
     </row>
     <row r="144" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -5700,7 +5700,7 @@
         <v>195</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>675</v>
+        <v>653</v>
       </c>
       <c r="F145" s="5">
         <v>-1600</v>
@@ -5732,7 +5732,7 @@
         <v>424</v>
       </c>
       <c r="I146" s="3" t="s">
-        <v>678</v>
+        <v>656</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -5755,7 +5755,7 @@
         <v>562</v>
       </c>
       <c r="I147" s="3" t="s">
-        <v>679</v>
+        <v>657</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
@@ -5778,7 +5778,7 @@
         <v>563</v>
       </c>
       <c r="I148" s="3" t="s">
-        <v>680</v>
+        <v>658</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -5801,7 +5801,7 @@
         <v>564</v>
       </c>
       <c r="I149" s="3" t="s">
-        <v>681</v>
+        <v>659</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
@@ -5821,7 +5821,7 @@
         <v>278</v>
       </c>
       <c r="I150" s="3" t="s">
-        <v>682</v>
+        <v>660</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
@@ -5861,7 +5861,7 @@
         <v>565</v>
       </c>
       <c r="I152" s="3" t="s">
-        <v>683</v>
+        <v>661</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -5887,7 +5887,7 @@
         <v>566</v>
       </c>
       <c r="I153" s="3" t="s">
-        <v>684</v>
+        <v>662</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
@@ -5928,7 +5928,7 @@
         <v>567</v>
       </c>
       <c r="I155" s="6" t="s">
-        <v>685</v>
+        <v>663</v>
       </c>
     </row>
     <row r="156" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -5939,7 +5939,7 @@
         <v>195</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>675</v>
+        <v>653</v>
       </c>
       <c r="F156" s="5"/>
       <c r="G156" s="5"/>
@@ -5965,7 +5965,7 @@
         <v>429</v>
       </c>
       <c r="I157" s="3" t="s">
-        <v>686</v>
+        <v>664</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -5985,7 +5985,7 @@
         <v>569</v>
       </c>
       <c r="I158" s="3" t="s">
-        <v>687</v>
+        <v>665</v>
       </c>
     </row>
     <row r="159" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -6056,7 +6056,7 @@
         <v>432</v>
       </c>
       <c r="I161" s="3" t="s">
-        <v>688</v>
+        <v>666</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -6082,7 +6082,7 @@
         <v>572</v>
       </c>
       <c r="I162" s="3" t="s">
-        <v>689</v>
+        <v>667</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
@@ -6105,7 +6105,7 @@
         <v>573</v>
       </c>
       <c r="I163" s="3" t="s">
-        <v>690</v>
+        <v>668</v>
       </c>
     </row>
     <row r="164" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6116,7 +6116,7 @@
         <v>195</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>675</v>
+        <v>653</v>
       </c>
       <c r="F164" s="5"/>
       <c r="G164" s="5" t="s">
@@ -6162,7 +6162,7 @@
         <v>435</v>
       </c>
       <c r="I166" s="3" t="s">
-        <v>691</v>
+        <v>669</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
@@ -6242,7 +6242,7 @@
         <v>575</v>
       </c>
       <c r="I170" s="3" t="s">
-        <v>692</v>
+        <v>670</v>
       </c>
     </row>
     <row r="171" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6286,7 +6286,7 @@
         <v>576</v>
       </c>
       <c r="I172" s="3" t="s">
-        <v>693</v>
+        <v>671</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -6312,7 +6312,7 @@
         <v>577</v>
       </c>
       <c r="I173" s="3" t="s">
-        <v>694</v>
+        <v>672</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
@@ -6332,7 +6332,7 @@
         <v>578</v>
       </c>
       <c r="I174" s="3" t="s">
-        <v>695</v>
+        <v>673</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
@@ -6352,7 +6352,7 @@
         <v>285</v>
       </c>
       <c r="I175" s="3" t="s">
-        <v>696</v>
+        <v>674</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
@@ -6375,7 +6375,7 @@
         <v>439</v>
       </c>
       <c r="I176" s="3" t="s">
-        <v>697</v>
+        <v>675</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
@@ -6424,7 +6424,7 @@
         <v>580</v>
       </c>
       <c r="I178" s="3" t="s">
-        <v>694</v>
+        <v>672</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
@@ -6491,7 +6491,7 @@
         <v>582</v>
       </c>
       <c r="I181" s="3" t="s">
-        <v>698</v>
+        <v>676</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
@@ -6511,7 +6511,7 @@
         <v>288</v>
       </c>
       <c r="I182" s="3" t="s">
-        <v>699</v>
+        <v>677</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
@@ -6534,7 +6534,7 @@
         <v>443</v>
       </c>
       <c r="I183" s="3" t="s">
-        <v>700</v>
+        <v>678</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
@@ -6611,7 +6611,7 @@
         <v>584</v>
       </c>
       <c r="I187" s="3" t="s">
-        <v>701</v>
+        <v>679</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
@@ -6680,7 +6680,7 @@
         <v>449</v>
       </c>
       <c r="I190" s="3" t="s">
-        <v>702</v>
+        <v>680</v>
       </c>
     </row>
     <row r="191" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6723,7 +6723,7 @@
         <v>450</v>
       </c>
       <c r="I192" s="3" t="s">
-        <v>703</v>
+        <v>681</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
@@ -6746,7 +6746,7 @@
         <v>451</v>
       </c>
       <c r="I193" s="3" t="s">
-        <v>704</v>
+        <v>682</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Done with dry firn identification exclusions for 2017 and 2018.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7423F77D-6880-4637-8C18-717888BAA05B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C911E330-F864-45C0-94D7-A32C99CAB232}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3675" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1231" uniqueCount="705">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="709">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -1710,9 +1710,6 @@
     <t>6480-6505 7200-7250</t>
   </si>
   <si>
-    <t>-7000</t>
-  </si>
-  <si>
     <t>5680-</t>
   </si>
   <si>
@@ -1932,9 +1929,6 @@
     <t>8960-9280 9570-</t>
   </si>
   <si>
-    <t>-1145 13500-17060 17630-21850</t>
-  </si>
-  <si>
     <t>2660-</t>
   </si>
   <si>
@@ -1944,36 +1938,24 @@
     <t>-645 835-1305</t>
   </si>
   <si>
-    <t>3770-</t>
-  </si>
-  <si>
     <t>2900-</t>
   </si>
   <si>
     <t>3520-</t>
   </si>
   <si>
-    <t>2950-</t>
-  </si>
-  <si>
     <t>7410-</t>
   </si>
   <si>
     <t>3600-</t>
   </si>
   <si>
-    <t>810-1115</t>
-  </si>
-  <si>
     <t>1080-1440</t>
   </si>
   <si>
     <t>2580-2675 4355-</t>
   </si>
   <si>
-    <t>5060-5800 6200-7700 8000-</t>
-  </si>
-  <si>
     <t>-1410 1770-2330 7460-</t>
   </si>
   <si>
@@ -1995,48 +1977,21 @@
     <t>Yes, -inf in data but replaces by NaNs, ok - deleted after dry firn identification though slabs at the surface …</t>
   </si>
   <si>
-    <t>-2040</t>
-  </si>
-  <si>
-    <t>3370-</t>
-  </si>
-  <si>
     <t>-1725</t>
   </si>
   <si>
     <t>810-</t>
   </si>
   <si>
-    <t>8155-</t>
-  </si>
-  <si>
     <t>-5500</t>
   </si>
   <si>
-    <t>-2180 2460-2550 4150-4270 4750-10810 12700-</t>
-  </si>
-  <si>
-    <t>-3240</t>
-  </si>
-  <si>
     <t>-1095 1290-</t>
   </si>
   <si>
-    <t>300-</t>
-  </si>
-  <si>
-    <t>3045-</t>
-  </si>
-  <si>
-    <t>-18830 19610-19950 43260-</t>
-  </si>
-  <si>
     <t>-1250</t>
   </si>
   <si>
-    <t>10600-</t>
-  </si>
-  <si>
     <t>-410</t>
   </si>
   <si>
@@ -2049,9 +2004,6 @@
     <t>-1580</t>
   </si>
   <si>
-    <t>-1500</t>
-  </si>
-  <si>
     <t>-1450</t>
   </si>
   <si>
@@ -2073,9 +2025,6 @@
     <t>-2720 2915-</t>
   </si>
   <si>
-    <t>4165-</t>
-  </si>
-  <si>
     <t>12440-25268 30580-30700 30780-30820</t>
   </si>
   <si>
@@ -2140,6 +2089,69 @@
   </si>
   <si>
     <t>-650 1695-2110 5015-5500 5665-5965 6740-7390 7685-8320 8480-</t>
+  </si>
+  <si>
+    <t>-1480 1670-2300 3030-3310 3370-4010 5160-5270 12090-13380 13500-17060 17630-21850</t>
+  </si>
+  <si>
+    <t>-460</t>
+  </si>
+  <si>
+    <t>3690-</t>
+  </si>
+  <si>
+    <t>2880-</t>
+  </si>
+  <si>
+    <t>5060-5820 5965-6030 6150-7775 8000-</t>
+  </si>
+  <si>
+    <t>7000-</t>
+  </si>
+  <si>
+    <t>-2060</t>
+  </si>
+  <si>
+    <t>2805-</t>
+  </si>
+  <si>
+    <t>810-1275 6015-6180 6300-6710 6785-7060 7190-7285 7470-7528 7675-</t>
+  </si>
+  <si>
+    <t>1065-1380 1700-</t>
+  </si>
+  <si>
+    <t>-2180 2460-2550 2820-4580 4750-10810 12050-</t>
+  </si>
+  <si>
+    <t>-5000</t>
+  </si>
+  <si>
+    <t>76-170 300-</t>
+  </si>
+  <si>
+    <t>-210 460-1720 1975-2610 2880-3280 3320-3970 4600-4900 6330-6370 6800-6880</t>
+  </si>
+  <si>
+    <t>2490-</t>
+  </si>
+  <si>
+    <t>-18830 19610-19950 42555-</t>
+  </si>
+  <si>
+    <t>5170-5345 5485-5700 5865-</t>
+  </si>
+  <si>
+    <t>-1285 1430-2005</t>
+  </si>
+  <si>
+    <t>-1670 1760-</t>
+  </si>
+  <si>
+    <t>5150-</t>
+  </si>
+  <si>
+    <t>4130-</t>
   </si>
 </sst>
 </file>
@@ -2516,8 +2528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
   <dimension ref="A1:I194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G138" sqref="G138"/>
+    <sheetView tabSelected="1" topLeftCell="E178" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F188" sqref="F188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2558,7 +2570,7 @@
         <v>307</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>589</v>
+        <v>588</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
@@ -2587,7 +2599,7 @@
         <v>503</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>590</v>
+        <v>589</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -2610,7 +2622,7 @@
         <v>505</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>591</v>
+        <v>590</v>
       </c>
     </row>
     <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2654,7 +2666,7 @@
         <v>506</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>592</v>
+        <v>591</v>
       </c>
     </row>
     <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -2665,7 +2677,7 @@
         <v>193</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="F6" s="5"/>
       <c r="G6" s="5"/>
@@ -2819,7 +2831,7 @@
         <v>510</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>683</v>
+        <v>666</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -2998,7 +3010,7 @@
         <v>309</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>593</v>
+        <v>592</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
@@ -3018,7 +3030,7 @@
         <v>310</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>594</v>
+        <v>593</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -3047,7 +3059,7 @@
         <v>514</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -3070,7 +3082,7 @@
         <v>515</v>
       </c>
       <c r="I26" s="4" t="s">
-        <v>684</v>
+        <v>667</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -3101,7 +3113,7 @@
         <v>193</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="F28" s="5"/>
       <c r="G28" s="5" t="s">
@@ -3153,7 +3165,7 @@
         <v>516</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>685</v>
+        <v>668</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -3202,7 +3214,7 @@
         <v>517</v>
       </c>
       <c r="I32" s="4" t="s">
-        <v>686</v>
+        <v>669</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -3248,7 +3260,7 @@
         <v>348</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>588</v>
+        <v>587</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -3274,7 +3286,7 @@
         <v>315</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>596</v>
+        <v>595</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3285,7 +3297,7 @@
         <v>193</v>
       </c>
       <c r="C36" s="5" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -3314,7 +3326,7 @@
         <v>518</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -3334,7 +3346,7 @@
         <v>353</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>598</v>
+        <v>597</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -3357,7 +3369,7 @@
         <v>-1815</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -3386,7 +3398,7 @@
         <v>519</v>
       </c>
       <c r="I40" s="4" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
     </row>
     <row r="41" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3397,7 +3409,7 @@
         <v>193</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>655</v>
+        <v>649</v>
       </c>
       <c r="F41" s="5" t="s">
         <v>240</v>
@@ -3431,7 +3443,7 @@
         <v>382</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -3457,7 +3469,7 @@
         <v>520</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>687</v>
+        <v>670</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -3480,7 +3492,7 @@
         <v>521</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -3503,7 +3515,7 @@
         <v>317</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>603</v>
+        <v>602</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -3566,7 +3578,7 @@
         <v>522</v>
       </c>
       <c r="I48" s="3" t="s">
-        <v>688</v>
+        <v>671</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -3592,7 +3604,7 @@
         <v>523</v>
       </c>
       <c r="I49" s="3" t="s">
-        <v>689</v>
+        <v>672</v>
       </c>
     </row>
     <row r="50" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -3603,7 +3615,7 @@
         <v>193</v>
       </c>
       <c r="C50" s="5" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="F50" s="5"/>
       <c r="G50" s="5"/>
@@ -3627,7 +3639,7 @@
         <v>524</v>
       </c>
       <c r="I51" s="3" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
@@ -3684,7 +3696,7 @@
         <v>193</v>
       </c>
       <c r="C54" s="5" t="s">
-        <v>654</v>
+        <v>648</v>
       </c>
       <c r="F54" s="10" t="s">
         <v>457</v>
@@ -3716,7 +3728,7 @@
         <v>320</v>
       </c>
       <c r="I55" s="3" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -3742,7 +3754,7 @@
         <v>527</v>
       </c>
       <c r="I56" s="3" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
@@ -3768,7 +3780,7 @@
         <v>322</v>
       </c>
       <c r="I57" s="3" t="s">
-        <v>607</v>
+        <v>606</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -3826,7 +3838,7 @@
         <v>364</v>
       </c>
       <c r="I60" s="3" t="s">
-        <v>690</v>
+        <v>673</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3849,7 +3861,7 @@
         <v>528</v>
       </c>
       <c r="I61" s="3" t="s">
-        <v>691</v>
+        <v>674</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3875,7 +3887,7 @@
         <v>323</v>
       </c>
       <c r="I62" s="3" t="s">
-        <v>608</v>
+        <v>607</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3898,10 +3910,10 @@
         <v>368</v>
       </c>
       <c r="H63" s="3" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="I63" s="3" t="s">
-        <v>692</v>
+        <v>675</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3927,7 +3939,7 @@
         <v>529</v>
       </c>
       <c r="I64" s="3" t="s">
-        <v>609</v>
+        <v>608</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3956,7 +3968,7 @@
         <v>325</v>
       </c>
       <c r="I65" s="3" t="s">
-        <v>610</v>
+        <v>609</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3979,7 +3991,7 @@
         <v>326</v>
       </c>
       <c r="I66" s="3" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -4002,7 +4014,7 @@
         <v>530</v>
       </c>
       <c r="I67" s="3" t="s">
-        <v>693</v>
+        <v>676</v>
       </c>
     </row>
     <row r="68" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4052,7 +4064,7 @@
         <v>531</v>
       </c>
       <c r="I69" s="3" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="70" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4063,7 +4075,7 @@
         <v>193</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="F70" s="5"/>
       <c r="G70" s="5"/>
@@ -4078,7 +4090,7 @@
         <v>193</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="F71" s="5" t="s">
         <v>248</v>
@@ -4107,7 +4119,7 @@
         <v>532</v>
       </c>
       <c r="I72" s="3" t="s">
-        <v>613</v>
+        <v>612</v>
       </c>
     </row>
     <row r="73" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4118,7 +4130,7 @@
         <v>193</v>
       </c>
       <c r="C73" s="5" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="F73" s="5">
         <v>-610</v>
@@ -4148,7 +4160,7 @@
         <v>533</v>
       </c>
       <c r="I74" s="3" t="s">
-        <v>614</v>
+        <v>613</v>
       </c>
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
@@ -4174,7 +4186,7 @@
         <v>374</v>
       </c>
       <c r="I75" s="3" t="s">
-        <v>615</v>
+        <v>614</v>
       </c>
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
@@ -4211,7 +4223,7 @@
         <v>73</v>
       </c>
       <c r="I77" s="3" t="s">
-        <v>616</v>
+        <v>615</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -4240,7 +4252,7 @@
         <v>534</v>
       </c>
       <c r="I78" s="3" t="s">
-        <v>617</v>
+        <v>616</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -4266,7 +4278,7 @@
         <v>330</v>
       </c>
       <c r="I79" s="3" t="s">
-        <v>694</v>
+        <v>677</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -4292,7 +4304,7 @@
         <v>535</v>
       </c>
       <c r="I80" s="3" t="s">
-        <v>618</v>
+        <v>617</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -4312,7 +4324,7 @@
         <v>381</v>
       </c>
       <c r="I81" s="3" t="s">
-        <v>619</v>
+        <v>618</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -4338,7 +4350,7 @@
         <v>536</v>
       </c>
       <c r="I82" s="3" t="s">
-        <v>620</v>
+        <v>619</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -4358,7 +4370,7 @@
         <v>250</v>
       </c>
       <c r="I83" s="3" t="s">
-        <v>695</v>
+        <v>678</v>
       </c>
     </row>
     <row r="84" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4369,13 +4381,13 @@
         <v>193</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="F84" s="5"/>
       <c r="G84" s="5"/>
       <c r="H84" s="5"/>
       <c r="I84" s="5" t="s">
-        <v>621</v>
+        <v>620</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -4395,7 +4407,7 @@
         <v>383</v>
       </c>
       <c r="I85" s="3" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -4424,7 +4436,7 @@
         <v>537</v>
       </c>
       <c r="I86" s="3" t="s">
-        <v>696</v>
+        <v>679</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -4450,7 +4462,7 @@
         <v>538</v>
       </c>
       <c r="I87" s="8" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
     </row>
     <row r="88" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4461,7 +4473,7 @@
         <v>193</v>
       </c>
       <c r="C88" s="5" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="F88" s="10" t="s">
         <v>462</v>
@@ -4490,7 +4502,7 @@
         <v>539</v>
       </c>
       <c r="I89" s="3" t="s">
-        <v>697</v>
+        <v>680</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -4516,7 +4528,7 @@
         <v>540</v>
       </c>
       <c r="I90" s="3" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
     </row>
     <row r="91" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4527,7 +4539,7 @@
         <v>193</v>
       </c>
       <c r="C91" s="5" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="F91" s="10" t="s">
         <v>463</v>
@@ -4557,7 +4569,7 @@
         <v>542</v>
       </c>
       <c r="I92" s="3" t="s">
-        <v>625</v>
+        <v>624</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -4580,7 +4592,7 @@
         <v>543</v>
       </c>
       <c r="I93" s="3" t="s">
-        <v>698</v>
+        <v>681</v>
       </c>
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
@@ -4603,7 +4615,7 @@
         <v>389</v>
       </c>
       <c r="I94" s="3" t="s">
-        <v>626</v>
+        <v>625</v>
       </c>
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
@@ -4626,7 +4638,7 @@
         <v>390</v>
       </c>
       <c r="I95" s="3" t="s">
-        <v>627</v>
+        <v>626</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -4646,7 +4658,7 @@
         <v>391</v>
       </c>
       <c r="I96" s="3" t="s">
-        <v>628</v>
+        <v>627</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -4666,7 +4678,7 @@
         <v>544</v>
       </c>
       <c r="I97" s="3" t="s">
-        <v>699</v>
+        <v>682</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -4686,7 +4698,7 @@
         <v>392</v>
       </c>
       <c r="I98" s="3" t="s">
-        <v>629</v>
+        <v>628</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -4709,7 +4721,7 @@
         <v>393</v>
       </c>
       <c r="I99" s="3" t="s">
-        <v>700</v>
+        <v>683</v>
       </c>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
@@ -4735,7 +4747,7 @@
         <v>545</v>
       </c>
       <c r="I100" s="3" t="s">
-        <v>630</v>
+        <v>629</v>
       </c>
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
@@ -4755,7 +4767,7 @@
         <v>394</v>
       </c>
       <c r="I101" s="3" t="s">
-        <v>631</v>
+        <v>630</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -4775,7 +4787,7 @@
         <v>395</v>
       </c>
       <c r="I102" s="3" t="s">
-        <v>701</v>
+        <v>684</v>
       </c>
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
@@ -4841,7 +4853,7 @@
         <v>397</v>
       </c>
       <c r="I105" s="3" t="s">
-        <v>702</v>
+        <v>685</v>
       </c>
     </row>
     <row r="106" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -4880,7 +4892,7 @@
         <v>546</v>
       </c>
       <c r="I107" s="6" t="s">
-        <v>703</v>
+        <v>686</v>
       </c>
     </row>
     <row r="108" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -4928,7 +4940,7 @@
         <v>547</v>
       </c>
       <c r="I109" s="3" t="s">
-        <v>632</v>
+        <v>631</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -4971,7 +4983,7 @@
         <v>402</v>
       </c>
       <c r="I111" s="3" t="s">
-        <v>633</v>
+        <v>632</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -4991,7 +5003,7 @@
         <v>261</v>
       </c>
       <c r="I112" s="3" t="s">
-        <v>704</v>
+        <v>687</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -5031,7 +5043,7 @@
         <v>403</v>
       </c>
       <c r="I114" s="3" t="s">
-        <v>634</v>
+        <v>633</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -5057,7 +5069,7 @@
         <v>548</v>
       </c>
       <c r="I115" s="3" t="s">
-        <v>635</v>
+        <v>688</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -5080,7 +5092,7 @@
         <v>324</v>
       </c>
       <c r="I116" s="3" t="s">
-        <v>636</v>
+        <v>634</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -5126,7 +5138,7 @@
         <v>406</v>
       </c>
       <c r="I118" s="3" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
     </row>
     <row r="119" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -5154,7 +5166,9 @@
       <c r="H119" s="6" t="s">
         <v>550</v>
       </c>
-      <c r="I119" s="6"/>
+      <c r="I119" s="6" t="s">
+        <v>689</v>
+      </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
@@ -5176,7 +5190,7 @@
         <v>367</v>
       </c>
       <c r="I120" s="3" t="s">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -5196,7 +5210,7 @@
         <v>408</v>
       </c>
       <c r="I121" s="3" t="s">
-        <v>638</v>
+        <v>636</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -5219,7 +5233,7 @@
         <v>409</v>
       </c>
       <c r="I122" s="3" t="s">
-        <v>639</v>
+        <v>690</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -5262,7 +5276,7 @@
         <v>411</v>
       </c>
       <c r="I124" s="3" t="s">
-        <v>640</v>
+        <v>637</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -5279,7 +5293,7 @@
         <v>121</v>
       </c>
       <c r="G125" s="3" t="s">
-        <v>641</v>
+        <v>638</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -5299,7 +5313,7 @@
         <v>412</v>
       </c>
       <c r="I126" s="3" t="s">
-        <v>642</v>
+        <v>691</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -5325,7 +5339,7 @@
         <v>552</v>
       </c>
       <c r="I127" s="3" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -5362,7 +5376,7 @@
         <v>351</v>
       </c>
       <c r="I129" s="3" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -5417,7 +5431,7 @@
         <v>350</v>
       </c>
       <c r="I132" s="3" t="s">
-        <v>645</v>
+        <v>651</v>
       </c>
     </row>
     <row r="133" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -5428,7 +5442,7 @@
         <v>193</v>
       </c>
       <c r="C133" s="5" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="F133" s="5" t="s">
         <v>270</v>
@@ -5464,7 +5478,7 @@
         <v>554</v>
       </c>
       <c r="I134" s="3" t="s">
-        <v>646</v>
+        <v>641</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -5487,7 +5501,7 @@
         <v>417</v>
       </c>
       <c r="I135" s="3" t="s">
-        <v>647</v>
+        <v>642</v>
       </c>
     </row>
     <row r="136" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -5535,7 +5549,7 @@
         <v>557</v>
       </c>
       <c r="I137" s="3" t="s">
-        <v>648</v>
+        <v>692</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -5561,7 +5575,7 @@
         <v>558</v>
       </c>
       <c r="I138" s="3" t="s">
-        <v>649</v>
+        <v>643</v>
       </c>
     </row>
     <row r="139" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -5581,7 +5595,7 @@
       <c r="G139" s="6"/>
       <c r="H139" s="6"/>
       <c r="I139" s="6" t="s">
-        <v>650</v>
+        <v>644</v>
       </c>
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
@@ -5607,7 +5621,7 @@
         <v>559</v>
       </c>
       <c r="I140" s="3" t="s">
-        <v>651</v>
+        <v>645</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
@@ -5664,7 +5678,7 @@
         <v>407</v>
       </c>
       <c r="I143" s="3" t="s">
-        <v>652</v>
+        <v>646</v>
       </c>
     </row>
     <row r="144" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -5688,7 +5702,7 @@
         <v>423</v>
       </c>
       <c r="H144" s="6" t="s">
-        <v>561</v>
+        <v>693</v>
       </c>
       <c r="I144" s="6"/>
     </row>
@@ -5700,7 +5714,7 @@
         <v>195</v>
       </c>
       <c r="C145" s="5" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="F145" s="5">
         <v>-1600</v>
@@ -5732,7 +5746,7 @@
         <v>424</v>
       </c>
       <c r="I146" s="3" t="s">
-        <v>656</v>
+        <v>694</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -5752,10 +5766,10 @@
         <v>425</v>
       </c>
       <c r="H147" s="3" t="s">
-        <v>562</v>
+        <v>561</v>
       </c>
       <c r="I147" s="3" t="s">
-        <v>657</v>
+        <v>695</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
@@ -5775,10 +5789,10 @@
         <v>426</v>
       </c>
       <c r="H148" s="3" t="s">
-        <v>563</v>
+        <v>562</v>
       </c>
       <c r="I148" s="3" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -5798,10 +5812,10 @@
         <v>277</v>
       </c>
       <c r="H149" s="3" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="I149" s="3" t="s">
-        <v>659</v>
+        <v>651</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
@@ -5821,7 +5835,7 @@
         <v>278</v>
       </c>
       <c r="I150" s="3" t="s">
-        <v>660</v>
+        <v>696</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
@@ -5838,7 +5852,7 @@
         <v>147</v>
       </c>
       <c r="I151" s="3" t="s">
-        <v>242</v>
+        <v>697</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
@@ -5858,10 +5872,10 @@
         <v>427</v>
       </c>
       <c r="H152" s="3" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="I152" s="3" t="s">
-        <v>661</v>
+        <v>652</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -5884,10 +5898,10 @@
         <v>428</v>
       </c>
       <c r="H153" s="3" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="I153" s="3" t="s">
-        <v>662</v>
+        <v>698</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
@@ -5925,10 +5939,10 @@
       </c>
       <c r="G155" s="6"/>
       <c r="H155" s="6" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="I155" s="6" t="s">
-        <v>663</v>
+        <v>699</v>
       </c>
     </row>
     <row r="156" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -5939,12 +5953,12 @@
         <v>195</v>
       </c>
       <c r="C156" s="5" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="F156" s="5"/>
       <c r="G156" s="5"/>
       <c r="H156" s="5" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="I156" s="5"/>
     </row>
@@ -5965,7 +5979,7 @@
         <v>429</v>
       </c>
       <c r="I157" s="3" t="s">
-        <v>664</v>
+        <v>653</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -5982,10 +5996,10 @@
         <v>154</v>
       </c>
       <c r="H158" s="3" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="I158" s="3" t="s">
-        <v>665</v>
+        <v>700</v>
       </c>
     </row>
     <row r="159" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
@@ -6008,9 +6022,11 @@
         <v>430</v>
       </c>
       <c r="H159" s="6" t="s">
-        <v>570</v>
-      </c>
-      <c r="I159" s="6"/>
+        <v>569</v>
+      </c>
+      <c r="I159" s="6" t="s">
+        <v>701</v>
+      </c>
     </row>
     <row r="160" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A160" s="9" t="s">
@@ -6032,9 +6048,11 @@
         <v>431</v>
       </c>
       <c r="H160" s="6" t="s">
-        <v>571</v>
-      </c>
-      <c r="I160" s="6"/>
+        <v>570</v>
+      </c>
+      <c r="I160" s="6" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
@@ -6056,7 +6074,7 @@
         <v>432</v>
       </c>
       <c r="I161" s="3" t="s">
-        <v>666</v>
+        <v>702</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -6079,10 +6097,10 @@
         <v>282</v>
       </c>
       <c r="H162" s="3" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="I162" s="3" t="s">
-        <v>667</v>
+        <v>703</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
@@ -6102,10 +6120,10 @@
         <v>433</v>
       </c>
       <c r="H163" s="3" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I163" s="3" t="s">
-        <v>668</v>
+        <v>654</v>
       </c>
     </row>
     <row r="164" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6116,14 +6134,14 @@
         <v>195</v>
       </c>
       <c r="C164" s="5" t="s">
-        <v>653</v>
+        <v>647</v>
       </c>
       <c r="F164" s="5"/>
       <c r="G164" s="5" t="s">
         <v>434</v>
       </c>
       <c r="H164" s="5" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="I164" s="5"/>
     </row>
@@ -6162,7 +6180,7 @@
         <v>435</v>
       </c>
       <c r="I166" s="3" t="s">
-        <v>669</v>
+        <v>704</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
@@ -6205,7 +6223,7 @@
         <v>436</v>
       </c>
       <c r="I168" s="3" t="s">
-        <v>340</v>
+        <v>705</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
@@ -6239,10 +6257,10 @@
         <v>166</v>
       </c>
       <c r="H170" s="3" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="I170" s="3" t="s">
-        <v>670</v>
+        <v>655</v>
       </c>
     </row>
     <row r="171" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6283,10 +6301,10 @@
         <v>437</v>
       </c>
       <c r="H172" s="3" t="s">
-        <v>576</v>
+        <v>575</v>
       </c>
       <c r="I172" s="3" t="s">
-        <v>671</v>
+        <v>656</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -6309,10 +6327,10 @@
         <v>438</v>
       </c>
       <c r="H173" s="3" t="s">
-        <v>577</v>
+        <v>576</v>
       </c>
       <c r="I173" s="3" t="s">
-        <v>672</v>
+        <v>657</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
@@ -6329,10 +6347,10 @@
         <v>170</v>
       </c>
       <c r="H174" s="3" t="s">
-        <v>578</v>
+        <v>577</v>
       </c>
       <c r="I174" s="3" t="s">
-        <v>673</v>
+        <v>658</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
@@ -6352,7 +6370,7 @@
         <v>285</v>
       </c>
       <c r="I175" s="3" t="s">
-        <v>674</v>
+        <v>706</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
@@ -6375,7 +6393,7 @@
         <v>439</v>
       </c>
       <c r="I176" s="3" t="s">
-        <v>675</v>
+        <v>659</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
@@ -6395,7 +6413,7 @@
         <v>340</v>
       </c>
       <c r="H177" s="3" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
@@ -6421,10 +6439,10 @@
         <v>440</v>
       </c>
       <c r="H178" s="3" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="I178" s="3" t="s">
-        <v>672</v>
+        <v>657</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
@@ -6443,6 +6461,9 @@
       <c r="G179" s="3" t="s">
         <v>382</v>
       </c>
+      <c r="I179" s="3" t="s">
+        <v>707</v>
+      </c>
     </row>
     <row r="180" spans="1:9" s="9" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A180" s="9" t="s">
@@ -6464,7 +6485,7 @@
         <v>441</v>
       </c>
       <c r="H180" s="6" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I180" s="6"/>
     </row>
@@ -6488,10 +6509,10 @@
         <v>442</v>
       </c>
       <c r="H181" s="3" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="I181" s="3" t="s">
-        <v>676</v>
+        <v>660</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
@@ -6511,7 +6532,7 @@
         <v>288</v>
       </c>
       <c r="I182" s="3" t="s">
-        <v>677</v>
+        <v>661</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
@@ -6534,7 +6555,7 @@
         <v>443</v>
       </c>
       <c r="I183" s="3" t="s">
-        <v>678</v>
+        <v>662</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
@@ -6585,7 +6606,7 @@
         <v>182</v>
       </c>
       <c r="H186" s="3" t="s">
-        <v>583</v>
+        <v>582</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
@@ -6608,10 +6629,10 @@
         <v>446</v>
       </c>
       <c r="H187" s="3" t="s">
-        <v>584</v>
+        <v>583</v>
       </c>
       <c r="I187" s="3" t="s">
-        <v>679</v>
+        <v>663</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
@@ -6631,7 +6652,7 @@
         <v>447</v>
       </c>
       <c r="H188" s="3" t="s">
-        <v>585</v>
+        <v>584</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
@@ -6654,7 +6675,7 @@
         <v>448</v>
       </c>
       <c r="H189" s="3" t="s">
-        <v>586</v>
+        <v>585</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
@@ -6680,7 +6701,7 @@
         <v>449</v>
       </c>
       <c r="I190" s="3" t="s">
-        <v>680</v>
+        <v>664</v>
       </c>
     </row>
     <row r="191" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
@@ -6723,7 +6744,7 @@
         <v>450</v>
       </c>
       <c r="I192" s="3" t="s">
-        <v>681</v>
+        <v>665</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
@@ -6746,7 +6767,7 @@
         <v>451</v>
       </c>
       <c r="I193" s="3" t="s">
-        <v>682</v>
+        <v>708</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
In 'aggregate_20022018_flightlines.py' try to perform a new way of doing intersection between data and GrIS mask In 'iceslabs_inland_expansion.py', continue coding Fig1 (display of panel b and c) In 'logbook_2017_2018_data_process.py', adding a new column for dry firn identification that will allow ice slabs likelihood consideration.
</commit_message>
<xml_diff>
--- a/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
+++ b/intial_selection_20172018/logbook_2017_2018_data_processing.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jullienn\Documents\working_environment\iceslabs_MacFerrin\intial_selection_20172018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C911E330-F864-45C0-94D7-A32C99CAB232}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08753F4D-2611-4671-AE53-4639DF1E5E8A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="3675" xr2:uid="{2330979D-87B3-4CD0-BAAE-0E715AE1AF11}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="710">
   <si>
     <t>20170322_01_003_006</t>
   </si>
@@ -2152,6 +2152,9 @@
   </si>
   <si>
     <t>4130-</t>
+  </si>
+  <si>
+    <t>Dry firn exclusions for likelihood</t>
   </si>
 </sst>
 </file>
@@ -2526,10 +2529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EF60F2B-D111-4EFE-8F11-ABA6164162FC}">
-  <dimension ref="A1:I194"/>
+  <dimension ref="A1:J194"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E178" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F188" sqref="F188"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2544,7 +2547,7 @@
     <col min="9" max="9" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>191</v>
       </c>
@@ -2572,8 +2575,11 @@
       <c r="I1" s="3" t="s">
         <v>588</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="3" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>191</v>
       </c>
@@ -2602,7 +2608,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -2625,7 +2631,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -2640,7 +2646,7 @@
       <c r="H4" s="5"/>
       <c r="I4" s="5"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2669,7 +2675,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
@@ -2686,7 +2692,7 @@
       </c>
       <c r="I6" s="5"/>
     </row>
-    <row r="7" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -2701,7 +2707,7 @@
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
     </row>
-    <row r="8" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>304</v>
       </c>
@@ -2718,7 +2724,7 @@
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
     </row>
-    <row r="9" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -2733,7 +2739,7 @@
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -2753,7 +2759,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -2770,7 +2776,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -2790,7 +2796,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
@@ -2805,7 +2811,7 @@
       <c r="H13" s="5"/>
       <c r="I13" s="5"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -2834,7 +2840,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -2857,7 +2863,7 @@
         <v>511</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>